<commit_message>
Finished a medium problme
</commit_message>
<xml_diff>
--- a/AllsWellThatEndsExcel_Case_and_Answers.xlsx
+++ b/AllsWellThatEndsExcel_Case_and_Answers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C97B5A-E34B-46EF-A9F4-A111AE2B3857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF9A3F2-4912-4B02-99C4-18D7B91D03F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14CF381A-4175-4F53-B406-22934FD6CEB0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{14CF381A-4175-4F53-B406-22934FD6CEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="16" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -8467,124 +8467,10 @@
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="60" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="60" fillId="7" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="15" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8685,6 +8571,120 @@
     </xf>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="60" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="60" fillId="7" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="15" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -11519,8 +11519,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6726002" y="25062196"/>
-          <a:ext cx="701364" cy="209696"/>
+          <a:off x="6752224" y="24916520"/>
+          <a:ext cx="699795" cy="205886"/>
           <a:chOff x="5262929" y="18783301"/>
           <a:chExt cx="663493" cy="205886"/>
         </a:xfrm>
@@ -11659,8 +11659,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6714582" y="25340487"/>
-          <a:ext cx="928119" cy="214865"/>
+          <a:off x="6735089" y="25192233"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -11799,8 +11799,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6724263" y="25636746"/>
-          <a:ext cx="726278" cy="216770"/>
+          <a:off x="6742865" y="25484010"/>
+          <a:ext cx="736139" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="698638" cy="211055"/>
         </a:xfrm>
@@ -11939,8 +11939,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6721022" y="25946052"/>
-          <a:ext cx="937644" cy="207245"/>
+          <a:off x="6747244" y="25785024"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -12079,8 +12079,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6723293" y="26243014"/>
-          <a:ext cx="689934" cy="200171"/>
+          <a:off x="6741895" y="26075598"/>
+          <a:ext cx="699795" cy="205886"/>
           <a:chOff x="5262929" y="18783301"/>
           <a:chExt cx="663493" cy="205886"/>
         </a:xfrm>
@@ -12219,8 +12219,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6728083" y="26498362"/>
-          <a:ext cx="930024" cy="207245"/>
+          <a:off x="6746685" y="26326464"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -12359,8 +12359,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6728239" y="26787001"/>
-          <a:ext cx="737708" cy="214865"/>
+          <a:off x="6754461" y="26618240"/>
+          <a:ext cx="736139" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="698638" cy="211055"/>
         </a:xfrm>
@@ -12499,8 +12499,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6734522" y="27109419"/>
-          <a:ext cx="939549" cy="207245"/>
+          <a:off x="6758839" y="26930461"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -12639,8 +12639,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6727268" y="27404476"/>
-          <a:ext cx="701364" cy="200171"/>
+          <a:off x="6753490" y="27221036"/>
+          <a:ext cx="699795" cy="205886"/>
           <a:chOff x="5262929" y="18783301"/>
           <a:chExt cx="663493" cy="205886"/>
         </a:xfrm>
@@ -15174,8 +15174,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6723641" y="21394205"/>
-          <a:ext cx="937644" cy="207245"/>
+          <a:off x="6749863" y="21300748"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -15314,8 +15314,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6725917" y="21886981"/>
-          <a:ext cx="930024" cy="216770"/>
+          <a:off x="6744519" y="21792515"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -15454,8 +15454,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6724159" y="22437371"/>
-          <a:ext cx="937644" cy="207245"/>
+          <a:off x="6750381" y="22332036"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -15594,8 +15594,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6721228" y="22742352"/>
-          <a:ext cx="937644" cy="207245"/>
+          <a:off x="6747450" y="22630629"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -15734,8 +15734,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6727089" y="23004543"/>
-          <a:ext cx="939549" cy="216770"/>
+          <a:off x="6753311" y="22894053"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -15874,8 +15874,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6725917" y="23312895"/>
-          <a:ext cx="930024" cy="207245"/>
+          <a:off x="6744519" y="23194112"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16014,8 +16014,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6724452" y="23612014"/>
-          <a:ext cx="930024" cy="205340"/>
+          <a:off x="6743054" y="23486844"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16154,8 +16154,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6722689" y="23907071"/>
-          <a:ext cx="699459" cy="200171"/>
+          <a:off x="6748911" y="23777418"/>
+          <a:ext cx="699795" cy="205886"/>
           <a:chOff x="5262929" y="18783301"/>
           <a:chExt cx="663493" cy="205886"/>
         </a:xfrm>
@@ -16294,8 +16294,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6732307" y="24206398"/>
-          <a:ext cx="937644" cy="216770"/>
+          <a:off x="6756624" y="24077979"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16434,8 +16434,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6721610" y="24514750"/>
-          <a:ext cx="937644" cy="207245"/>
+          <a:off x="6747832" y="24378039"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16574,8 +16574,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6727765" y="24813868"/>
-          <a:ext cx="930024" cy="209150"/>
+          <a:off x="6746367" y="24670769"/>
+          <a:ext cx="936075" cy="206573"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16714,8 +16714,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6726779" y="20905965"/>
-          <a:ext cx="930024" cy="207245"/>
+          <a:off x="6745381" y="20818896"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16854,8 +16854,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6721434" y="22186962"/>
-          <a:ext cx="928119" cy="207245"/>
+          <a:off x="6740036" y="22086109"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -18106,8 +18106,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5763144" y="1198765"/>
-          <a:ext cx="16283326" cy="14110508"/>
+          <a:off x="5766954" y="1222664"/>
+          <a:ext cx="16277958" cy="14187055"/>
           <a:chOff x="5611090" y="1281546"/>
           <a:chExt cx="15831149" cy="14356773"/>
         </a:xfrm>
@@ -18488,7 +18488,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4461"/>
+                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4463"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -18556,7 +18556,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4462"/>
+                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4464"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -19186,8 +19186,8 @@
   </sheetPr>
   <dimension ref="A1:N271"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L74" sqref="L74"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B117" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H126" sqref="H126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.6640625" defaultRowHeight="25.8" outlineLevelRow="1"/>
@@ -19210,19 +19210,19 @@
       <c r="A1"/>
     </row>
     <row r="2" spans="1:12" ht="59.25" customHeight="1">
-      <c r="B2" s="223" t="s">
+      <c r="B2" s="185" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
-      <c r="L2" s="224"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="186"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" outlineLevel="1">
       <c r="A3"/>
@@ -19239,19 +19239,19 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" ht="75" customHeight="1" outlineLevel="1">
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="187" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="225"/>
-      <c r="D4" s="225"/>
-      <c r="E4" s="225"/>
-      <c r="F4" s="225"/>
-      <c r="G4" s="225"/>
-      <c r="H4" s="225"/>
-      <c r="I4" s="225"/>
-      <c r="J4" s="225"/>
-      <c r="K4" s="225"/>
-      <c r="L4" s="225"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="187"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="B5" s="2"/>
@@ -19267,112 +19267,112 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="33" customHeight="1">
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="193"/>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="193"/>
-      <c r="H6" s="193"/>
-      <c r="I6" s="226"/>
+      <c r="C6" s="184"/>
+      <c r="D6" s="184"/>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="184"/>
+      <c r="H6" s="184"/>
+      <c r="I6" s="188"/>
       <c r="J6"/>
-      <c r="K6" s="227" t="s">
+      <c r="K6" s="189" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="228"/>
+      <c r="L6" s="190"/>
     </row>
     <row r="7" spans="1:12" ht="25.95" customHeight="1">
-      <c r="B7" s="229" t="s">
+      <c r="B7" s="191" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="230"/>
-      <c r="D7" s="230"/>
-      <c r="E7" s="230"/>
-      <c r="F7" s="230"/>
-      <c r="G7" s="230"/>
-      <c r="H7" s="230"/>
-      <c r="I7" s="231"/>
+      <c r="C7" s="192"/>
+      <c r="D7" s="192"/>
+      <c r="E7" s="192"/>
+      <c r="F7" s="192"/>
+      <c r="G7" s="192"/>
+      <c r="H7" s="192"/>
+      <c r="I7" s="193"/>
       <c r="K7" s="5"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="232"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233"/>
-      <c r="H8" s="233"/>
-      <c r="I8" s="234"/>
+      <c r="B8" s="194"/>
+      <c r="C8" s="195"/>
+      <c r="D8" s="195"/>
+      <c r="E8" s="195"/>
+      <c r="F8" s="195"/>
+      <c r="G8" s="195"/>
+      <c r="H8" s="195"/>
+      <c r="I8" s="196"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="232"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
-      <c r="G9" s="233"/>
-      <c r="H9" s="233"/>
-      <c r="I9" s="234"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="195"/>
+      <c r="D9" s="195"/>
+      <c r="E9" s="195"/>
+      <c r="F9" s="195"/>
+      <c r="G9" s="195"/>
+      <c r="H9" s="195"/>
+      <c r="I9" s="196"/>
       <c r="J9"/>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="B10" s="232"/>
-      <c r="C10" s="233"/>
-      <c r="D10" s="233"/>
-      <c r="E10" s="233"/>
-      <c r="F10" s="233"/>
-      <c r="G10" s="233"/>
-      <c r="H10" s="233"/>
-      <c r="I10" s="234"/>
+      <c r="B10" s="194"/>
+      <c r="C10" s="195"/>
+      <c r="D10" s="195"/>
+      <c r="E10" s="195"/>
+      <c r="F10" s="195"/>
+      <c r="G10" s="195"/>
+      <c r="H10" s="195"/>
+      <c r="I10" s="196"/>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="B11" s="232"/>
-      <c r="C11" s="233"/>
-      <c r="D11" s="233"/>
-      <c r="E11" s="233"/>
-      <c r="F11" s="233"/>
-      <c r="G11" s="233"/>
-      <c r="H11" s="233"/>
-      <c r="I11" s="234"/>
+      <c r="B11" s="194"/>
+      <c r="C11" s="195"/>
+      <c r="D11" s="195"/>
+      <c r="E11" s="195"/>
+      <c r="F11" s="195"/>
+      <c r="G11" s="195"/>
+      <c r="H11" s="195"/>
+      <c r="I11" s="196"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="B12" s="232"/>
-      <c r="C12" s="233"/>
-      <c r="D12" s="233"/>
-      <c r="E12" s="233"/>
-      <c r="F12" s="233"/>
-      <c r="G12" s="233"/>
-      <c r="H12" s="233"/>
-      <c r="I12" s="234"/>
+      <c r="B12" s="194"/>
+      <c r="C12" s="195"/>
+      <c r="D12" s="195"/>
+      <c r="E12" s="195"/>
+      <c r="F12" s="195"/>
+      <c r="G12" s="195"/>
+      <c r="H12" s="195"/>
+      <c r="I12" s="196"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:12" ht="23.25" customHeight="1">
-      <c r="B13" s="232"/>
-      <c r="C13" s="233"/>
-      <c r="D13" s="233"/>
-      <c r="E13" s="233"/>
-      <c r="F13" s="233"/>
-      <c r="G13" s="233"/>
-      <c r="H13" s="233"/>
-      <c r="I13" s="234"/>
+      <c r="B13" s="194"/>
+      <c r="C13" s="195"/>
+      <c r="D13" s="195"/>
+      <c r="E13" s="195"/>
+      <c r="F13" s="195"/>
+      <c r="G13" s="195"/>
+      <c r="H13" s="195"/>
+      <c r="I13" s="196"/>
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:12" ht="33" customHeight="1">
-      <c r="B14" s="235"/>
-      <c r="C14" s="236"/>
-      <c r="D14" s="236"/>
-      <c r="E14" s="236"/>
-      <c r="F14" s="236"/>
-      <c r="G14" s="236"/>
-      <c r="H14" s="236"/>
-      <c r="I14" s="237"/>
+      <c r="B14" s="197"/>
+      <c r="C14" s="198"/>
+      <c r="D14" s="198"/>
+      <c r="E14" s="198"/>
+      <c r="F14" s="198"/>
+      <c r="G14" s="198"/>
+      <c r="H14" s="198"/>
+      <c r="I14" s="199"/>
       <c r="K14" s="34" t="s">
         <v>0</v>
       </c>
@@ -19386,60 +19386,60 @@
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B16" s="192" t="s">
+      <c r="B16" s="183" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="193"/>
-      <c r="D16" s="193"/>
-      <c r="E16" s="193"/>
-      <c r="F16" s="193"/>
-      <c r="G16" s="193"/>
-      <c r="H16" s="193"/>
-      <c r="I16" s="193"/>
-      <c r="J16" s="193"/>
-      <c r="K16" s="193"/>
-      <c r="L16" s="193"/>
+      <c r="C16" s="184"/>
+      <c r="D16" s="184"/>
+      <c r="E16" s="184"/>
+      <c r="F16" s="184"/>
+      <c r="G16" s="184"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="184"/>
+      <c r="J16" s="184"/>
+      <c r="K16" s="184"/>
+      <c r="L16" s="184"/>
     </row>
     <row r="17" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B17" s="238" t="s">
+      <c r="B17" s="200" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="239"/>
-      <c r="D17" s="239"/>
-      <c r="E17" s="239"/>
-      <c r="F17" s="239"/>
-      <c r="G17" s="239"/>
-      <c r="H17" s="239"/>
-      <c r="I17" s="239"/>
-      <c r="J17" s="239"/>
-      <c r="K17" s="239"/>
-      <c r="L17" s="240"/>
+      <c r="C17" s="201"/>
+      <c r="D17" s="201"/>
+      <c r="E17" s="201"/>
+      <c r="F17" s="201"/>
+      <c r="G17" s="201"/>
+      <c r="H17" s="201"/>
+      <c r="I17" s="201"/>
+      <c r="J17" s="201"/>
+      <c r="K17" s="201"/>
+      <c r="L17" s="202"/>
     </row>
     <row r="18" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B18" s="241"/>
-      <c r="C18" s="242"/>
-      <c r="D18" s="242"/>
-      <c r="E18" s="242"/>
-      <c r="F18" s="242"/>
-      <c r="G18" s="242"/>
-      <c r="H18" s="242"/>
-      <c r="I18" s="242"/>
-      <c r="J18" s="242"/>
-      <c r="K18" s="242"/>
-      <c r="L18" s="243"/>
+      <c r="B18" s="203"/>
+      <c r="C18" s="204"/>
+      <c r="D18" s="204"/>
+      <c r="E18" s="204"/>
+      <c r="F18" s="204"/>
+      <c r="G18" s="204"/>
+      <c r="H18" s="204"/>
+      <c r="I18" s="204"/>
+      <c r="J18" s="204"/>
+      <c r="K18" s="204"/>
+      <c r="L18" s="205"/>
     </row>
     <row r="19" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B19" s="244"/>
-      <c r="C19" s="245"/>
-      <c r="D19" s="245"/>
-      <c r="E19" s="245"/>
-      <c r="F19" s="245"/>
-      <c r="G19" s="245"/>
-      <c r="H19" s="245"/>
-      <c r="I19" s="245"/>
-      <c r="J19" s="245"/>
-      <c r="K19" s="245"/>
-      <c r="L19" s="246"/>
+      <c r="B19" s="206"/>
+      <c r="C19" s="207"/>
+      <c r="D19" s="207"/>
+      <c r="E19" s="207"/>
+      <c r="F19" s="207"/>
+      <c r="G19" s="207"/>
+      <c r="H19" s="207"/>
+      <c r="I19" s="207"/>
+      <c r="J19" s="207"/>
+      <c r="K19" s="207"/>
+      <c r="L19" s="208"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="B20" s="8"/>
@@ -19455,19 +19455,19 @@
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B21" s="192" t="s">
+      <c r="B21" s="183" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="193"/>
-      <c r="D21" s="193"/>
-      <c r="E21" s="193"/>
-      <c r="F21" s="193"/>
-      <c r="G21" s="193"/>
-      <c r="H21" s="193"/>
-      <c r="I21" s="193"/>
-      <c r="J21" s="193"/>
-      <c r="K21" s="193"/>
-      <c r="L21" s="193"/>
+      <c r="C21" s="184"/>
+      <c r="D21" s="184"/>
+      <c r="E21" s="184"/>
+      <c r="F21" s="184"/>
+      <c r="G21" s="184"/>
+      <c r="H21" s="184"/>
+      <c r="I21" s="184"/>
+      <c r="J21" s="184"/>
+      <c r="K21" s="184"/>
+      <c r="L21" s="184"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="B22" s="9"/>
@@ -19549,14 +19549,14 @@
         <f>IF(ISBLANK(E26),0,IF(E26=Answers!E26,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G26" s="247" t="s">
+      <c r="G26" s="209" t="s">
         <v>187</v>
       </c>
-      <c r="H26" s="248"/>
-      <c r="I26" s="248"/>
-      <c r="J26" s="248"/>
-      <c r="K26" s="248"/>
-      <c r="L26" s="249"/>
+      <c r="H26" s="210"/>
+      <c r="I26" s="210"/>
+      <c r="J26" s="210"/>
+      <c r="K26" s="210"/>
+      <c r="L26" s="211"/>
     </row>
     <row r="27" spans="1:12" ht="33.75" customHeight="1">
       <c r="B27" s="36" t="s">
@@ -19573,14 +19573,14 @@
         <f>IF(ISBLANK(E27),0,IF(E27=Answers!E27,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G27" s="250" t="s">
+      <c r="G27" s="212" t="s">
         <v>186</v>
       </c>
-      <c r="H27" s="251"/>
-      <c r="I27" s="251"/>
-      <c r="J27" s="251"/>
-      <c r="K27" s="251"/>
-      <c r="L27" s="252"/>
+      <c r="H27" s="213"/>
+      <c r="I27" s="213"/>
+      <c r="J27" s="213"/>
+      <c r="K27" s="213"/>
+      <c r="L27" s="214"/>
     </row>
     <row r="28" spans="1:12" ht="54" customHeight="1">
       <c r="B28" s="36" t="s">
@@ -19597,14 +19597,14 @@
         <f>IF(ISBLANK(E28),0,IF(E28=Answers!E28,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="253" t="s">
+      <c r="G28" s="215" t="s">
         <v>345</v>
       </c>
-      <c r="H28" s="254"/>
-      <c r="I28" s="254"/>
-      <c r="J28" s="254"/>
-      <c r="K28" s="254"/>
-      <c r="L28" s="255"/>
+      <c r="H28" s="216"/>
+      <c r="I28" s="216"/>
+      <c r="J28" s="216"/>
+      <c r="K28" s="216"/>
+      <c r="L28" s="217"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="B29" s="2"/>
@@ -19620,19 +19620,19 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="B30" s="192" t="s">
+      <c r="B30" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="193"/>
-      <c r="D30" s="193"/>
-      <c r="E30" s="193"/>
-      <c r="F30" s="193"/>
-      <c r="G30" s="193"/>
-      <c r="H30" s="193"/>
-      <c r="I30" s="193"/>
-      <c r="J30" s="193"/>
-      <c r="K30" s="193"/>
-      <c r="L30" s="193"/>
+      <c r="C30" s="184"/>
+      <c r="D30" s="184"/>
+      <c r="E30" s="184"/>
+      <c r="F30" s="184"/>
+      <c r="G30" s="184"/>
+      <c r="H30" s="184"/>
+      <c r="I30" s="184"/>
+      <c r="J30" s="184"/>
+      <c r="K30" s="184"/>
+      <c r="L30" s="184"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="B31" s="16"/>
@@ -19662,10 +19662,10 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
-      <c r="K32" s="192" t="s">
+      <c r="K32" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="L32" s="193"/>
+      <c r="L32" s="184"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1">
       <c r="A33" s="13"/>
@@ -19678,11 +19678,11 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
-      <c r="K33" s="194" cm="1">
+      <c r="K33" s="227" cm="1">
         <f t="array" ref="K33">SUMPRODUCT(--($F$26:$F$262=1),$D$26:$D$262)</f>
-        <v>160</v>
-      </c>
-      <c r="L33" s="195"/>
+        <v>300</v>
+      </c>
+      <c r="L33" s="228"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1">
       <c r="A34"/>
@@ -19697,8 +19697,8 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
-      <c r="K34" s="196"/>
-      <c r="L34" s="197"/>
+      <c r="K34" s="229"/>
+      <c r="L34" s="230"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1">
       <c r="A35" s="13"/>
@@ -19713,8 +19713,8 @@
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
-      <c r="K35" s="196"/>
-      <c r="L35" s="197"/>
+      <c r="K35" s="229"/>
+      <c r="L35" s="230"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1">
       <c r="A36" s="13"/>
@@ -19727,8 +19727,8 @@
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
-      <c r="K36" s="198"/>
-      <c r="L36" s="199"/>
+      <c r="K36" s="231"/>
+      <c r="L36" s="232"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1">
       <c r="A37" s="13"/>
@@ -19867,10 +19867,10 @@
         <v>122</v>
       </c>
       <c r="F45" s="18"/>
-      <c r="G45" s="200" t="s">
+      <c r="G45" s="233" t="s">
         <v>324</v>
       </c>
-      <c r="H45" s="201"/>
+      <c r="H45" s="234"/>
       <c r="I45" s="91" t="s">
         <v>52</v>
       </c>
@@ -20329,14 +20329,14 @@
       <c r="F63" s="18"/>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
-      <c r="I63" s="202" t="s">
+      <c r="I63" s="235" t="s">
         <v>138</v>
       </c>
-      <c r="J63" s="203"/>
-      <c r="K63" s="206" t="s">
+      <c r="J63" s="236"/>
+      <c r="K63" s="239" t="s">
         <v>141</v>
       </c>
-      <c r="L63" s="207"/>
+      <c r="L63" s="240"/>
     </row>
     <row r="64" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A64" s="13"/>
@@ -20349,10 +20349,10 @@
       <c r="F64" s="18"/>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
-      <c r="I64" s="204"/>
-      <c r="J64" s="205"/>
-      <c r="K64" s="208"/>
-      <c r="L64" s="209"/>
+      <c r="I64" s="237"/>
+      <c r="J64" s="238"/>
+      <c r="K64" s="241"/>
+      <c r="L64" s="242"/>
     </row>
     <row r="65" spans="1:14" ht="15" customHeight="1">
       <c r="A65" s="13"/>
@@ -20556,12 +20556,12 @@
       </c>
       <c r="F75" s="18"/>
       <c r="G75" s="13"/>
-      <c r="H75" s="210" t="s">
+      <c r="H75" s="243" t="s">
         <v>136</v>
       </c>
-      <c r="I75" s="211"/>
-      <c r="J75" s="211"/>
-      <c r="K75" s="212"/>
+      <c r="I75" s="244"/>
+      <c r="J75" s="244"/>
+      <c r="K75" s="245"/>
       <c r="L75" s="176" t="s">
         <v>135</v>
       </c>
@@ -21283,119 +21283,119 @@
       <c r="L99" s="20"/>
     </row>
     <row r="100" spans="1:13">
-      <c r="B100" s="192" t="s">
+      <c r="B100" s="183" t="s">
         <v>21</v>
       </c>
-      <c r="C100" s="193"/>
-      <c r="D100" s="193"/>
-      <c r="E100" s="193"/>
-      <c r="F100" s="193"/>
-      <c r="G100" s="193"/>
-      <c r="H100" s="193"/>
-      <c r="I100" s="193"/>
-      <c r="J100" s="193"/>
-      <c r="K100" s="193"/>
-      <c r="L100" s="193"/>
+      <c r="C100" s="184"/>
+      <c r="D100" s="184"/>
+      <c r="E100" s="184"/>
+      <c r="F100" s="184"/>
+      <c r="G100" s="184"/>
+      <c r="H100" s="184"/>
+      <c r="I100" s="184"/>
+      <c r="J100" s="184"/>
+      <c r="K100" s="184"/>
+      <c r="L100" s="184"/>
     </row>
     <row r="101" spans="1:13" ht="15" customHeight="1">
       <c r="A101" s="13"/>
-      <c r="B101" s="183" t="s">
+      <c r="B101" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C101" s="213"/>
-      <c r="D101" s="213"/>
-      <c r="E101" s="213"/>
-      <c r="F101" s="213"/>
-      <c r="G101" s="213"/>
-      <c r="H101" s="213"/>
-      <c r="I101" s="213"/>
-      <c r="J101" s="213"/>
-      <c r="K101" s="213"/>
-      <c r="L101" s="214"/>
+      <c r="C101" s="246"/>
+      <c r="D101" s="246"/>
+      <c r="E101" s="246"/>
+      <c r="F101" s="246"/>
+      <c r="G101" s="246"/>
+      <c r="H101" s="246"/>
+      <c r="I101" s="246"/>
+      <c r="J101" s="246"/>
+      <c r="K101" s="246"/>
+      <c r="L101" s="247"/>
     </row>
     <row r="102" spans="1:13" ht="15" customHeight="1">
       <c r="A102" s="13"/>
-      <c r="B102" s="215"/>
-      <c r="C102" s="216"/>
-      <c r="D102" s="216"/>
-      <c r="E102" s="216"/>
-      <c r="F102" s="216"/>
-      <c r="G102" s="216"/>
-      <c r="H102" s="216"/>
-      <c r="I102" s="216"/>
-      <c r="J102" s="216"/>
-      <c r="K102" s="216"/>
-      <c r="L102" s="217"/>
+      <c r="B102" s="248"/>
+      <c r="C102" s="249"/>
+      <c r="D102" s="249"/>
+      <c r="E102" s="249"/>
+      <c r="F102" s="249"/>
+      <c r="G102" s="249"/>
+      <c r="H102" s="249"/>
+      <c r="I102" s="249"/>
+      <c r="J102" s="249"/>
+      <c r="K102" s="249"/>
+      <c r="L102" s="250"/>
     </row>
     <row r="103" spans="1:13" ht="15" customHeight="1">
       <c r="A103" s="13"/>
-      <c r="B103" s="215"/>
-      <c r="C103" s="216"/>
-      <c r="D103" s="216"/>
-      <c r="E103" s="216"/>
-      <c r="F103" s="216"/>
-      <c r="G103" s="216"/>
-      <c r="H103" s="216"/>
-      <c r="I103" s="216"/>
-      <c r="J103" s="216"/>
-      <c r="K103" s="216"/>
-      <c r="L103" s="217"/>
+      <c r="B103" s="248"/>
+      <c r="C103" s="249"/>
+      <c r="D103" s="249"/>
+      <c r="E103" s="249"/>
+      <c r="F103" s="249"/>
+      <c r="G103" s="249"/>
+      <c r="H103" s="249"/>
+      <c r="I103" s="249"/>
+      <c r="J103" s="249"/>
+      <c r="K103" s="249"/>
+      <c r="L103" s="250"/>
     </row>
     <row r="104" spans="1:13" ht="15" customHeight="1">
       <c r="A104" s="13"/>
-      <c r="B104" s="215"/>
-      <c r="C104" s="216"/>
-      <c r="D104" s="216"/>
-      <c r="E104" s="216"/>
-      <c r="F104" s="216"/>
-      <c r="G104" s="216"/>
-      <c r="H104" s="216"/>
-      <c r="I104" s="216"/>
-      <c r="J104" s="216"/>
-      <c r="K104" s="216"/>
-      <c r="L104" s="217"/>
+      <c r="B104" s="248"/>
+      <c r="C104" s="249"/>
+      <c r="D104" s="249"/>
+      <c r="E104" s="249"/>
+      <c r="F104" s="249"/>
+      <c r="G104" s="249"/>
+      <c r="H104" s="249"/>
+      <c r="I104" s="249"/>
+      <c r="J104" s="249"/>
+      <c r="K104" s="249"/>
+      <c r="L104" s="250"/>
     </row>
     <row r="105" spans="1:13" ht="15" customHeight="1">
       <c r="A105" s="13"/>
-      <c r="B105" s="215"/>
-      <c r="C105" s="216"/>
-      <c r="D105" s="216"/>
-      <c r="E105" s="216"/>
-      <c r="F105" s="216"/>
-      <c r="G105" s="216"/>
-      <c r="H105" s="216"/>
-      <c r="I105" s="216"/>
-      <c r="J105" s="216"/>
-      <c r="K105" s="216"/>
-      <c r="L105" s="217"/>
+      <c r="B105" s="248"/>
+      <c r="C105" s="249"/>
+      <c r="D105" s="249"/>
+      <c r="E105" s="249"/>
+      <c r="F105" s="249"/>
+      <c r="G105" s="249"/>
+      <c r="H105" s="249"/>
+      <c r="I105" s="249"/>
+      <c r="J105" s="249"/>
+      <c r="K105" s="249"/>
+      <c r="L105" s="250"/>
     </row>
     <row r="106" spans="1:13" ht="15" customHeight="1">
       <c r="A106" s="13"/>
-      <c r="B106" s="215"/>
-      <c r="C106" s="216"/>
-      <c r="D106" s="216"/>
-      <c r="E106" s="216"/>
-      <c r="F106" s="216"/>
-      <c r="G106" s="216"/>
-      <c r="H106" s="216"/>
-      <c r="I106" s="216"/>
-      <c r="J106" s="216"/>
-      <c r="K106" s="216"/>
-      <c r="L106" s="217"/>
+      <c r="B106" s="248"/>
+      <c r="C106" s="249"/>
+      <c r="D106" s="249"/>
+      <c r="E106" s="249"/>
+      <c r="F106" s="249"/>
+      <c r="G106" s="249"/>
+      <c r="H106" s="249"/>
+      <c r="I106" s="249"/>
+      <c r="J106" s="249"/>
+      <c r="K106" s="249"/>
+      <c r="L106" s="250"/>
     </row>
     <row r="107" spans="1:13" ht="15" customHeight="1">
       <c r="A107" s="13"/>
-      <c r="B107" s="218"/>
-      <c r="C107" s="219"/>
-      <c r="D107" s="219"/>
-      <c r="E107" s="219"/>
-      <c r="F107" s="219"/>
-      <c r="G107" s="219"/>
-      <c r="H107" s="219"/>
-      <c r="I107" s="219"/>
-      <c r="J107" s="219"/>
-      <c r="K107" s="219"/>
-      <c r="L107" s="220"/>
+      <c r="B107" s="251"/>
+      <c r="C107" s="252"/>
+      <c r="D107" s="252"/>
+      <c r="E107" s="252"/>
+      <c r="F107" s="252"/>
+      <c r="G107" s="252"/>
+      <c r="H107" s="252"/>
+      <c r="I107" s="252"/>
+      <c r="J107" s="252"/>
+      <c r="K107" s="252"/>
+      <c r="L107" s="253"/>
     </row>
     <row r="108" spans="1:13" ht="15" customHeight="1">
       <c r="A108" s="13"/>
@@ -21412,19 +21412,19 @@
       <c r="L108" s="20"/>
     </row>
     <row r="109" spans="1:13">
-      <c r="B109" s="192" t="s">
+      <c r="B109" s="183" t="s">
         <v>118</v>
       </c>
-      <c r="C109" s="193"/>
-      <c r="D109" s="193"/>
-      <c r="E109" s="193"/>
-      <c r="F109" s="193"/>
-      <c r="G109" s="193"/>
-      <c r="H109" s="193"/>
-      <c r="I109" s="193"/>
-      <c r="J109" s="193"/>
-      <c r="K109" s="193"/>
-      <c r="L109" s="193"/>
+      <c r="C109" s="184"/>
+      <c r="D109" s="184"/>
+      <c r="E109" s="184"/>
+      <c r="F109" s="184"/>
+      <c r="G109" s="184"/>
+      <c r="H109" s="184"/>
+      <c r="I109" s="184"/>
+      <c r="J109" s="184"/>
+      <c r="K109" s="184"/>
+      <c r="L109" s="184"/>
     </row>
     <row r="110" spans="1:13" ht="15" customHeight="1">
       <c r="A110" s="13"/>
@@ -21548,8 +21548,8 @@
     </row>
     <row r="118" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A118" s="13"/>
-      <c r="B118" s="221"/>
-      <c r="C118" s="222"/>
+      <c r="B118" s="254"/>
+      <c r="C118" s="255"/>
       <c r="D118" s="63"/>
       <c r="E118" s="63"/>
       <c r="F118" s="62"/>
@@ -21562,8 +21562,8 @@
     </row>
     <row r="119" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A119" s="13"/>
-      <c r="B119" s="221"/>
-      <c r="C119" s="222"/>
+      <c r="B119" s="254"/>
+      <c r="C119" s="255"/>
       <c r="D119" s="63"/>
       <c r="E119" s="63"/>
       <c r="F119" s="62"/>
@@ -22030,7 +22030,7 @@
       <c r="K144" s="27"/>
       <c r="L144" s="27"/>
     </row>
-    <row r="145" spans="1:12" ht="15" customHeight="1" thickBot="1">
+    <row r="145" spans="1:13" ht="15" customHeight="1" thickBot="1">
       <c r="A145" s="13"/>
       <c r="B145" s="22"/>
       <c r="C145" s="20"/>
@@ -22044,7 +22044,7 @@
       <c r="K145" s="27"/>
       <c r="L145" s="27"/>
     </row>
-    <row r="146" spans="1:12" ht="25.5" customHeight="1" thickBot="1">
+    <row r="146" spans="1:13" ht="25.5" customHeight="1" thickBot="1">
       <c r="A146" s="13"/>
       <c r="B146" s="108" t="s">
         <v>1</v>
@@ -22072,7 +22072,7 @@
       <c r="K146" s="13"/>
       <c r="L146" s="13"/>
     </row>
-    <row r="147" spans="1:12" ht="15" customHeight="1">
+    <row r="147" spans="1:13" ht="15" customHeight="1">
       <c r="A147" s="13"/>
       <c r="B147" s="20"/>
       <c r="C147" s="20"/>
@@ -22086,7 +22086,7 @@
       <c r="K147" s="27"/>
       <c r="L147" s="27"/>
     </row>
-    <row r="148" spans="1:12" ht="23.25" customHeight="1">
+    <row r="148" spans="1:13" ht="23.25" customHeight="1">
       <c r="A148" s="13"/>
       <c r="B148" s="36" t="s">
         <v>11</v>
@@ -22117,7 +22117,7 @@
       <c r="K148" s="27"/>
       <c r="L148" s="27"/>
     </row>
-    <row r="149" spans="1:12" ht="15" customHeight="1">
+    <row r="149" spans="1:13" ht="15" customHeight="1">
       <c r="A149" s="13"/>
       <c r="B149" s="20"/>
       <c r="C149" s="20"/>
@@ -22131,7 +22131,7 @@
       <c r="K149" s="27"/>
       <c r="L149" s="27"/>
     </row>
-    <row r="150" spans="1:12" ht="23.25" customHeight="1">
+    <row r="150" spans="1:13" ht="23.25" customHeight="1">
       <c r="A150" s="13"/>
       <c r="B150" s="36">
         <v>31</v>
@@ -22142,10 +22142,12 @@
       <c r="D150" s="38">
         <v>7</v>
       </c>
-      <c r="E150" s="54"/>
+      <c r="E150" s="54">
+        <v>132</v>
+      </c>
       <c r="F150" s="33">
         <f>IF(ISBLANK(E150),0,IF(E150=Answers!E150,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G150" s="100" t="s">
         <v>62</v>
@@ -22156,11 +22158,22 @@
       <c r="I150" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="J150" s="29"/>
-      <c r="K150" s="27"/>
-      <c r="L150" s="27"/>
-    </row>
-    <row r="151" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J150" s="29" cm="1">
+        <f t="array" ref="J150:L150">_xlfn.XLOOKUP(G150:I150,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>3</v>
+      </c>
+      <c r="K150" s="27">
+        <v>12</v>
+      </c>
+      <c r="L150" s="27">
+        <v>11</v>
+      </c>
+      <c r="M150">
+        <f>LCM(_xlfn.ANCHORARRAY(J150))</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" ht="23.25" customHeight="1">
       <c r="A151" s="13"/>
       <c r="B151" s="36">
         <v>32</v>
@@ -22171,10 +22184,12 @@
       <c r="D151" s="38">
         <v>7</v>
       </c>
-      <c r="E151" s="54"/>
+      <c r="E151" s="54">
+        <v>63</v>
+      </c>
       <c r="F151" s="33">
         <f>IF(ISBLANK(E151),0,IF(E151=Answers!E151,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G151" s="100" t="s">
         <v>67</v>
@@ -22185,11 +22200,22 @@
       <c r="I151" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="J151" s="29"/>
-      <c r="K151" s="27"/>
-      <c r="L151" s="27"/>
-    </row>
-    <row r="152" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J151" s="29" cm="1">
+        <f t="array" ref="J151:L151">_xlfn.XLOOKUP(G151:I151,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>7</v>
+      </c>
+      <c r="K151" s="27">
+        <v>3</v>
+      </c>
+      <c r="L151" s="27">
+        <v>9</v>
+      </c>
+      <c r="M151">
+        <f t="shared" ref="M151:M169" si="0">LCM(_xlfn.ANCHORARRAY(J151))</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" ht="23.25" customHeight="1">
       <c r="A152" s="13"/>
       <c r="B152" s="36">
         <v>33</v>
@@ -22200,10 +22226,12 @@
       <c r="D152" s="38">
         <v>7</v>
       </c>
-      <c r="E152" s="54"/>
+      <c r="E152" s="54">
+        <v>20</v>
+      </c>
       <c r="F152" s="33">
         <f>IF(ISBLANK(E152),0,IF(E152=Answers!E152,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G152" s="100" t="s">
         <v>70</v>
@@ -22214,11 +22242,22 @@
       <c r="I152" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="J152" s="29"/>
-      <c r="K152" s="27"/>
-      <c r="L152" s="27"/>
-    </row>
-    <row r="153" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J152" s="29" cm="1">
+        <f t="array" ref="J152:L152">_xlfn.XLOOKUP(G152:I152,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>10</v>
+      </c>
+      <c r="K152" s="27">
+        <v>4</v>
+      </c>
+      <c r="L152" s="27">
+        <v>5</v>
+      </c>
+      <c r="M152">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" ht="23.25" customHeight="1">
       <c r="A153" s="13"/>
       <c r="B153" s="36">
         <v>34</v>
@@ -22229,10 +22268,12 @@
       <c r="D153" s="38">
         <v>7</v>
       </c>
-      <c r="E153" s="54"/>
+      <c r="E153" s="54">
+        <v>70</v>
+      </c>
       <c r="F153" s="33">
         <f>IF(ISBLANK(E153),0,IF(E153=Answers!E153,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G153" s="100" t="s">
         <v>65</v>
@@ -22243,11 +22284,22 @@
       <c r="I153" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="J153" s="29"/>
-      <c r="K153" s="27"/>
-      <c r="L153" s="27"/>
-    </row>
-    <row r="154" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J153" s="29" cm="1">
+        <f t="array" ref="J153:L153">_xlfn.XLOOKUP(G153:I153,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>5</v>
+      </c>
+      <c r="K153" s="27">
+        <v>2</v>
+      </c>
+      <c r="L153" s="27">
+        <v>7</v>
+      </c>
+      <c r="M153">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" ht="23.25" customHeight="1">
       <c r="A154" s="13"/>
       <c r="B154" s="36">
         <v>35</v>
@@ -22258,10 +22310,12 @@
       <c r="D154" s="38">
         <v>7</v>
       </c>
-      <c r="E154" s="54"/>
+      <c r="E154" s="54">
+        <v>140</v>
+      </c>
       <c r="F154" s="33">
         <f>IF(ISBLANK(E154),0,IF(E154=Answers!E154,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G154" s="100" t="s">
         <v>63</v>
@@ -22272,11 +22326,22 @@
       <c r="I154" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="J154" s="29"/>
-      <c r="K154" s="27"/>
-      <c r="L154" s="27"/>
-    </row>
-    <row r="155" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J154" s="29" cm="1">
+        <f t="array" ref="J154:L154">_xlfn.XLOOKUP(G154:I154,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>4</v>
+      </c>
+      <c r="K154" s="27">
+        <v>10</v>
+      </c>
+      <c r="L154" s="27">
+        <v>7</v>
+      </c>
+      <c r="M154">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" ht="23.25" customHeight="1">
       <c r="A155" s="13"/>
       <c r="B155" s="36">
         <v>36</v>
@@ -22287,10 +22352,12 @@
       <c r="D155" s="38">
         <v>7</v>
       </c>
-      <c r="E155" s="54"/>
+      <c r="E155" s="54">
+        <v>210</v>
+      </c>
       <c r="F155" s="33">
         <f>IF(ISBLANK(E155),0,IF(E155=Answers!E155,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G155" s="100" t="s">
         <v>70</v>
@@ -22301,11 +22368,22 @@
       <c r="I155" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="J155" s="29"/>
-      <c r="K155" s="27"/>
-      <c r="L155" s="27"/>
-    </row>
-    <row r="156" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J155" s="29" cm="1">
+        <f t="array" ref="J155:L155">_xlfn.XLOOKUP(G155:I155,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>10</v>
+      </c>
+      <c r="K155" s="27">
+        <v>3</v>
+      </c>
+      <c r="L155" s="27">
+        <v>7</v>
+      </c>
+      <c r="M155">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" ht="23.25" customHeight="1">
       <c r="A156" s="13"/>
       <c r="B156" s="36">
         <v>37</v>
@@ -22316,10 +22394,12 @@
       <c r="D156" s="38">
         <v>7</v>
       </c>
-      <c r="E156" s="54"/>
+      <c r="E156" s="54">
+        <v>126</v>
+      </c>
       <c r="F156" s="33">
         <f>IF(ISBLANK(E156),0,IF(E156=Answers!E156,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G156" s="100" t="s">
         <v>66</v>
@@ -22330,11 +22410,22 @@
       <c r="I156" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="J156" s="29"/>
-      <c r="K156" s="27"/>
-      <c r="L156" s="27"/>
-    </row>
-    <row r="157" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J156" s="29" cm="1">
+        <f t="array" ref="J156:L156">_xlfn.XLOOKUP(G156:I156,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>6</v>
+      </c>
+      <c r="K156" s="27">
+        <v>7</v>
+      </c>
+      <c r="L156" s="27">
+        <v>9</v>
+      </c>
+      <c r="M156">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" ht="23.25" customHeight="1">
       <c r="A157" s="13"/>
       <c r="B157" s="36">
         <v>38</v>
@@ -22345,10 +22436,12 @@
       <c r="D157" s="38">
         <v>7</v>
       </c>
-      <c r="E157" s="54"/>
+      <c r="E157" s="54">
+        <v>231</v>
+      </c>
       <c r="F157" s="33">
         <f>IF(ISBLANK(E157),0,IF(E157=Answers!E157,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G157" s="100" t="s">
         <v>67</v>
@@ -22359,11 +22452,22 @@
       <c r="I157" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="J157" s="29"/>
-      <c r="K157" s="27"/>
-      <c r="L157" s="27"/>
-    </row>
-    <row r="158" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J157" s="29" cm="1">
+        <f t="array" ref="J157:L157">_xlfn.XLOOKUP(G157:I157,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>7</v>
+      </c>
+      <c r="K157" s="27">
+        <v>11</v>
+      </c>
+      <c r="L157" s="27">
+        <v>3</v>
+      </c>
+      <c r="M157">
+        <f t="shared" si="0"/>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" ht="23.25" customHeight="1">
       <c r="A158" s="13"/>
       <c r="B158" s="36">
         <v>39</v>
@@ -22374,10 +22478,12 @@
       <c r="D158" s="38">
         <v>7</v>
       </c>
-      <c r="E158" s="54"/>
+      <c r="E158" s="54">
+        <v>12</v>
+      </c>
       <c r="F158" s="33">
         <f>IF(ISBLANK(E158),0,IF(E158=Answers!E158,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G158" s="100" t="s">
         <v>72</v>
@@ -22388,11 +22494,22 @@
       <c r="I158" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="J158" s="29"/>
-      <c r="K158" s="27"/>
-      <c r="L158" s="27"/>
-    </row>
-    <row r="159" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J158" s="29" cm="1">
+        <f t="array" ref="J158:L158">_xlfn.XLOOKUP(G158:I158,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>12</v>
+      </c>
+      <c r="K158" s="27">
+        <v>3</v>
+      </c>
+      <c r="L158" s="27">
+        <v>12</v>
+      </c>
+      <c r="M158">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" ht="23.25" customHeight="1">
       <c r="A159" s="13"/>
       <c r="B159" s="36">
         <v>40</v>
@@ -22403,10 +22520,12 @@
       <c r="D159" s="38">
         <v>7</v>
       </c>
-      <c r="E159" s="54"/>
+      <c r="E159" s="54">
+        <v>14</v>
+      </c>
       <c r="F159" s="33">
         <f>IF(ISBLANK(E159),0,IF(E159=Answers!E159,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G159" s="100" t="s">
         <v>61</v>
@@ -22417,11 +22536,22 @@
       <c r="I159" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="J159" s="29"/>
-      <c r="K159" s="27"/>
-      <c r="L159" s="27"/>
-    </row>
-    <row r="160" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J159" s="29" cm="1">
+        <f t="array" ref="J159:L159">_xlfn.XLOOKUP(G159:I159,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>2</v>
+      </c>
+      <c r="K159" s="27">
+        <v>7</v>
+      </c>
+      <c r="L159" s="27">
+        <v>7</v>
+      </c>
+      <c r="M159">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" ht="23.25" customHeight="1">
       <c r="A160" s="13"/>
       <c r="B160" s="36">
         <v>41</v>
@@ -22432,10 +22562,12 @@
       <c r="D160" s="38">
         <v>7</v>
       </c>
-      <c r="E160" s="54"/>
+      <c r="E160" s="54">
+        <v>60</v>
+      </c>
       <c r="F160" s="33">
         <f>IF(ISBLANK(E160),0,IF(E160=Answers!E160,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G160" s="100" t="s">
         <v>63</v>
@@ -22446,11 +22578,22 @@
       <c r="I160" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="J160" s="29"/>
-      <c r="K160" s="27"/>
-      <c r="L160" s="27"/>
-    </row>
-    <row r="161" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J160" s="29" cm="1">
+        <f t="array" ref="J160:L160">_xlfn.XLOOKUP(G160:I160,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>4</v>
+      </c>
+      <c r="K160" s="27">
+        <v>6</v>
+      </c>
+      <c r="L160" s="27">
+        <v>10</v>
+      </c>
+      <c r="M160">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" ht="23.25" customHeight="1">
       <c r="A161" s="13"/>
       <c r="B161" s="36">
         <v>42</v>
@@ -22461,10 +22604,12 @@
       <c r="D161" s="38">
         <v>7</v>
       </c>
-      <c r="E161" s="54"/>
+      <c r="E161" s="54">
+        <v>616</v>
+      </c>
       <c r="F161" s="33">
         <f>IF(ISBLANK(E161),0,IF(E161=Answers!E161,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G161" s="100" t="s">
         <v>67</v>
@@ -22475,11 +22620,22 @@
       <c r="I161" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="J161" s="29"/>
-      <c r="K161" s="27"/>
-      <c r="L161" s="27"/>
-    </row>
-    <row r="162" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J161" s="29" cm="1">
+        <f t="array" ref="J161:L161">_xlfn.XLOOKUP(G161:I161,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>7</v>
+      </c>
+      <c r="K161" s="27">
+        <v>11</v>
+      </c>
+      <c r="L161" s="27">
+        <v>8</v>
+      </c>
+      <c r="M161">
+        <f t="shared" si="0"/>
+        <v>616</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" ht="23.25" customHeight="1">
       <c r="A162" s="13"/>
       <c r="B162" s="36">
         <v>43</v>
@@ -22490,10 +22646,12 @@
       <c r="D162" s="38">
         <v>7</v>
       </c>
-      <c r="E162" s="54"/>
+      <c r="E162" s="54">
+        <v>180</v>
+      </c>
       <c r="F162" s="33">
         <f>IF(ISBLANK(E162),0,IF(E162=Answers!E162,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G162" s="100" t="s">
         <v>70</v>
@@ -22504,11 +22662,22 @@
       <c r="I162" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="J162" s="29"/>
-      <c r="K162" s="27"/>
-      <c r="L162" s="27"/>
-    </row>
-    <row r="163" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J162" s="29" cm="1">
+        <f t="array" ref="J162:L162">_xlfn.XLOOKUP(G162:I162,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>10</v>
+      </c>
+      <c r="K162" s="27">
+        <v>9</v>
+      </c>
+      <c r="L162" s="27">
+        <v>12</v>
+      </c>
+      <c r="M162">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" ht="23.25" customHeight="1">
       <c r="A163" s="13"/>
       <c r="B163" s="36">
         <v>44</v>
@@ -22519,10 +22688,12 @@
       <c r="D163" s="38">
         <v>7</v>
       </c>
-      <c r="E163" s="54"/>
+      <c r="E163" s="54">
+        <v>8</v>
+      </c>
       <c r="F163" s="33">
         <f>IF(ISBLANK(E163),0,IF(E163=Answers!E163,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G163" s="100" t="s">
         <v>63</v>
@@ -22533,11 +22704,22 @@
       <c r="I163" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="J163" s="29"/>
-      <c r="K163" s="27"/>
-      <c r="L163" s="27"/>
-    </row>
-    <row r="164" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J163" s="29" cm="1">
+        <f t="array" ref="J163:L163">_xlfn.XLOOKUP(G163:I163,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>4</v>
+      </c>
+      <c r="K163" s="27">
+        <v>2</v>
+      </c>
+      <c r="L163" s="27">
+        <v>8</v>
+      </c>
+      <c r="M163">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" ht="23.25" customHeight="1">
       <c r="A164" s="13"/>
       <c r="B164" s="36">
         <v>45</v>
@@ -22548,10 +22730,12 @@
       <c r="D164" s="38">
         <v>7</v>
       </c>
-      <c r="E164" s="54"/>
+      <c r="E164" s="54">
+        <v>330</v>
+      </c>
       <c r="F164" s="33">
         <f>IF(ISBLANK(E164),0,IF(E164=Answers!E164,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G164" s="100" t="s">
         <v>71</v>
@@ -22562,11 +22746,22 @@
       <c r="I164" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="J164" s="29"/>
-      <c r="K164" s="27"/>
-      <c r="L164" s="27"/>
-    </row>
-    <row r="165" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J164" s="29" cm="1">
+        <f t="array" ref="J164:L164">_xlfn.XLOOKUP(G164:I164,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>11</v>
+      </c>
+      <c r="K164" s="27">
+        <v>6</v>
+      </c>
+      <c r="L164" s="27">
+        <v>10</v>
+      </c>
+      <c r="M164">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" ht="23.25" customHeight="1">
       <c r="A165" s="13"/>
       <c r="B165" s="36">
         <v>46</v>
@@ -22577,10 +22772,12 @@
       <c r="D165" s="38">
         <v>7</v>
       </c>
-      <c r="E165" s="54"/>
+      <c r="E165" s="54">
+        <v>18</v>
+      </c>
       <c r="F165" s="33">
         <f>IF(ISBLANK(E165),0,IF(E165=Answers!E165,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G165" s="100" t="s">
         <v>61</v>
@@ -22591,11 +22788,22 @@
       <c r="I165" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="J165" s="29"/>
-      <c r="K165" s="27"/>
-      <c r="L165" s="27"/>
-    </row>
-    <row r="166" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J165" s="29" cm="1">
+        <f t="array" ref="J165:L165">_xlfn.XLOOKUP(G165:I165,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>2</v>
+      </c>
+      <c r="K165" s="27">
+        <v>2</v>
+      </c>
+      <c r="L165" s="27">
+        <v>9</v>
+      </c>
+      <c r="M165">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" ht="23.25" customHeight="1">
       <c r="A166" s="13"/>
       <c r="B166" s="36">
         <v>47</v>
@@ -22606,10 +22814,12 @@
       <c r="D166" s="38">
         <v>7</v>
       </c>
-      <c r="E166" s="54"/>
+      <c r="E166" s="54">
+        <v>180</v>
+      </c>
       <c r="F166" s="33">
         <f>IF(ISBLANK(E166),0,IF(E166=Answers!E166,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G166" s="100" t="s">
         <v>63</v>
@@ -22620,11 +22830,22 @@
       <c r="I166" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="J166" s="29"/>
-      <c r="K166" s="27"/>
-      <c r="L166" s="27"/>
-    </row>
-    <row r="167" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J166" s="29" cm="1">
+        <f t="array" ref="J166:L166">_xlfn.XLOOKUP(G166:I166,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>4</v>
+      </c>
+      <c r="K166" s="27">
+        <v>5</v>
+      </c>
+      <c r="L166" s="27">
+        <v>9</v>
+      </c>
+      <c r="M166">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" ht="23.25" customHeight="1">
       <c r="A167" s="13"/>
       <c r="B167" s="36">
         <v>48</v>
@@ -22635,10 +22856,12 @@
       <c r="D167" s="38">
         <v>7</v>
       </c>
-      <c r="E167" s="54"/>
+      <c r="E167" s="54">
+        <v>36</v>
+      </c>
       <c r="F167" s="33">
         <f>IF(ISBLANK(E167),0,IF(E167=Answers!E167,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G167" s="100" t="s">
         <v>63</v>
@@ -22649,11 +22872,22 @@
       <c r="I167" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="J167" s="29"/>
-      <c r="K167" s="27"/>
-      <c r="L167" s="27"/>
-    </row>
-    <row r="168" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J167" s="29" cm="1">
+        <f t="array" ref="J167:L167">_xlfn.XLOOKUP(G167:I167,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>4</v>
+      </c>
+      <c r="K167" s="27">
+        <v>9</v>
+      </c>
+      <c r="L167" s="27">
+        <v>3</v>
+      </c>
+      <c r="M167">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" ht="23.25" customHeight="1">
       <c r="A168" s="13"/>
       <c r="B168" s="36">
         <v>49</v>
@@ -22664,10 +22898,12 @@
       <c r="D168" s="38">
         <v>7</v>
       </c>
-      <c r="E168" s="54"/>
+      <c r="E168" s="54">
+        <v>360</v>
+      </c>
       <c r="F168" s="33">
         <f>IF(ISBLANK(E168),0,IF(E168=Answers!E168,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G168" s="100" t="s">
         <v>69</v>
@@ -22678,11 +22914,22 @@
       <c r="I168" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="J168" s="29"/>
-      <c r="K168" s="27"/>
-      <c r="L168" s="27"/>
-    </row>
-    <row r="169" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J168" s="29" cm="1">
+        <f t="array" ref="J168:L168">_xlfn.XLOOKUP(G168:I168,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>9</v>
+      </c>
+      <c r="K168" s="27">
+        <v>8</v>
+      </c>
+      <c r="L168" s="27">
+        <v>10</v>
+      </c>
+      <c r="M168">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" ht="23.25" customHeight="1">
       <c r="A169" s="13"/>
       <c r="B169" s="36">
         <v>50</v>
@@ -22693,10 +22940,12 @@
       <c r="D169" s="38">
         <v>7</v>
       </c>
-      <c r="E169" s="54"/>
+      <c r="E169" s="54">
+        <v>1001</v>
+      </c>
       <c r="F169" s="33">
         <f>IF(ISBLANK(E169),0,IF(E169=Answers!E169,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G169" s="100" t="s">
         <v>67</v>
@@ -22707,11 +22956,22 @@
       <c r="I169" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="J169" s="29"/>
-      <c r="K169" s="27"/>
-      <c r="L169" s="27"/>
-    </row>
-    <row r="170" spans="1:12" ht="15" customHeight="1">
+      <c r="J169" s="29" cm="1">
+        <f t="array" ref="J169:L169">_xlfn.XLOOKUP(G169:I169,TRANSPOSE($I$120:$I$131),TRANSPOSE($J$120:$J$131))</f>
+        <v>7</v>
+      </c>
+      <c r="K169" s="27">
+        <v>11</v>
+      </c>
+      <c r="L169" s="27">
+        <v>13</v>
+      </c>
+      <c r="M169">
+        <f t="shared" si="0"/>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" ht="15" customHeight="1">
       <c r="A170" s="27"/>
       <c r="B170" s="27"/>
       <c r="C170" s="27"/>
@@ -22725,7 +22985,7 @@
       <c r="K170" s="27"/>
       <c r="L170" s="27"/>
     </row>
-    <row r="171" spans="1:12" ht="15" customHeight="1" thickBot="1">
+    <row r="171" spans="1:13" ht="15" customHeight="1" thickBot="1">
       <c r="A171" s="27"/>
       <c r="B171" s="27"/>
       <c r="C171" s="27"/>
@@ -22739,7 +22999,7 @@
       <c r="K171" s="27"/>
       <c r="L171" s="27"/>
     </row>
-    <row r="172" spans="1:12" ht="25.5" customHeight="1" thickBot="1">
+    <row r="172" spans="1:13" ht="25.5" customHeight="1" thickBot="1">
       <c r="A172" s="13"/>
       <c r="B172" s="115" t="s">
         <v>26</v>
@@ -22757,7 +23017,7 @@
       <c r="K172" s="27"/>
       <c r="L172" s="13"/>
     </row>
-    <row r="173" spans="1:12" ht="15" customHeight="1">
+    <row r="173" spans="1:13" ht="15" customHeight="1">
       <c r="A173" s="13"/>
       <c r="B173" s="22"/>
       <c r="C173" s="20"/>
@@ -22771,7 +23031,7 @@
       <c r="K173" s="13"/>
       <c r="L173" s="13"/>
     </row>
-    <row r="174" spans="1:12" ht="15" customHeight="1">
+    <row r="174" spans="1:13" ht="15" customHeight="1">
       <c r="A174" s="13"/>
       <c r="B174" s="48" t="s">
         <v>314</v>
@@ -22787,7 +23047,7 @@
       <c r="K174" s="13"/>
       <c r="L174" s="13"/>
     </row>
-    <row r="175" spans="1:12" ht="15" customHeight="1">
+    <row r="175" spans="1:13" ht="15" customHeight="1">
       <c r="A175" s="13"/>
       <c r="B175" s="48" t="s">
         <v>200</v>
@@ -22803,7 +23063,7 @@
       <c r="K175" s="13"/>
       <c r="L175" s="13"/>
     </row>
-    <row r="176" spans="1:12" ht="15" customHeight="1">
+    <row r="176" spans="1:13" ht="15" customHeight="1">
       <c r="A176" s="13"/>
       <c r="B176" s="48" t="s">
         <v>201</v>
@@ -24514,128 +24774,140 @@
       <c r="L262" s="27"/>
     </row>
     <row r="263" spans="1:12">
-      <c r="B263" s="192" t="s">
+      <c r="B263" s="183" t="s">
         <v>22</v>
       </c>
-      <c r="C263" s="193"/>
-      <c r="D263" s="193"/>
-      <c r="E263" s="193"/>
-      <c r="F263" s="193"/>
-      <c r="G263" s="193"/>
-      <c r="H263" s="193"/>
-      <c r="I263" s="193"/>
-      <c r="J263" s="193"/>
-      <c r="K263" s="193"/>
-      <c r="L263" s="193"/>
+      <c r="C263" s="184"/>
+      <c r="D263" s="184"/>
+      <c r="E263" s="184"/>
+      <c r="F263" s="184"/>
+      <c r="G263" s="184"/>
+      <c r="H263" s="184"/>
+      <c r="I263" s="184"/>
+      <c r="J263" s="184"/>
+      <c r="K263" s="184"/>
+      <c r="L263" s="184"/>
     </row>
     <row r="264" spans="1:12">
-      <c r="B264" s="183" t="s">
+      <c r="B264" s="218" t="s">
         <v>317</v>
       </c>
-      <c r="C264" s="184"/>
-      <c r="D264" s="184"/>
-      <c r="E264" s="184"/>
-      <c r="F264" s="184"/>
-      <c r="G264" s="184"/>
-      <c r="H264" s="184"/>
-      <c r="I264" s="184"/>
-      <c r="J264" s="184"/>
-      <c r="K264" s="184"/>
-      <c r="L264" s="185"/>
+      <c r="C264" s="219"/>
+      <c r="D264" s="219"/>
+      <c r="E264" s="219"/>
+      <c r="F264" s="219"/>
+      <c r="G264" s="219"/>
+      <c r="H264" s="219"/>
+      <c r="I264" s="219"/>
+      <c r="J264" s="219"/>
+      <c r="K264" s="219"/>
+      <c r="L264" s="220"/>
     </row>
     <row r="265" spans="1:12">
-      <c r="B265" s="186"/>
-      <c r="C265" s="187"/>
-      <c r="D265" s="187"/>
-      <c r="E265" s="187"/>
-      <c r="F265" s="187"/>
-      <c r="G265" s="187"/>
-      <c r="H265" s="187"/>
-      <c r="I265" s="187"/>
-      <c r="J265" s="187"/>
-      <c r="K265" s="187"/>
-      <c r="L265" s="188"/>
+      <c r="B265" s="221"/>
+      <c r="C265" s="222"/>
+      <c r="D265" s="222"/>
+      <c r="E265" s="222"/>
+      <c r="F265" s="222"/>
+      <c r="G265" s="222"/>
+      <c r="H265" s="222"/>
+      <c r="I265" s="222"/>
+      <c r="J265" s="222"/>
+      <c r="K265" s="222"/>
+      <c r="L265" s="223"/>
     </row>
     <row r="266" spans="1:12">
-      <c r="B266" s="186"/>
-      <c r="C266" s="187"/>
-      <c r="D266" s="187"/>
-      <c r="E266" s="187"/>
-      <c r="F266" s="187"/>
-      <c r="G266" s="187"/>
-      <c r="H266" s="187"/>
-      <c r="I266" s="187"/>
-      <c r="J266" s="187"/>
-      <c r="K266" s="187"/>
-      <c r="L266" s="188"/>
+      <c r="B266" s="221"/>
+      <c r="C266" s="222"/>
+      <c r="D266" s="222"/>
+      <c r="E266" s="222"/>
+      <c r="F266" s="222"/>
+      <c r="G266" s="222"/>
+      <c r="H266" s="222"/>
+      <c r="I266" s="222"/>
+      <c r="J266" s="222"/>
+      <c r="K266" s="222"/>
+      <c r="L266" s="223"/>
     </row>
     <row r="267" spans="1:12">
-      <c r="B267" s="186"/>
-      <c r="C267" s="187"/>
-      <c r="D267" s="187"/>
-      <c r="E267" s="187"/>
-      <c r="F267" s="187"/>
-      <c r="G267" s="187"/>
-      <c r="H267" s="187"/>
-      <c r="I267" s="187"/>
-      <c r="J267" s="187"/>
-      <c r="K267" s="187"/>
-      <c r="L267" s="188"/>
+      <c r="B267" s="221"/>
+      <c r="C267" s="222"/>
+      <c r="D267" s="222"/>
+      <c r="E267" s="222"/>
+      <c r="F267" s="222"/>
+      <c r="G267" s="222"/>
+      <c r="H267" s="222"/>
+      <c r="I267" s="222"/>
+      <c r="J267" s="222"/>
+      <c r="K267" s="222"/>
+      <c r="L267" s="223"/>
     </row>
     <row r="268" spans="1:12">
-      <c r="B268" s="186"/>
-      <c r="C268" s="187"/>
-      <c r="D268" s="187"/>
-      <c r="E268" s="187"/>
-      <c r="F268" s="187"/>
-      <c r="G268" s="187"/>
-      <c r="H268" s="187"/>
-      <c r="I268" s="187"/>
-      <c r="J268" s="187"/>
-      <c r="K268" s="187"/>
-      <c r="L268" s="188"/>
+      <c r="B268" s="221"/>
+      <c r="C268" s="222"/>
+      <c r="D268" s="222"/>
+      <c r="E268" s="222"/>
+      <c r="F268" s="222"/>
+      <c r="G268" s="222"/>
+      <c r="H268" s="222"/>
+      <c r="I268" s="222"/>
+      <c r="J268" s="222"/>
+      <c r="K268" s="222"/>
+      <c r="L268" s="223"/>
     </row>
     <row r="269" spans="1:12">
-      <c r="B269" s="186"/>
-      <c r="C269" s="187"/>
-      <c r="D269" s="187"/>
-      <c r="E269" s="187"/>
-      <c r="F269" s="187"/>
-      <c r="G269" s="187"/>
-      <c r="H269" s="187"/>
-      <c r="I269" s="187"/>
-      <c r="J269" s="187"/>
-      <c r="K269" s="187"/>
-      <c r="L269" s="188"/>
+      <c r="B269" s="221"/>
+      <c r="C269" s="222"/>
+      <c r="D269" s="222"/>
+      <c r="E269" s="222"/>
+      <c r="F269" s="222"/>
+      <c r="G269" s="222"/>
+      <c r="H269" s="222"/>
+      <c r="I269" s="222"/>
+      <c r="J269" s="222"/>
+      <c r="K269" s="222"/>
+      <c r="L269" s="223"/>
     </row>
     <row r="270" spans="1:12">
-      <c r="B270" s="186"/>
-      <c r="C270" s="187"/>
-      <c r="D270" s="187"/>
-      <c r="E270" s="187"/>
-      <c r="F270" s="187"/>
-      <c r="G270" s="187"/>
-      <c r="H270" s="187"/>
-      <c r="I270" s="187"/>
-      <c r="J270" s="187"/>
-      <c r="K270" s="187"/>
-      <c r="L270" s="188"/>
+      <c r="B270" s="221"/>
+      <c r="C270" s="222"/>
+      <c r="D270" s="222"/>
+      <c r="E270" s="222"/>
+      <c r="F270" s="222"/>
+      <c r="G270" s="222"/>
+      <c r="H270" s="222"/>
+      <c r="I270" s="222"/>
+      <c r="J270" s="222"/>
+      <c r="K270" s="222"/>
+      <c r="L270" s="223"/>
     </row>
     <row r="271" spans="1:12">
-      <c r="B271" s="189"/>
-      <c r="C271" s="190"/>
-      <c r="D271" s="190"/>
-      <c r="E271" s="190"/>
-      <c r="F271" s="190"/>
-      <c r="G271" s="190"/>
-      <c r="H271" s="190"/>
-      <c r="I271" s="190"/>
-      <c r="J271" s="190"/>
-      <c r="K271" s="190"/>
-      <c r="L271" s="191"/>
+      <c r="B271" s="224"/>
+      <c r="C271" s="225"/>
+      <c r="D271" s="225"/>
+      <c r="E271" s="225"/>
+      <c r="F271" s="225"/>
+      <c r="G271" s="225"/>
+      <c r="H271" s="225"/>
+      <c r="I271" s="225"/>
+      <c r="J271" s="225"/>
+      <c r="K271" s="225"/>
+      <c r="L271" s="226"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B264:L271"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L36"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I63:J64"/>
+    <mergeCell ref="K63:L64"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="B100:L100"/>
+    <mergeCell ref="B101:L107"/>
+    <mergeCell ref="B109:L109"/>
+    <mergeCell ref="B118:C119"/>
+    <mergeCell ref="B263:L263"/>
     <mergeCell ref="B30:L30"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B4:L4"/>
@@ -24648,18 +24920,6 @@
     <mergeCell ref="G26:L26"/>
     <mergeCell ref="G27:L27"/>
     <mergeCell ref="G28:L28"/>
-    <mergeCell ref="B264:L271"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L36"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I63:J64"/>
-    <mergeCell ref="K63:L64"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="B100:L100"/>
-    <mergeCell ref="B101:L107"/>
-    <mergeCell ref="B109:L109"/>
-    <mergeCell ref="B118:C119"/>
-    <mergeCell ref="B263:L263"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24715,15 +24975,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="22.8">
-      <c r="B2" s="192" t="s">
+      <c r="B2" s="183" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="193"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="184"/>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="179" t="s">
@@ -25013,15 +25273,15 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="22.8">
-      <c r="B18" s="192" t="s">
+      <c r="B18" s="183" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="193"/>
-      <c r="D18" s="193"/>
-      <c r="E18" s="193"/>
-      <c r="F18" s="193"/>
-      <c r="G18" s="193"/>
-      <c r="H18" s="193"/>
+      <c r="C18" s="184"/>
+      <c r="D18" s="184"/>
+      <c r="E18" s="184"/>
+      <c r="F18" s="184"/>
+      <c r="G18" s="184"/>
+      <c r="H18" s="184"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="U5:X14">
@@ -29609,8 +29869,8 @@
   </sheetPr>
   <dimension ref="A1:L271"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView showGridLines="0" topLeftCell="A152" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K160" sqref="K160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.6640625" defaultRowHeight="25.8" outlineLevelRow="1"/>
@@ -29632,19 +29892,19 @@
       <c r="A1"/>
     </row>
     <row r="2" spans="1:12" ht="59.25" customHeight="1">
-      <c r="B2" s="223" t="s">
+      <c r="B2" s="185" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
-      <c r="L2" s="224"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="186"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" outlineLevel="1">
       <c r="A3"/>
@@ -29661,19 +29921,19 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" ht="75" customHeight="1" outlineLevel="1">
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="187" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="225"/>
-      <c r="D4" s="225"/>
-      <c r="E4" s="225"/>
-      <c r="F4" s="225"/>
-      <c r="G4" s="225"/>
-      <c r="H4" s="225"/>
-      <c r="I4" s="225"/>
-      <c r="J4" s="225"/>
-      <c r="K4" s="225"/>
-      <c r="L4" s="225"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="187"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="B5" s="2"/>
@@ -29689,112 +29949,112 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="33" customHeight="1">
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="193"/>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="193"/>
-      <c r="H6" s="193"/>
-      <c r="I6" s="226"/>
+      <c r="C6" s="184"/>
+      <c r="D6" s="184"/>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="184"/>
+      <c r="H6" s="184"/>
+      <c r="I6" s="188"/>
       <c r="J6"/>
-      <c r="K6" s="227" t="s">
+      <c r="K6" s="189" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="228"/>
+      <c r="L6" s="190"/>
     </row>
     <row r="7" spans="1:12" ht="25.95" customHeight="1">
-      <c r="B7" s="229" t="s">
+      <c r="B7" s="191" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="230"/>
-      <c r="D7" s="230"/>
-      <c r="E7" s="230"/>
-      <c r="F7" s="230"/>
-      <c r="G7" s="230"/>
-      <c r="H7" s="230"/>
-      <c r="I7" s="231"/>
+      <c r="C7" s="192"/>
+      <c r="D7" s="192"/>
+      <c r="E7" s="192"/>
+      <c r="F7" s="192"/>
+      <c r="G7" s="192"/>
+      <c r="H7" s="192"/>
+      <c r="I7" s="193"/>
       <c r="K7" s="5"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="232"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233"/>
-      <c r="H8" s="233"/>
-      <c r="I8" s="234"/>
+      <c r="B8" s="194"/>
+      <c r="C8" s="195"/>
+      <c r="D8" s="195"/>
+      <c r="E8" s="195"/>
+      <c r="F8" s="195"/>
+      <c r="G8" s="195"/>
+      <c r="H8" s="195"/>
+      <c r="I8" s="196"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="232"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
-      <c r="G9" s="233"/>
-      <c r="H9" s="233"/>
-      <c r="I9" s="234"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="195"/>
+      <c r="D9" s="195"/>
+      <c r="E9" s="195"/>
+      <c r="F9" s="195"/>
+      <c r="G9" s="195"/>
+      <c r="H9" s="195"/>
+      <c r="I9" s="196"/>
       <c r="J9"/>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="B10" s="232"/>
-      <c r="C10" s="233"/>
-      <c r="D10" s="233"/>
-      <c r="E10" s="233"/>
-      <c r="F10" s="233"/>
-      <c r="G10" s="233"/>
-      <c r="H10" s="233"/>
-      <c r="I10" s="234"/>
+      <c r="B10" s="194"/>
+      <c r="C10" s="195"/>
+      <c r="D10" s="195"/>
+      <c r="E10" s="195"/>
+      <c r="F10" s="195"/>
+      <c r="G10" s="195"/>
+      <c r="H10" s="195"/>
+      <c r="I10" s="196"/>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="B11" s="232"/>
-      <c r="C11" s="233"/>
-      <c r="D11" s="233"/>
-      <c r="E11" s="233"/>
-      <c r="F11" s="233"/>
-      <c r="G11" s="233"/>
-      <c r="H11" s="233"/>
-      <c r="I11" s="234"/>
+      <c r="B11" s="194"/>
+      <c r="C11" s="195"/>
+      <c r="D11" s="195"/>
+      <c r="E11" s="195"/>
+      <c r="F11" s="195"/>
+      <c r="G11" s="195"/>
+      <c r="H11" s="195"/>
+      <c r="I11" s="196"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="B12" s="232"/>
-      <c r="C12" s="233"/>
-      <c r="D12" s="233"/>
-      <c r="E12" s="233"/>
-      <c r="F12" s="233"/>
-      <c r="G12" s="233"/>
-      <c r="H12" s="233"/>
-      <c r="I12" s="234"/>
+      <c r="B12" s="194"/>
+      <c r="C12" s="195"/>
+      <c r="D12" s="195"/>
+      <c r="E12" s="195"/>
+      <c r="F12" s="195"/>
+      <c r="G12" s="195"/>
+      <c r="H12" s="195"/>
+      <c r="I12" s="196"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:12" ht="23.25" customHeight="1">
-      <c r="B13" s="232"/>
-      <c r="C13" s="233"/>
-      <c r="D13" s="233"/>
-      <c r="E13" s="233"/>
-      <c r="F13" s="233"/>
-      <c r="G13" s="233"/>
-      <c r="H13" s="233"/>
-      <c r="I13" s="234"/>
+      <c r="B13" s="194"/>
+      <c r="C13" s="195"/>
+      <c r="D13" s="195"/>
+      <c r="E13" s="195"/>
+      <c r="F13" s="195"/>
+      <c r="G13" s="195"/>
+      <c r="H13" s="195"/>
+      <c r="I13" s="196"/>
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:12" ht="33" customHeight="1">
-      <c r="B14" s="235"/>
-      <c r="C14" s="236"/>
-      <c r="D14" s="236"/>
-      <c r="E14" s="236"/>
-      <c r="F14" s="236"/>
-      <c r="G14" s="236"/>
-      <c r="H14" s="236"/>
-      <c r="I14" s="237"/>
+      <c r="B14" s="197"/>
+      <c r="C14" s="198"/>
+      <c r="D14" s="198"/>
+      <c r="E14" s="198"/>
+      <c r="F14" s="198"/>
+      <c r="G14" s="198"/>
+      <c r="H14" s="198"/>
+      <c r="I14" s="199"/>
       <c r="K14" s="34" t="s">
         <v>0</v>
       </c>
@@ -29808,60 +30068,60 @@
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B16" s="192" t="s">
+      <c r="B16" s="183" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="193"/>
-      <c r="D16" s="193"/>
-      <c r="E16" s="193"/>
-      <c r="F16" s="193"/>
-      <c r="G16" s="193"/>
-      <c r="H16" s="193"/>
-      <c r="I16" s="193"/>
-      <c r="J16" s="193"/>
-      <c r="K16" s="193"/>
-      <c r="L16" s="193"/>
+      <c r="C16" s="184"/>
+      <c r="D16" s="184"/>
+      <c r="E16" s="184"/>
+      <c r="F16" s="184"/>
+      <c r="G16" s="184"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="184"/>
+      <c r="J16" s="184"/>
+      <c r="K16" s="184"/>
+      <c r="L16" s="184"/>
     </row>
     <row r="17" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B17" s="238" t="s">
+      <c r="B17" s="200" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="239"/>
-      <c r="D17" s="239"/>
-      <c r="E17" s="239"/>
-      <c r="F17" s="239"/>
-      <c r="G17" s="239"/>
-      <c r="H17" s="239"/>
-      <c r="I17" s="239"/>
-      <c r="J17" s="239"/>
-      <c r="K17" s="239"/>
-      <c r="L17" s="240"/>
+      <c r="C17" s="201"/>
+      <c r="D17" s="201"/>
+      <c r="E17" s="201"/>
+      <c r="F17" s="201"/>
+      <c r="G17" s="201"/>
+      <c r="H17" s="201"/>
+      <c r="I17" s="201"/>
+      <c r="J17" s="201"/>
+      <c r="K17" s="201"/>
+      <c r="L17" s="202"/>
     </row>
     <row r="18" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B18" s="241"/>
-      <c r="C18" s="242"/>
-      <c r="D18" s="242"/>
-      <c r="E18" s="242"/>
-      <c r="F18" s="242"/>
-      <c r="G18" s="242"/>
-      <c r="H18" s="242"/>
-      <c r="I18" s="242"/>
-      <c r="J18" s="242"/>
-      <c r="K18" s="242"/>
-      <c r="L18" s="243"/>
+      <c r="B18" s="203"/>
+      <c r="C18" s="204"/>
+      <c r="D18" s="204"/>
+      <c r="E18" s="204"/>
+      <c r="F18" s="204"/>
+      <c r="G18" s="204"/>
+      <c r="H18" s="204"/>
+      <c r="I18" s="204"/>
+      <c r="J18" s="204"/>
+      <c r="K18" s="204"/>
+      <c r="L18" s="205"/>
     </row>
     <row r="19" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B19" s="244"/>
-      <c r="C19" s="245"/>
-      <c r="D19" s="245"/>
-      <c r="E19" s="245"/>
-      <c r="F19" s="245"/>
-      <c r="G19" s="245"/>
-      <c r="H19" s="245"/>
-      <c r="I19" s="245"/>
-      <c r="J19" s="245"/>
-      <c r="K19" s="245"/>
-      <c r="L19" s="246"/>
+      <c r="B19" s="206"/>
+      <c r="C19" s="207"/>
+      <c r="D19" s="207"/>
+      <c r="E19" s="207"/>
+      <c r="F19" s="207"/>
+      <c r="G19" s="207"/>
+      <c r="H19" s="207"/>
+      <c r="I19" s="207"/>
+      <c r="J19" s="207"/>
+      <c r="K19" s="207"/>
+      <c r="L19" s="208"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="B20" s="8"/>
@@ -29877,19 +30137,19 @@
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B21" s="192" t="s">
+      <c r="B21" s="183" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="193"/>
-      <c r="D21" s="193"/>
-      <c r="E21" s="193"/>
-      <c r="F21" s="193"/>
-      <c r="G21" s="193"/>
-      <c r="H21" s="193"/>
-      <c r="I21" s="193"/>
-      <c r="J21" s="193"/>
-      <c r="K21" s="193"/>
-      <c r="L21" s="193"/>
+      <c r="C21" s="184"/>
+      <c r="D21" s="184"/>
+      <c r="E21" s="184"/>
+      <c r="F21" s="184"/>
+      <c r="G21" s="184"/>
+      <c r="H21" s="184"/>
+      <c r="I21" s="184"/>
+      <c r="J21" s="184"/>
+      <c r="K21" s="184"/>
+      <c r="L21" s="184"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="B22" s="9"/>
@@ -29970,14 +30230,14 @@
         <v>2</v>
       </c>
       <c r="F26" s="33"/>
-      <c r="G26" s="247" t="s">
+      <c r="G26" s="209" t="s">
         <v>187</v>
       </c>
-      <c r="H26" s="248"/>
-      <c r="I26" s="248"/>
-      <c r="J26" s="248"/>
-      <c r="K26" s="248"/>
-      <c r="L26" s="249"/>
+      <c r="H26" s="210"/>
+      <c r="I26" s="210"/>
+      <c r="J26" s="210"/>
+      <c r="K26" s="210"/>
+      <c r="L26" s="211"/>
     </row>
     <row r="27" spans="1:12" ht="33.75" customHeight="1">
       <c r="B27" s="36" t="s">
@@ -29993,14 +30253,14 @@
         <v>360360</v>
       </c>
       <c r="F27" s="33"/>
-      <c r="G27" s="250" t="s">
+      <c r="G27" s="212" t="s">
         <v>186</v>
       </c>
-      <c r="H27" s="251"/>
-      <c r="I27" s="251"/>
-      <c r="J27" s="251"/>
-      <c r="K27" s="251"/>
-      <c r="L27" s="252"/>
+      <c r="H27" s="213"/>
+      <c r="I27" s="213"/>
+      <c r="J27" s="213"/>
+      <c r="K27" s="213"/>
+      <c r="L27" s="214"/>
     </row>
     <row r="28" spans="1:12" ht="54" customHeight="1">
       <c r="B28" s="36" t="s">
@@ -30016,14 +30276,14 @@
         <v>312</v>
       </c>
       <c r="F28" s="33"/>
-      <c r="G28" s="253" t="s">
+      <c r="G28" s="215" t="s">
         <v>345</v>
       </c>
-      <c r="H28" s="254"/>
-      <c r="I28" s="254"/>
-      <c r="J28" s="254"/>
-      <c r="K28" s="254"/>
-      <c r="L28" s="255"/>
+      <c r="H28" s="216"/>
+      <c r="I28" s="216"/>
+      <c r="J28" s="216"/>
+      <c r="K28" s="216"/>
+      <c r="L28" s="217"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="B29" s="2"/>
@@ -30039,19 +30299,19 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="B30" s="192" t="s">
+      <c r="B30" s="183" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="193"/>
-      <c r="D30" s="193"/>
-      <c r="E30" s="193"/>
-      <c r="F30" s="193"/>
-      <c r="G30" s="193"/>
-      <c r="H30" s="193"/>
-      <c r="I30" s="193"/>
-      <c r="J30" s="193"/>
-      <c r="K30" s="193"/>
-      <c r="L30" s="193"/>
+      <c r="C30" s="184"/>
+      <c r="D30" s="184"/>
+      <c r="E30" s="184"/>
+      <c r="F30" s="184"/>
+      <c r="G30" s="184"/>
+      <c r="H30" s="184"/>
+      <c r="I30" s="184"/>
+      <c r="J30" s="184"/>
+      <c r="K30" s="184"/>
+      <c r="L30" s="184"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="B31" s="16"/>
@@ -30281,10 +30541,10 @@
         <v>122</v>
       </c>
       <c r="F45" s="18"/>
-      <c r="G45" s="200" t="s">
+      <c r="G45" s="233" t="s">
         <v>324</v>
       </c>
-      <c r="H45" s="201"/>
+      <c r="H45" s="234"/>
       <c r="I45" s="91" t="s">
         <v>52</v>
       </c>
@@ -30677,14 +30937,14 @@
       <c r="F63" s="18"/>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
-      <c r="I63" s="202" t="s">
+      <c r="I63" s="235" t="s">
         <v>138</v>
       </c>
-      <c r="J63" s="203"/>
-      <c r="K63" s="206" t="s">
+      <c r="J63" s="236"/>
+      <c r="K63" s="239" t="s">
         <v>141</v>
       </c>
-      <c r="L63" s="207"/>
+      <c r="L63" s="240"/>
     </row>
     <row r="64" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A64" s="13"/>
@@ -30697,10 +30957,10 @@
       <c r="F64" s="18"/>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
-      <c r="I64" s="204"/>
-      <c r="J64" s="205"/>
-      <c r="K64" s="208"/>
-      <c r="L64" s="209"/>
+      <c r="I64" s="237"/>
+      <c r="J64" s="238"/>
+      <c r="K64" s="241"/>
+      <c r="L64" s="242"/>
     </row>
     <row r="65" spans="1:12" ht="15" customHeight="1">
       <c r="A65" s="13"/>
@@ -30869,16 +31129,16 @@
         <v>349</v>
       </c>
       <c r="F75" s="85"/>
-      <c r="G75" s="210" t="s">
+      <c r="G75" s="243" t="s">
         <v>136</v>
       </c>
-      <c r="H75" s="211"/>
-      <c r="I75" s="211"/>
-      <c r="J75" s="212"/>
-      <c r="K75" s="210" t="s">
+      <c r="H75" s="244"/>
+      <c r="I75" s="244"/>
+      <c r="J75" s="245"/>
+      <c r="K75" s="243" t="s">
         <v>135</v>
       </c>
-      <c r="L75" s="212"/>
+      <c r="L75" s="245"/>
     </row>
     <row r="76" spans="1:12" ht="15" customHeight="1">
       <c r="A76" s="13"/>
@@ -31469,119 +31729,119 @@
       <c r="L99" s="20"/>
     </row>
     <row r="100" spans="1:12">
-      <c r="B100" s="192" t="s">
+      <c r="B100" s="183" t="s">
         <v>21</v>
       </c>
-      <c r="C100" s="193"/>
-      <c r="D100" s="193"/>
-      <c r="E100" s="193"/>
-      <c r="F100" s="193"/>
-      <c r="G100" s="193"/>
-      <c r="H100" s="193"/>
-      <c r="I100" s="193"/>
-      <c r="J100" s="193"/>
-      <c r="K100" s="193"/>
-      <c r="L100" s="193"/>
+      <c r="C100" s="184"/>
+      <c r="D100" s="184"/>
+      <c r="E100" s="184"/>
+      <c r="F100" s="184"/>
+      <c r="G100" s="184"/>
+      <c r="H100" s="184"/>
+      <c r="I100" s="184"/>
+      <c r="J100" s="184"/>
+      <c r="K100" s="184"/>
+      <c r="L100" s="184"/>
     </row>
     <row r="101" spans="1:12" ht="15" customHeight="1">
       <c r="A101" s="13"/>
-      <c r="B101" s="183" t="s">
+      <c r="B101" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C101" s="213"/>
-      <c r="D101" s="213"/>
-      <c r="E101" s="213"/>
-      <c r="F101" s="213"/>
-      <c r="G101" s="213"/>
-      <c r="H101" s="213"/>
-      <c r="I101" s="213"/>
-      <c r="J101" s="213"/>
-      <c r="K101" s="213"/>
-      <c r="L101" s="214"/>
+      <c r="C101" s="246"/>
+      <c r="D101" s="246"/>
+      <c r="E101" s="246"/>
+      <c r="F101" s="246"/>
+      <c r="G101" s="246"/>
+      <c r="H101" s="246"/>
+      <c r="I101" s="246"/>
+      <c r="J101" s="246"/>
+      <c r="K101" s="246"/>
+      <c r="L101" s="247"/>
     </row>
     <row r="102" spans="1:12" ht="15" customHeight="1">
       <c r="A102" s="13"/>
-      <c r="B102" s="215"/>
-      <c r="C102" s="216"/>
-      <c r="D102" s="216"/>
-      <c r="E102" s="216"/>
-      <c r="F102" s="216"/>
-      <c r="G102" s="216"/>
-      <c r="H102" s="216"/>
-      <c r="I102" s="216"/>
-      <c r="J102" s="216"/>
-      <c r="K102" s="216"/>
-      <c r="L102" s="217"/>
+      <c r="B102" s="248"/>
+      <c r="C102" s="249"/>
+      <c r="D102" s="249"/>
+      <c r="E102" s="249"/>
+      <c r="F102" s="249"/>
+      <c r="G102" s="249"/>
+      <c r="H102" s="249"/>
+      <c r="I102" s="249"/>
+      <c r="J102" s="249"/>
+      <c r="K102" s="249"/>
+      <c r="L102" s="250"/>
     </row>
     <row r="103" spans="1:12" ht="15" customHeight="1">
       <c r="A103" s="13"/>
-      <c r="B103" s="215"/>
-      <c r="C103" s="216"/>
-      <c r="D103" s="216"/>
-      <c r="E103" s="216"/>
-      <c r="F103" s="216"/>
-      <c r="G103" s="216"/>
-      <c r="H103" s="216"/>
-      <c r="I103" s="216"/>
-      <c r="J103" s="216"/>
-      <c r="K103" s="216"/>
-      <c r="L103" s="217"/>
+      <c r="B103" s="248"/>
+      <c r="C103" s="249"/>
+      <c r="D103" s="249"/>
+      <c r="E103" s="249"/>
+      <c r="F103" s="249"/>
+      <c r="G103" s="249"/>
+      <c r="H103" s="249"/>
+      <c r="I103" s="249"/>
+      <c r="J103" s="249"/>
+      <c r="K103" s="249"/>
+      <c r="L103" s="250"/>
     </row>
     <row r="104" spans="1:12" ht="15" customHeight="1">
       <c r="A104" s="13"/>
-      <c r="B104" s="215"/>
-      <c r="C104" s="216"/>
-      <c r="D104" s="216"/>
-      <c r="E104" s="216"/>
-      <c r="F104" s="216"/>
-      <c r="G104" s="216"/>
-      <c r="H104" s="216"/>
-      <c r="I104" s="216"/>
-      <c r="J104" s="216"/>
-      <c r="K104" s="216"/>
-      <c r="L104" s="217"/>
+      <c r="B104" s="248"/>
+      <c r="C104" s="249"/>
+      <c r="D104" s="249"/>
+      <c r="E104" s="249"/>
+      <c r="F104" s="249"/>
+      <c r="G104" s="249"/>
+      <c r="H104" s="249"/>
+      <c r="I104" s="249"/>
+      <c r="J104" s="249"/>
+      <c r="K104" s="249"/>
+      <c r="L104" s="250"/>
     </row>
     <row r="105" spans="1:12" ht="15" customHeight="1">
       <c r="A105" s="13"/>
-      <c r="B105" s="215"/>
-      <c r="C105" s="216"/>
-      <c r="D105" s="216"/>
-      <c r="E105" s="216"/>
-      <c r="F105" s="216"/>
-      <c r="G105" s="216"/>
-      <c r="H105" s="216"/>
-      <c r="I105" s="216"/>
-      <c r="J105" s="216"/>
-      <c r="K105" s="216"/>
-      <c r="L105" s="217"/>
+      <c r="B105" s="248"/>
+      <c r="C105" s="249"/>
+      <c r="D105" s="249"/>
+      <c r="E105" s="249"/>
+      <c r="F105" s="249"/>
+      <c r="G105" s="249"/>
+      <c r="H105" s="249"/>
+      <c r="I105" s="249"/>
+      <c r="J105" s="249"/>
+      <c r="K105" s="249"/>
+      <c r="L105" s="250"/>
     </row>
     <row r="106" spans="1:12" ht="15" customHeight="1">
       <c r="A106" s="13"/>
-      <c r="B106" s="215"/>
-      <c r="C106" s="216"/>
-      <c r="D106" s="216"/>
-      <c r="E106" s="216"/>
-      <c r="F106" s="216"/>
-      <c r="G106" s="216"/>
-      <c r="H106" s="216"/>
-      <c r="I106" s="216"/>
-      <c r="J106" s="216"/>
-      <c r="K106" s="216"/>
-      <c r="L106" s="217"/>
+      <c r="B106" s="248"/>
+      <c r="C106" s="249"/>
+      <c r="D106" s="249"/>
+      <c r="E106" s="249"/>
+      <c r="F106" s="249"/>
+      <c r="G106" s="249"/>
+      <c r="H106" s="249"/>
+      <c r="I106" s="249"/>
+      <c r="J106" s="249"/>
+      <c r="K106" s="249"/>
+      <c r="L106" s="250"/>
     </row>
     <row r="107" spans="1:12" ht="15" customHeight="1">
       <c r="A107" s="13"/>
-      <c r="B107" s="218"/>
-      <c r="C107" s="219"/>
-      <c r="D107" s="219"/>
-      <c r="E107" s="219"/>
-      <c r="F107" s="219"/>
-      <c r="G107" s="219"/>
-      <c r="H107" s="219"/>
-      <c r="I107" s="219"/>
-      <c r="J107" s="219"/>
-      <c r="K107" s="219"/>
-      <c r="L107" s="220"/>
+      <c r="B107" s="251"/>
+      <c r="C107" s="252"/>
+      <c r="D107" s="252"/>
+      <c r="E107" s="252"/>
+      <c r="F107" s="252"/>
+      <c r="G107" s="252"/>
+      <c r="H107" s="252"/>
+      <c r="I107" s="252"/>
+      <c r="J107" s="252"/>
+      <c r="K107" s="252"/>
+      <c r="L107" s="253"/>
     </row>
     <row r="108" spans="1:12" ht="15" customHeight="1">
       <c r="A108" s="13"/>
@@ -31598,19 +31858,19 @@
       <c r="L108" s="20"/>
     </row>
     <row r="109" spans="1:12">
-      <c r="B109" s="192" t="s">
+      <c r="B109" s="183" t="s">
         <v>118</v>
       </c>
-      <c r="C109" s="193"/>
-      <c r="D109" s="193"/>
-      <c r="E109" s="193"/>
-      <c r="F109" s="193"/>
-      <c r="G109" s="193"/>
-      <c r="H109" s="193"/>
-      <c r="I109" s="193"/>
-      <c r="J109" s="193"/>
-      <c r="K109" s="193"/>
-      <c r="L109" s="193"/>
+      <c r="C109" s="184"/>
+      <c r="D109" s="184"/>
+      <c r="E109" s="184"/>
+      <c r="F109" s="184"/>
+      <c r="G109" s="184"/>
+      <c r="H109" s="184"/>
+      <c r="I109" s="184"/>
+      <c r="J109" s="184"/>
+      <c r="K109" s="184"/>
+      <c r="L109" s="184"/>
     </row>
     <row r="110" spans="1:12" ht="15" customHeight="1">
       <c r="A110" s="13"/>
@@ -31734,8 +31994,8 @@
     </row>
     <row r="118" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A118" s="13"/>
-      <c r="B118" s="221"/>
-      <c r="C118" s="222"/>
+      <c r="B118" s="254"/>
+      <c r="C118" s="255"/>
       <c r="D118" s="63"/>
       <c r="E118" s="63"/>
       <c r="F118" s="62"/>
@@ -31748,8 +32008,8 @@
     </row>
     <row r="119" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A119" s="13"/>
-      <c r="B119" s="221"/>
-      <c r="C119" s="222"/>
+      <c r="B119" s="254"/>
+      <c r="C119" s="255"/>
       <c r="D119" s="63"/>
       <c r="E119" s="63"/>
       <c r="F119" s="62"/>
@@ -34631,128 +34891,136 @@
       <c r="L262" s="27"/>
     </row>
     <row r="263" spans="1:12">
-      <c r="B263" s="192" t="s">
+      <c r="B263" s="183" t="s">
         <v>22</v>
       </c>
-      <c r="C263" s="193"/>
-      <c r="D263" s="193"/>
-      <c r="E263" s="193"/>
-      <c r="F263" s="193"/>
-      <c r="G263" s="193"/>
-      <c r="H263" s="193"/>
-      <c r="I263" s="193"/>
-      <c r="J263" s="193"/>
-      <c r="K263" s="193"/>
-      <c r="L263" s="193"/>
+      <c r="C263" s="184"/>
+      <c r="D263" s="184"/>
+      <c r="E263" s="184"/>
+      <c r="F263" s="184"/>
+      <c r="G263" s="184"/>
+      <c r="H263" s="184"/>
+      <c r="I263" s="184"/>
+      <c r="J263" s="184"/>
+      <c r="K263" s="184"/>
+      <c r="L263" s="184"/>
     </row>
     <row r="264" spans="1:12">
-      <c r="B264" s="183" t="s">
+      <c r="B264" s="218" t="s">
         <v>317</v>
       </c>
-      <c r="C264" s="184"/>
-      <c r="D264" s="184"/>
-      <c r="E264" s="184"/>
-      <c r="F264" s="184"/>
-      <c r="G264" s="184"/>
-      <c r="H264" s="184"/>
-      <c r="I264" s="184"/>
-      <c r="J264" s="184"/>
-      <c r="K264" s="184"/>
-      <c r="L264" s="185"/>
+      <c r="C264" s="219"/>
+      <c r="D264" s="219"/>
+      <c r="E264" s="219"/>
+      <c r="F264" s="219"/>
+      <c r="G264" s="219"/>
+      <c r="H264" s="219"/>
+      <c r="I264" s="219"/>
+      <c r="J264" s="219"/>
+      <c r="K264" s="219"/>
+      <c r="L264" s="220"/>
     </row>
     <row r="265" spans="1:12">
-      <c r="B265" s="186"/>
-      <c r="C265" s="187"/>
-      <c r="D265" s="187"/>
-      <c r="E265" s="187"/>
-      <c r="F265" s="187"/>
-      <c r="G265" s="187"/>
-      <c r="H265" s="187"/>
-      <c r="I265" s="187"/>
-      <c r="J265" s="187"/>
-      <c r="K265" s="187"/>
-      <c r="L265" s="188"/>
+      <c r="B265" s="221"/>
+      <c r="C265" s="222"/>
+      <c r="D265" s="222"/>
+      <c r="E265" s="222"/>
+      <c r="F265" s="222"/>
+      <c r="G265" s="222"/>
+      <c r="H265" s="222"/>
+      <c r="I265" s="222"/>
+      <c r="J265" s="222"/>
+      <c r="K265" s="222"/>
+      <c r="L265" s="223"/>
     </row>
     <row r="266" spans="1:12">
-      <c r="B266" s="186"/>
-      <c r="C266" s="187"/>
-      <c r="D266" s="187"/>
-      <c r="E266" s="187"/>
-      <c r="F266" s="187"/>
-      <c r="G266" s="187"/>
-      <c r="H266" s="187"/>
-      <c r="I266" s="187"/>
-      <c r="J266" s="187"/>
-      <c r="K266" s="187"/>
-      <c r="L266" s="188"/>
+      <c r="B266" s="221"/>
+      <c r="C266" s="222"/>
+      <c r="D266" s="222"/>
+      <c r="E266" s="222"/>
+      <c r="F266" s="222"/>
+      <c r="G266" s="222"/>
+      <c r="H266" s="222"/>
+      <c r="I266" s="222"/>
+      <c r="J266" s="222"/>
+      <c r="K266" s="222"/>
+      <c r="L266" s="223"/>
     </row>
     <row r="267" spans="1:12">
-      <c r="B267" s="186"/>
-      <c r="C267" s="187"/>
-      <c r="D267" s="187"/>
-      <c r="E267" s="187"/>
-      <c r="F267" s="187"/>
-      <c r="G267" s="187"/>
-      <c r="H267" s="187"/>
-      <c r="I267" s="187"/>
-      <c r="J267" s="187"/>
-      <c r="K267" s="187"/>
-      <c r="L267" s="188"/>
+      <c r="B267" s="221"/>
+      <c r="C267" s="222"/>
+      <c r="D267" s="222"/>
+      <c r="E267" s="222"/>
+      <c r="F267" s="222"/>
+      <c r="G267" s="222"/>
+      <c r="H267" s="222"/>
+      <c r="I267" s="222"/>
+      <c r="J267" s="222"/>
+      <c r="K267" s="222"/>
+      <c r="L267" s="223"/>
     </row>
     <row r="268" spans="1:12">
-      <c r="B268" s="186"/>
-      <c r="C268" s="187"/>
-      <c r="D268" s="187"/>
-      <c r="E268" s="187"/>
-      <c r="F268" s="187"/>
-      <c r="G268" s="187"/>
-      <c r="H268" s="187"/>
-      <c r="I268" s="187"/>
-      <c r="J268" s="187"/>
-      <c r="K268" s="187"/>
-      <c r="L268" s="188"/>
+      <c r="B268" s="221"/>
+      <c r="C268" s="222"/>
+      <c r="D268" s="222"/>
+      <c r="E268" s="222"/>
+      <c r="F268" s="222"/>
+      <c r="G268" s="222"/>
+      <c r="H268" s="222"/>
+      <c r="I268" s="222"/>
+      <c r="J268" s="222"/>
+      <c r="K268" s="222"/>
+      <c r="L268" s="223"/>
     </row>
     <row r="269" spans="1:12">
-      <c r="B269" s="186"/>
-      <c r="C269" s="187"/>
-      <c r="D269" s="187"/>
-      <c r="E269" s="187"/>
-      <c r="F269" s="187"/>
-      <c r="G269" s="187"/>
-      <c r="H269" s="187"/>
-      <c r="I269" s="187"/>
-      <c r="J269" s="187"/>
-      <c r="K269" s="187"/>
-      <c r="L269" s="188"/>
+      <c r="B269" s="221"/>
+      <c r="C269" s="222"/>
+      <c r="D269" s="222"/>
+      <c r="E269" s="222"/>
+      <c r="F269" s="222"/>
+      <c r="G269" s="222"/>
+      <c r="H269" s="222"/>
+      <c r="I269" s="222"/>
+      <c r="J269" s="222"/>
+      <c r="K269" s="222"/>
+      <c r="L269" s="223"/>
     </row>
     <row r="270" spans="1:12">
-      <c r="B270" s="186"/>
-      <c r="C270" s="187"/>
-      <c r="D270" s="187"/>
-      <c r="E270" s="187"/>
-      <c r="F270" s="187"/>
-      <c r="G270" s="187"/>
-      <c r="H270" s="187"/>
-      <c r="I270" s="187"/>
-      <c r="J270" s="187"/>
-      <c r="K270" s="187"/>
-      <c r="L270" s="188"/>
+      <c r="B270" s="221"/>
+      <c r="C270" s="222"/>
+      <c r="D270" s="222"/>
+      <c r="E270" s="222"/>
+      <c r="F270" s="222"/>
+      <c r="G270" s="222"/>
+      <c r="H270" s="222"/>
+      <c r="I270" s="222"/>
+      <c r="J270" s="222"/>
+      <c r="K270" s="222"/>
+      <c r="L270" s="223"/>
     </row>
     <row r="271" spans="1:12">
-      <c r="B271" s="189"/>
-      <c r="C271" s="190"/>
-      <c r="D271" s="190"/>
-      <c r="E271" s="190"/>
-      <c r="F271" s="190"/>
-      <c r="G271" s="190"/>
-      <c r="H271" s="190"/>
-      <c r="I271" s="190"/>
-      <c r="J271" s="190"/>
-      <c r="K271" s="190"/>
-      <c r="L271" s="191"/>
+      <c r="B271" s="224"/>
+      <c r="C271" s="225"/>
+      <c r="D271" s="225"/>
+      <c r="E271" s="225"/>
+      <c r="F271" s="225"/>
+      <c r="G271" s="225"/>
+      <c r="H271" s="225"/>
+      <c r="I271" s="225"/>
+      <c r="J271" s="225"/>
+      <c r="K271" s="225"/>
+      <c r="L271" s="226"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B16:L16"/>
+    <mergeCell ref="B17:L19"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B4:L4"/>
     <mergeCell ref="B264:L271"/>
     <mergeCell ref="B109:L109"/>
     <mergeCell ref="B7:I14"/>
@@ -34768,14 +35036,6 @@
     <mergeCell ref="K75:L75"/>
     <mergeCell ref="B263:L263"/>
     <mergeCell ref="B101:L107"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B17:L19"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B4:L4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished last problem. Bonus left
</commit_message>
<xml_diff>
--- a/AllsWellThatEndsExcel_Case_and_Answers.xlsx
+++ b/AllsWellThatEndsExcel_Case_and_Answers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77F40E7-BA14-4B41-B8CF-1AEC6B714722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224820F7-9BF3-48C6-B1ED-0E678FBEEF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{14CF381A-4175-4F53-B406-22934FD6CEB0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{14CF381A-4175-4F53-B406-22934FD6CEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="16" r:id="rId1"/>
@@ -8539,124 +8539,11 @@
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="60" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="60" fillId="7" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="15" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8758,10 +8645,123 @@
     <xf numFmtId="0" fontId="75" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="60" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="60" fillId="7" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="15" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma 2" xfId="6" xr:uid="{9E1DC8CC-A226-4805-A2F5-EBF43D6D2724}"/>
@@ -10260,9 +10260,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>59167</xdr:colOff>
+      <xdr:colOff>55357</xdr:colOff>
       <xdr:row>120</xdr:row>
-      <xdr:rowOff>135479</xdr:rowOff>
+      <xdr:rowOff>131669</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10310,7 +10310,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>56030</xdr:colOff>
+      <xdr:colOff>59840</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>393</xdr:rowOff>
     </xdr:to>
@@ -10410,9 +10410,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1540418</xdr:colOff>
+      <xdr:colOff>1544228</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>16921</xdr:rowOff>
+      <xdr:rowOff>20731</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10518,9 +10518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>282267</xdr:colOff>
+      <xdr:colOff>286077</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>19507</xdr:rowOff>
+      <xdr:rowOff>15697</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10573,7 +10573,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>17949</xdr:colOff>
+      <xdr:colOff>21759</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -10628,7 +10628,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>131445</xdr:colOff>
+      <xdr:colOff>135255</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>155165</xdr:rowOff>
     </xdr:to>
@@ -10677,9 +10677,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1584147</xdr:colOff>
+      <xdr:colOff>1580337</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>130372</xdr:rowOff>
+      <xdr:rowOff>134182</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10726,9 +10726,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>282779</xdr:colOff>
+      <xdr:colOff>286589</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>474290</xdr:rowOff>
+      <xdr:rowOff>478100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10778,7 +10778,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>419941</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>478689</xdr:rowOff>
+      <xdr:rowOff>474879</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10826,9 +10826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>853468</xdr:colOff>
+      <xdr:colOff>857278</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>210276</xdr:rowOff>
+      <xdr:rowOff>206466</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10876,9 +10876,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>54953</xdr:colOff>
+      <xdr:colOff>58763</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>399516</xdr:rowOff>
+      <xdr:rowOff>403326</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10926,9 +10926,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1808261</xdr:colOff>
+      <xdr:colOff>1812071</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>437025</xdr:rowOff>
+      <xdr:rowOff>440835</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10976,9 +10976,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1045244</xdr:colOff>
+      <xdr:colOff>1049054</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>170481</xdr:rowOff>
+      <xdr:rowOff>174291</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11026,9 +11026,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1351158</xdr:colOff>
+      <xdr:colOff>1354968</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>437006</xdr:rowOff>
+      <xdr:rowOff>440816</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11076,9 +11076,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>248522</xdr:colOff>
+      <xdr:colOff>244712</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>396478</xdr:rowOff>
+      <xdr:rowOff>400288</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11126,9 +11126,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>821151</xdr:colOff>
+      <xdr:colOff>817341</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>21878</xdr:rowOff>
+      <xdr:rowOff>18068</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11176,9 +11176,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1850291</xdr:colOff>
+      <xdr:colOff>1846481</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>17497</xdr:rowOff>
+      <xdr:rowOff>21307</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11525,9 +11525,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>783425</xdr:colOff>
+      <xdr:colOff>779615</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>136152</xdr:rowOff>
+      <xdr:rowOff>132342</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12835,7 +12835,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>285233</xdr:colOff>
+      <xdr:colOff>289043</xdr:colOff>
       <xdr:row>106</xdr:row>
       <xdr:rowOff>37685</xdr:rowOff>
     </xdr:to>
@@ -12885,9 +12885,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1165341</xdr:colOff>
+      <xdr:colOff>1161531</xdr:colOff>
       <xdr:row>106</xdr:row>
-      <xdr:rowOff>21648</xdr:rowOff>
+      <xdr:rowOff>17838</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12935,7 +12935,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>54273</xdr:colOff>
+      <xdr:colOff>58083</xdr:colOff>
       <xdr:row>106</xdr:row>
       <xdr:rowOff>115403</xdr:rowOff>
     </xdr:to>
@@ -12987,7 +12987,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>112378</xdr:colOff>
       <xdr:row>103</xdr:row>
-      <xdr:rowOff>54641</xdr:rowOff>
+      <xdr:rowOff>58451</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13035,9 +13035,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1699078</xdr:colOff>
+      <xdr:colOff>1695268</xdr:colOff>
       <xdr:row>107</xdr:row>
-      <xdr:rowOff>17309</xdr:rowOff>
+      <xdr:rowOff>21119</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13085,9 +13085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>626374</xdr:colOff>
+      <xdr:colOff>630184</xdr:colOff>
       <xdr:row>103</xdr:row>
-      <xdr:rowOff>171220</xdr:rowOff>
+      <xdr:rowOff>175030</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13135,7 +13135,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1164646</xdr:colOff>
+      <xdr:colOff>1160836</xdr:colOff>
       <xdr:row>104</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
@@ -13185,7 +13185,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>817719</xdr:colOff>
+      <xdr:colOff>821529</xdr:colOff>
       <xdr:row>105</xdr:row>
       <xdr:rowOff>38104</xdr:rowOff>
     </xdr:to>
@@ -13235,9 +13235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>283152</xdr:colOff>
+      <xdr:colOff>286962</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>169717</xdr:rowOff>
+      <xdr:rowOff>173527</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13285,9 +13285,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1772367</xdr:colOff>
+      <xdr:colOff>1768557</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>171474</xdr:rowOff>
+      <xdr:rowOff>167664</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13335,9 +13335,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>20840</xdr:colOff>
+      <xdr:colOff>17030</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>20842</xdr:rowOff>
+      <xdr:rowOff>17032</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13394,7 +13394,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1883500</xdr:colOff>
+      <xdr:colOff>1887310</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>263338</xdr:rowOff>
     </xdr:to>
@@ -14275,13 +14275,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>263</xdr:row>
+      <xdr:row>277</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>212418</xdr:colOff>
-      <xdr:row>265</xdr:row>
+      <xdr:colOff>208608</xdr:colOff>
+      <xdr:row>279</xdr:row>
       <xdr:rowOff>308229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -14325,14 +14325,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>923925</xdr:colOff>
-      <xdr:row>266</xdr:row>
+      <xdr:row>280</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1655589</xdr:colOff>
-      <xdr:row>268</xdr:row>
-      <xdr:rowOff>212433</xdr:rowOff>
+      <xdr:colOff>1659399</xdr:colOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>208623</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14375,13 +14375,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1083070</xdr:colOff>
-      <xdr:row>263</xdr:row>
+      <xdr:row>277</xdr:row>
       <xdr:rowOff>193941</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>92555</xdr:colOff>
-      <xdr:row>266</xdr:row>
+      <xdr:colOff>96365</xdr:colOff>
+      <xdr:row>280</xdr:row>
       <xdr:rowOff>112557</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -14425,14 +14425,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>263</xdr:row>
+      <xdr:row>277</xdr:row>
       <xdr:rowOff>247650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>38402</xdr:colOff>
-      <xdr:row>266</xdr:row>
-      <xdr:rowOff>15593</xdr:rowOff>
+      <xdr:row>280</xdr:row>
+      <xdr:rowOff>19403</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14475,14 +14475,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>822114</xdr:colOff>
-      <xdr:row>264</xdr:row>
+      <xdr:row>278</xdr:row>
       <xdr:rowOff>39856</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1275135</xdr:colOff>
-      <xdr:row>265</xdr:row>
-      <xdr:rowOff>173762</xdr:rowOff>
+      <xdr:colOff>1278945</xdr:colOff>
+      <xdr:row>279</xdr:row>
+      <xdr:rowOff>169952</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14525,14 +14525,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1519873</xdr:colOff>
-      <xdr:row>268</xdr:row>
+      <xdr:row>282</xdr:row>
       <xdr:rowOff>229491</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>245417</xdr:colOff>
-      <xdr:row>270</xdr:row>
-      <xdr:rowOff>130103</xdr:rowOff>
+      <xdr:colOff>249227</xdr:colOff>
+      <xdr:row>284</xdr:row>
+      <xdr:rowOff>133913</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14575,14 +14575,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>146959</xdr:colOff>
-      <xdr:row>434</xdr:row>
+      <xdr:row>448</xdr:row>
       <xdr:rowOff>89163</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>878623</xdr:colOff>
-      <xdr:row>436</xdr:row>
-      <xdr:rowOff>170150</xdr:rowOff>
+      <xdr:row>450</xdr:row>
+      <xdr:rowOff>173960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14625,14 +14625,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>276227</xdr:colOff>
-      <xdr:row>264</xdr:row>
+      <xdr:row>278</xdr:row>
       <xdr:rowOff>67416</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1006863</xdr:colOff>
-      <xdr:row>266</xdr:row>
-      <xdr:rowOff>134841</xdr:rowOff>
+      <xdr:colOff>1010673</xdr:colOff>
+      <xdr:row>280</xdr:row>
+      <xdr:rowOff>131031</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14675,14 +14675,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>843028</xdr:colOff>
-      <xdr:row>266</xdr:row>
+      <xdr:row>280</xdr:row>
       <xdr:rowOff>135949</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1772668</xdr:colOff>
-      <xdr:row>269</xdr:row>
-      <xdr:rowOff>57844</xdr:rowOff>
+      <xdr:colOff>1768858</xdr:colOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>54034</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14725,14 +14725,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>514124</xdr:colOff>
-      <xdr:row>263</xdr:row>
+      <xdr:row>277</xdr:row>
       <xdr:rowOff>15377</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1635057</xdr:colOff>
-      <xdr:row>266</xdr:row>
-      <xdr:rowOff>132549</xdr:rowOff>
+      <xdr:row>280</xdr:row>
+      <xdr:rowOff>136359</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14775,14 +14775,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1763185</xdr:colOff>
-      <xdr:row>266</xdr:row>
+      <xdr:row>280</xdr:row>
       <xdr:rowOff>254052</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>285367</xdr:colOff>
-      <xdr:row>268</xdr:row>
-      <xdr:rowOff>16542</xdr:rowOff>
+      <xdr:colOff>289177</xdr:colOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>20352</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14825,14 +14825,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>145106</xdr:colOff>
-      <xdr:row>267</xdr:row>
+      <xdr:row>281</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>97481</xdr:colOff>
-      <xdr:row>270</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>93671</xdr:colOff>
+      <xdr:row>284</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14875,14 +14875,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>558146</xdr:colOff>
-      <xdr:row>265</xdr:row>
+      <xdr:row>279</xdr:row>
       <xdr:rowOff>245918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>835236</xdr:colOff>
-      <xdr:row>268</xdr:row>
-      <xdr:rowOff>171623</xdr:rowOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>167813</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14925,14 +14925,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>166754</xdr:colOff>
-      <xdr:row>266</xdr:row>
+      <xdr:row>280</xdr:row>
       <xdr:rowOff>31173</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1088774</xdr:colOff>
-      <xdr:row>268</xdr:row>
-      <xdr:rowOff>286443</xdr:rowOff>
+      <xdr:colOff>1084964</xdr:colOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>282633</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14975,14 +14975,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1771650</xdr:colOff>
-      <xdr:row>267</xdr:row>
+      <xdr:row>281</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>270</xdr:row>
-      <xdr:rowOff>207645</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>284</xdr:row>
+      <xdr:rowOff>211455</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15025,14 +15025,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>267</xdr:row>
+      <xdr:row>281</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>270</xdr:row>
-      <xdr:rowOff>207645</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>284</xdr:row>
+      <xdr:rowOff>211455</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15075,14 +15075,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1171575</xdr:colOff>
-      <xdr:row>263</xdr:row>
+      <xdr:row>277</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>265</xdr:row>
-      <xdr:rowOff>245745</xdr:rowOff>
+      <xdr:row>279</xdr:row>
+      <xdr:rowOff>249555</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15125,14 +15125,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>267</xdr:row>
+      <xdr:row>281</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1695450</xdr:colOff>
-      <xdr:row>270</xdr:row>
-      <xdr:rowOff>243840</xdr:rowOff>
+      <xdr:colOff>1691640</xdr:colOff>
+      <xdr:row>284</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15175,14 +15175,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1114425</xdr:colOff>
-      <xdr:row>268</xdr:row>
+      <xdr:row>282</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>270</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>284</xdr:row>
+      <xdr:rowOff>243840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -18561,7 +18561,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4467"/>
+                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4471"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -18629,7 +18629,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4468"/>
+                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4472"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -19257,10 +19257,10 @@
     <tabColor rgb="FFC8B960"/>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N271"/>
+  <dimension ref="A1:N285"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B188" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E195" sqref="E195:E214"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.6640625" defaultRowHeight="25.8" outlineLevelRow="1"/>
@@ -19283,19 +19283,19 @@
       <c r="A1"/>
     </row>
     <row r="2" spans="1:12" ht="59.25" customHeight="1">
-      <c r="B2" s="223" t="s">
+      <c r="B2" s="186" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
-      <c r="L2" s="224"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" outlineLevel="1">
       <c r="A3"/>
@@ -19312,19 +19312,19 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" ht="75" customHeight="1" outlineLevel="1">
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="188" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="225"/>
-      <c r="D4" s="225"/>
-      <c r="E4" s="225"/>
-      <c r="F4" s="225"/>
-      <c r="G4" s="225"/>
-      <c r="H4" s="225"/>
-      <c r="I4" s="225"/>
-      <c r="J4" s="225"/>
-      <c r="K4" s="225"/>
-      <c r="L4" s="225"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="188"/>
+      <c r="K4" s="188"/>
+      <c r="L4" s="188"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="B5" s="2"/>
@@ -19340,112 +19340,112 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="33" customHeight="1">
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="184" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="193"/>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="193"/>
-      <c r="H6" s="193"/>
-      <c r="I6" s="226"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="185"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="189"/>
       <c r="J6"/>
-      <c r="K6" s="227" t="s">
+      <c r="K6" s="190" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="228"/>
+      <c r="L6" s="191"/>
     </row>
     <row r="7" spans="1:12" ht="25.95" customHeight="1">
-      <c r="B7" s="229" t="s">
+      <c r="B7" s="192" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="230"/>
-      <c r="D7" s="230"/>
-      <c r="E7" s="230"/>
-      <c r="F7" s="230"/>
-      <c r="G7" s="230"/>
-      <c r="H7" s="230"/>
-      <c r="I7" s="231"/>
+      <c r="C7" s="193"/>
+      <c r="D7" s="193"/>
+      <c r="E7" s="193"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="193"/>
+      <c r="I7" s="194"/>
       <c r="K7" s="5"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="232"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233"/>
-      <c r="H8" s="233"/>
-      <c r="I8" s="234"/>
+      <c r="B8" s="195"/>
+      <c r="C8" s="196"/>
+      <c r="D8" s="196"/>
+      <c r="E8" s="196"/>
+      <c r="F8" s="196"/>
+      <c r="G8" s="196"/>
+      <c r="H8" s="196"/>
+      <c r="I8" s="197"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="232"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
-      <c r="G9" s="233"/>
-      <c r="H9" s="233"/>
-      <c r="I9" s="234"/>
+      <c r="B9" s="195"/>
+      <c r="C9" s="196"/>
+      <c r="D9" s="196"/>
+      <c r="E9" s="196"/>
+      <c r="F9" s="196"/>
+      <c r="G9" s="196"/>
+      <c r="H9" s="196"/>
+      <c r="I9" s="197"/>
       <c r="J9"/>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="B10" s="232"/>
-      <c r="C10" s="233"/>
-      <c r="D10" s="233"/>
-      <c r="E10" s="233"/>
-      <c r="F10" s="233"/>
-      <c r="G10" s="233"/>
-      <c r="H10" s="233"/>
-      <c r="I10" s="234"/>
+      <c r="B10" s="195"/>
+      <c r="C10" s="196"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="196"/>
+      <c r="H10" s="196"/>
+      <c r="I10" s="197"/>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="B11" s="232"/>
-      <c r="C11" s="233"/>
-      <c r="D11" s="233"/>
-      <c r="E11" s="233"/>
-      <c r="F11" s="233"/>
-      <c r="G11" s="233"/>
-      <c r="H11" s="233"/>
-      <c r="I11" s="234"/>
+      <c r="B11" s="195"/>
+      <c r="C11" s="196"/>
+      <c r="D11" s="196"/>
+      <c r="E11" s="196"/>
+      <c r="F11" s="196"/>
+      <c r="G11" s="196"/>
+      <c r="H11" s="196"/>
+      <c r="I11" s="197"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="B12" s="232"/>
-      <c r="C12" s="233"/>
-      <c r="D12" s="233"/>
-      <c r="E12" s="233"/>
-      <c r="F12" s="233"/>
-      <c r="G12" s="233"/>
-      <c r="H12" s="233"/>
-      <c r="I12" s="234"/>
+      <c r="B12" s="195"/>
+      <c r="C12" s="196"/>
+      <c r="D12" s="196"/>
+      <c r="E12" s="196"/>
+      <c r="F12" s="196"/>
+      <c r="G12" s="196"/>
+      <c r="H12" s="196"/>
+      <c r="I12" s="197"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:12" ht="23.25" customHeight="1">
-      <c r="B13" s="232"/>
-      <c r="C13" s="233"/>
-      <c r="D13" s="233"/>
-      <c r="E13" s="233"/>
-      <c r="F13" s="233"/>
-      <c r="G13" s="233"/>
-      <c r="H13" s="233"/>
-      <c r="I13" s="234"/>
+      <c r="B13" s="195"/>
+      <c r="C13" s="196"/>
+      <c r="D13" s="196"/>
+      <c r="E13" s="196"/>
+      <c r="F13" s="196"/>
+      <c r="G13" s="196"/>
+      <c r="H13" s="196"/>
+      <c r="I13" s="197"/>
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:12" ht="33" customHeight="1">
-      <c r="B14" s="235"/>
-      <c r="C14" s="236"/>
-      <c r="D14" s="236"/>
-      <c r="E14" s="236"/>
-      <c r="F14" s="236"/>
-      <c r="G14" s="236"/>
-      <c r="H14" s="236"/>
-      <c r="I14" s="237"/>
+      <c r="B14" s="198"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="199"/>
+      <c r="F14" s="199"/>
+      <c r="G14" s="199"/>
+      <c r="H14" s="199"/>
+      <c r="I14" s="200"/>
       <c r="K14" s="34" t="s">
         <v>0</v>
       </c>
@@ -19459,60 +19459,60 @@
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B16" s="192" t="s">
+      <c r="B16" s="184" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="193"/>
-      <c r="D16" s="193"/>
-      <c r="E16" s="193"/>
-      <c r="F16" s="193"/>
-      <c r="G16" s="193"/>
-      <c r="H16" s="193"/>
-      <c r="I16" s="193"/>
-      <c r="J16" s="193"/>
-      <c r="K16" s="193"/>
-      <c r="L16" s="193"/>
+      <c r="C16" s="185"/>
+      <c r="D16" s="185"/>
+      <c r="E16" s="185"/>
+      <c r="F16" s="185"/>
+      <c r="G16" s="185"/>
+      <c r="H16" s="185"/>
+      <c r="I16" s="185"/>
+      <c r="J16" s="185"/>
+      <c r="K16" s="185"/>
+      <c r="L16" s="185"/>
     </row>
     <row r="17" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B17" s="238" t="s">
+      <c r="B17" s="201" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="239"/>
-      <c r="D17" s="239"/>
-      <c r="E17" s="239"/>
-      <c r="F17" s="239"/>
-      <c r="G17" s="239"/>
-      <c r="H17" s="239"/>
-      <c r="I17" s="239"/>
-      <c r="J17" s="239"/>
-      <c r="K17" s="239"/>
-      <c r="L17" s="240"/>
+      <c r="C17" s="202"/>
+      <c r="D17" s="202"/>
+      <c r="E17" s="202"/>
+      <c r="F17" s="202"/>
+      <c r="G17" s="202"/>
+      <c r="H17" s="202"/>
+      <c r="I17" s="202"/>
+      <c r="J17" s="202"/>
+      <c r="K17" s="202"/>
+      <c r="L17" s="203"/>
     </row>
     <row r="18" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B18" s="241"/>
-      <c r="C18" s="242"/>
-      <c r="D18" s="242"/>
-      <c r="E18" s="242"/>
-      <c r="F18" s="242"/>
-      <c r="G18" s="242"/>
-      <c r="H18" s="242"/>
-      <c r="I18" s="242"/>
-      <c r="J18" s="242"/>
-      <c r="K18" s="242"/>
-      <c r="L18" s="243"/>
+      <c r="B18" s="204"/>
+      <c r="C18" s="205"/>
+      <c r="D18" s="205"/>
+      <c r="E18" s="205"/>
+      <c r="F18" s="205"/>
+      <c r="G18" s="205"/>
+      <c r="H18" s="205"/>
+      <c r="I18" s="205"/>
+      <c r="J18" s="205"/>
+      <c r="K18" s="205"/>
+      <c r="L18" s="206"/>
     </row>
     <row r="19" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B19" s="244"/>
-      <c r="C19" s="245"/>
-      <c r="D19" s="245"/>
-      <c r="E19" s="245"/>
-      <c r="F19" s="245"/>
-      <c r="G19" s="245"/>
-      <c r="H19" s="245"/>
-      <c r="I19" s="245"/>
-      <c r="J19" s="245"/>
-      <c r="K19" s="245"/>
-      <c r="L19" s="246"/>
+      <c r="B19" s="207"/>
+      <c r="C19" s="208"/>
+      <c r="D19" s="208"/>
+      <c r="E19" s="208"/>
+      <c r="F19" s="208"/>
+      <c r="G19" s="208"/>
+      <c r="H19" s="208"/>
+      <c r="I19" s="208"/>
+      <c r="J19" s="208"/>
+      <c r="K19" s="208"/>
+      <c r="L19" s="209"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="B20" s="8"/>
@@ -19528,19 +19528,19 @@
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B21" s="192" t="s">
+      <c r="B21" s="184" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="193"/>
-      <c r="D21" s="193"/>
-      <c r="E21" s="193"/>
-      <c r="F21" s="193"/>
-      <c r="G21" s="193"/>
-      <c r="H21" s="193"/>
-      <c r="I21" s="193"/>
-      <c r="J21" s="193"/>
-      <c r="K21" s="193"/>
-      <c r="L21" s="193"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="185"/>
+      <c r="E21" s="185"/>
+      <c r="F21" s="185"/>
+      <c r="G21" s="185"/>
+      <c r="H21" s="185"/>
+      <c r="I21" s="185"/>
+      <c r="J21" s="185"/>
+      <c r="K21" s="185"/>
+      <c r="L21" s="185"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="B22" s="9"/>
@@ -19622,14 +19622,14 @@
         <f>IF(ISBLANK(E26),0,IF(E26=Answers!E26,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G26" s="247" t="s">
+      <c r="G26" s="210" t="s">
         <v>187</v>
       </c>
-      <c r="H26" s="248"/>
-      <c r="I26" s="248"/>
-      <c r="J26" s="248"/>
-      <c r="K26" s="248"/>
-      <c r="L26" s="249"/>
+      <c r="H26" s="211"/>
+      <c r="I26" s="211"/>
+      <c r="J26" s="211"/>
+      <c r="K26" s="211"/>
+      <c r="L26" s="212"/>
     </row>
     <row r="27" spans="1:12" ht="33.75" customHeight="1">
       <c r="B27" s="36" t="s">
@@ -19646,14 +19646,14 @@
         <f>IF(ISBLANK(E27),0,IF(E27=Answers!E27,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G27" s="250" t="s">
+      <c r="G27" s="213" t="s">
         <v>186</v>
       </c>
-      <c r="H27" s="251"/>
-      <c r="I27" s="251"/>
-      <c r="J27" s="251"/>
-      <c r="K27" s="251"/>
-      <c r="L27" s="252"/>
+      <c r="H27" s="214"/>
+      <c r="I27" s="214"/>
+      <c r="J27" s="214"/>
+      <c r="K27" s="214"/>
+      <c r="L27" s="215"/>
     </row>
     <row r="28" spans="1:12" ht="54" customHeight="1">
       <c r="B28" s="36" t="s">
@@ -19670,14 +19670,14 @@
         <f>IF(ISBLANK(E28),0,IF(E28=Answers!E28,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="253" t="s">
+      <c r="G28" s="216" t="s">
         <v>345</v>
       </c>
-      <c r="H28" s="254"/>
-      <c r="I28" s="254"/>
-      <c r="J28" s="254"/>
-      <c r="K28" s="254"/>
-      <c r="L28" s="255"/>
+      <c r="H28" s="217"/>
+      <c r="I28" s="217"/>
+      <c r="J28" s="217"/>
+      <c r="K28" s="217"/>
+      <c r="L28" s="218"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="B29" s="2"/>
@@ -19693,19 +19693,19 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="B30" s="192" t="s">
+      <c r="B30" s="184" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="193"/>
-      <c r="D30" s="193"/>
-      <c r="E30" s="193"/>
-      <c r="F30" s="193"/>
-      <c r="G30" s="193"/>
-      <c r="H30" s="193"/>
-      <c r="I30" s="193"/>
-      <c r="J30" s="193"/>
-      <c r="K30" s="193"/>
-      <c r="L30" s="193"/>
+      <c r="C30" s="185"/>
+      <c r="D30" s="185"/>
+      <c r="E30" s="185"/>
+      <c r="F30" s="185"/>
+      <c r="G30" s="185"/>
+      <c r="H30" s="185"/>
+      <c r="I30" s="185"/>
+      <c r="J30" s="185"/>
+      <c r="K30" s="185"/>
+      <c r="L30" s="185"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="B31" s="16"/>
@@ -19735,10 +19735,10 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
-      <c r="K32" s="192" t="s">
+      <c r="K32" s="184" t="s">
         <v>15</v>
       </c>
-      <c r="L32" s="193"/>
+      <c r="L32" s="185"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1">
       <c r="A33" s="13"/>
@@ -19751,11 +19751,11 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
-      <c r="K33" s="194" cm="1">
-        <f t="array" ref="K33">SUMPRODUCT(--($F$26:$F$262=1),$D$26:$D$262)</f>
-        <v>460</v>
-      </c>
-      <c r="L33" s="195"/>
+      <c r="K33" s="228" cm="1">
+        <f t="array" ref="K33">SUMPRODUCT(--($F$26:$F$276=1),$D$26:$D$276)</f>
+        <v>640</v>
+      </c>
+      <c r="L33" s="229"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1">
       <c r="A34"/>
@@ -19770,8 +19770,8 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
-      <c r="K34" s="196"/>
-      <c r="L34" s="197"/>
+      <c r="K34" s="230"/>
+      <c r="L34" s="231"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1">
       <c r="A35" s="13"/>
@@ -19786,8 +19786,8 @@
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
-      <c r="K35" s="196"/>
-      <c r="L35" s="197"/>
+      <c r="K35" s="230"/>
+      <c r="L35" s="231"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1">
       <c r="A36" s="13"/>
@@ -19800,8 +19800,8 @@
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
-      <c r="K36" s="198"/>
-      <c r="L36" s="199"/>
+      <c r="K36" s="232"/>
+      <c r="L36" s="233"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1">
       <c r="A37" s="13"/>
@@ -19940,10 +19940,10 @@
         <v>122</v>
       </c>
       <c r="F45" s="18"/>
-      <c r="G45" s="200" t="s">
+      <c r="G45" s="234" t="s">
         <v>324</v>
       </c>
-      <c r="H45" s="201"/>
+      <c r="H45" s="235"/>
       <c r="I45" s="91" t="s">
         <v>52</v>
       </c>
@@ -20402,14 +20402,14 @@
       <c r="F63" s="18"/>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
-      <c r="I63" s="202" t="s">
+      <c r="I63" s="236" t="s">
         <v>138</v>
       </c>
-      <c r="J63" s="203"/>
-      <c r="K63" s="206" t="s">
+      <c r="J63" s="237"/>
+      <c r="K63" s="240" t="s">
         <v>141</v>
       </c>
-      <c r="L63" s="207"/>
+      <c r="L63" s="241"/>
     </row>
     <row r="64" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A64" s="13"/>
@@ -20422,10 +20422,10 @@
       <c r="F64" s="18"/>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
-      <c r="I64" s="204"/>
-      <c r="J64" s="205"/>
-      <c r="K64" s="208"/>
-      <c r="L64" s="209"/>
+      <c r="I64" s="238"/>
+      <c r="J64" s="239"/>
+      <c r="K64" s="242"/>
+      <c r="L64" s="243"/>
     </row>
     <row r="65" spans="1:14" ht="15" customHeight="1">
       <c r="A65" s="13"/>
@@ -20629,12 +20629,12 @@
       </c>
       <c r="F75" s="18"/>
       <c r="G75" s="13"/>
-      <c r="H75" s="210" t="s">
+      <c r="H75" s="244" t="s">
         <v>136</v>
       </c>
-      <c r="I75" s="211"/>
-      <c r="J75" s="211"/>
-      <c r="K75" s="212"/>
+      <c r="I75" s="245"/>
+      <c r="J75" s="245"/>
+      <c r="K75" s="246"/>
       <c r="L75" s="176" t="s">
         <v>135</v>
       </c>
@@ -21356,119 +21356,119 @@
       <c r="L99" s="20"/>
     </row>
     <row r="100" spans="1:13">
-      <c r="B100" s="192" t="s">
+      <c r="B100" s="184" t="s">
         <v>21</v>
       </c>
-      <c r="C100" s="193"/>
-      <c r="D100" s="193"/>
-      <c r="E100" s="193"/>
-      <c r="F100" s="193"/>
-      <c r="G100" s="193"/>
-      <c r="H100" s="193"/>
-      <c r="I100" s="193"/>
-      <c r="J100" s="193"/>
-      <c r="K100" s="193"/>
-      <c r="L100" s="193"/>
+      <c r="C100" s="185"/>
+      <c r="D100" s="185"/>
+      <c r="E100" s="185"/>
+      <c r="F100" s="185"/>
+      <c r="G100" s="185"/>
+      <c r="H100" s="185"/>
+      <c r="I100" s="185"/>
+      <c r="J100" s="185"/>
+      <c r="K100" s="185"/>
+      <c r="L100" s="185"/>
     </row>
     <row r="101" spans="1:13" ht="15" customHeight="1">
       <c r="A101" s="13"/>
-      <c r="B101" s="183" t="s">
+      <c r="B101" s="219" t="s">
         <v>198</v>
       </c>
-      <c r="C101" s="213"/>
-      <c r="D101" s="213"/>
-      <c r="E101" s="213"/>
-      <c r="F101" s="213"/>
-      <c r="G101" s="213"/>
-      <c r="H101" s="213"/>
-      <c r="I101" s="213"/>
-      <c r="J101" s="213"/>
-      <c r="K101" s="213"/>
-      <c r="L101" s="214"/>
+      <c r="C101" s="247"/>
+      <c r="D101" s="247"/>
+      <c r="E101" s="247"/>
+      <c r="F101" s="247"/>
+      <c r="G101" s="247"/>
+      <c r="H101" s="247"/>
+      <c r="I101" s="247"/>
+      <c r="J101" s="247"/>
+      <c r="K101" s="247"/>
+      <c r="L101" s="248"/>
     </row>
     <row r="102" spans="1:13" ht="15" customHeight="1">
       <c r="A102" s="13"/>
-      <c r="B102" s="215"/>
-      <c r="C102" s="216"/>
-      <c r="D102" s="216"/>
-      <c r="E102" s="216"/>
-      <c r="F102" s="216"/>
-      <c r="G102" s="216"/>
-      <c r="H102" s="216"/>
-      <c r="I102" s="216"/>
-      <c r="J102" s="216"/>
-      <c r="K102" s="216"/>
-      <c r="L102" s="217"/>
+      <c r="B102" s="249"/>
+      <c r="C102" s="250"/>
+      <c r="D102" s="250"/>
+      <c r="E102" s="250"/>
+      <c r="F102" s="250"/>
+      <c r="G102" s="250"/>
+      <c r="H102" s="250"/>
+      <c r="I102" s="250"/>
+      <c r="J102" s="250"/>
+      <c r="K102" s="250"/>
+      <c r="L102" s="251"/>
     </row>
     <row r="103" spans="1:13" ht="15" customHeight="1">
       <c r="A103" s="13"/>
-      <c r="B103" s="215"/>
-      <c r="C103" s="216"/>
-      <c r="D103" s="216"/>
-      <c r="E103" s="216"/>
-      <c r="F103" s="216"/>
-      <c r="G103" s="216"/>
-      <c r="H103" s="216"/>
-      <c r="I103" s="216"/>
-      <c r="J103" s="216"/>
-      <c r="K103" s="216"/>
-      <c r="L103" s="217"/>
+      <c r="B103" s="249"/>
+      <c r="C103" s="250"/>
+      <c r="D103" s="250"/>
+      <c r="E103" s="250"/>
+      <c r="F103" s="250"/>
+      <c r="G103" s="250"/>
+      <c r="H103" s="250"/>
+      <c r="I103" s="250"/>
+      <c r="J103" s="250"/>
+      <c r="K103" s="250"/>
+      <c r="L103" s="251"/>
     </row>
     <row r="104" spans="1:13" ht="15" customHeight="1">
       <c r="A104" s="13"/>
-      <c r="B104" s="215"/>
-      <c r="C104" s="216"/>
-      <c r="D104" s="216"/>
-      <c r="E104" s="216"/>
-      <c r="F104" s="216"/>
-      <c r="G104" s="216"/>
-      <c r="H104" s="216"/>
-      <c r="I104" s="216"/>
-      <c r="J104" s="216"/>
-      <c r="K104" s="216"/>
-      <c r="L104" s="217"/>
+      <c r="B104" s="249"/>
+      <c r="C104" s="250"/>
+      <c r="D104" s="250"/>
+      <c r="E104" s="250"/>
+      <c r="F104" s="250"/>
+      <c r="G104" s="250"/>
+      <c r="H104" s="250"/>
+      <c r="I104" s="250"/>
+      <c r="J104" s="250"/>
+      <c r="K104" s="250"/>
+      <c r="L104" s="251"/>
     </row>
     <row r="105" spans="1:13" ht="15" customHeight="1">
       <c r="A105" s="13"/>
-      <c r="B105" s="215"/>
-      <c r="C105" s="216"/>
-      <c r="D105" s="216"/>
-      <c r="E105" s="216"/>
-      <c r="F105" s="216"/>
-      <c r="G105" s="216"/>
-      <c r="H105" s="216"/>
-      <c r="I105" s="216"/>
-      <c r="J105" s="216"/>
-      <c r="K105" s="216"/>
-      <c r="L105" s="217"/>
+      <c r="B105" s="249"/>
+      <c r="C105" s="250"/>
+      <c r="D105" s="250"/>
+      <c r="E105" s="250"/>
+      <c r="F105" s="250"/>
+      <c r="G105" s="250"/>
+      <c r="H105" s="250"/>
+      <c r="I105" s="250"/>
+      <c r="J105" s="250"/>
+      <c r="K105" s="250"/>
+      <c r="L105" s="251"/>
     </row>
     <row r="106" spans="1:13" ht="15" customHeight="1">
       <c r="A106" s="13"/>
-      <c r="B106" s="215"/>
-      <c r="C106" s="216"/>
-      <c r="D106" s="216"/>
-      <c r="E106" s="216"/>
-      <c r="F106" s="216"/>
-      <c r="G106" s="216"/>
-      <c r="H106" s="216"/>
-      <c r="I106" s="216"/>
-      <c r="J106" s="216"/>
-      <c r="K106" s="216"/>
-      <c r="L106" s="217"/>
+      <c r="B106" s="249"/>
+      <c r="C106" s="250"/>
+      <c r="D106" s="250"/>
+      <c r="E106" s="250"/>
+      <c r="F106" s="250"/>
+      <c r="G106" s="250"/>
+      <c r="H106" s="250"/>
+      <c r="I106" s="250"/>
+      <c r="J106" s="250"/>
+      <c r="K106" s="250"/>
+      <c r="L106" s="251"/>
     </row>
     <row r="107" spans="1:13" ht="15" customHeight="1">
       <c r="A107" s="13"/>
-      <c r="B107" s="218"/>
-      <c r="C107" s="219"/>
-      <c r="D107" s="219"/>
-      <c r="E107" s="219"/>
-      <c r="F107" s="219"/>
-      <c r="G107" s="219"/>
-      <c r="H107" s="219"/>
-      <c r="I107" s="219"/>
-      <c r="J107" s="219"/>
-      <c r="K107" s="219"/>
-      <c r="L107" s="220"/>
+      <c r="B107" s="252"/>
+      <c r="C107" s="253"/>
+      <c r="D107" s="253"/>
+      <c r="E107" s="253"/>
+      <c r="F107" s="253"/>
+      <c r="G107" s="253"/>
+      <c r="H107" s="253"/>
+      <c r="I107" s="253"/>
+      <c r="J107" s="253"/>
+      <c r="K107" s="253"/>
+      <c r="L107" s="254"/>
     </row>
     <row r="108" spans="1:13" ht="15" customHeight="1">
       <c r="A108" s="13"/>
@@ -21485,19 +21485,19 @@
       <c r="L108" s="20"/>
     </row>
     <row r="109" spans="1:13">
-      <c r="B109" s="192" t="s">
+      <c r="B109" s="184" t="s">
         <v>118</v>
       </c>
-      <c r="C109" s="193"/>
-      <c r="D109" s="193"/>
-      <c r="E109" s="193"/>
-      <c r="F109" s="193"/>
-      <c r="G109" s="193"/>
-      <c r="H109" s="193"/>
-      <c r="I109" s="193"/>
-      <c r="J109" s="193"/>
-      <c r="K109" s="193"/>
-      <c r="L109" s="193"/>
+      <c r="C109" s="185"/>
+      <c r="D109" s="185"/>
+      <c r="E109" s="185"/>
+      <c r="F109" s="185"/>
+      <c r="G109" s="185"/>
+      <c r="H109" s="185"/>
+      <c r="I109" s="185"/>
+      <c r="J109" s="185"/>
+      <c r="K109" s="185"/>
+      <c r="L109" s="185"/>
     </row>
     <row r="110" spans="1:13" ht="15" customHeight="1">
       <c r="A110" s="13"/>
@@ -21621,8 +21621,8 @@
     </row>
     <row r="118" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A118" s="13"/>
-      <c r="B118" s="221"/>
-      <c r="C118" s="222"/>
+      <c r="B118" s="255"/>
+      <c r="C118" s="256"/>
       <c r="D118" s="63"/>
       <c r="E118" s="63"/>
       <c r="F118" s="62"/>
@@ -21635,8 +21635,8 @@
     </row>
     <row r="119" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A119" s="13"/>
-      <c r="B119" s="221"/>
-      <c r="C119" s="222"/>
+      <c r="B119" s="255"/>
+      <c r="C119" s="256"/>
       <c r="D119" s="63"/>
       <c r="E119" s="63"/>
       <c r="F119" s="62"/>
@@ -24312,8 +24312,6 @@
       <c r="F238" s="18"/>
       <c r="G238" s="20"/>
       <c r="H238" s="27"/>
-      <c r="I238" s="27"/>
-      <c r="J238" s="20"/>
       <c r="K238" s="27"/>
       <c r="L238" s="27"/>
     </row>
@@ -24338,8 +24336,14 @@
       <c r="G239" s="159" t="s">
         <v>288</v>
       </c>
-      <c r="H239" s="27"/>
-      <c r="I239" s="27"/>
+      <c r="H239" s="27" t="str">
+        <f>G239</f>
+        <v>L24</v>
+      </c>
+      <c r="I239" s="27" cm="1">
+        <f t="array" aca="1" ref="I239" ca="1">SUM(_xlfn.XLOOKUP(_xlfn.TOCOL(OFFSET(INDIRECT("'Birnam Forest'!"&amp;H239),-2,-2,5,5)),'Birnam Forest'!$AK$7:$AK$13,'Birnam Forest'!AM7:$AM$13,0))</f>
+        <v>20</v>
+      </c>
       <c r="J239" s="20"/>
       <c r="K239" s="27"/>
       <c r="L239" s="27"/>
@@ -24351,8 +24355,10 @@
       <c r="D240" s="20"/>
       <c r="E240" s="32"/>
       <c r="F240" s="18"/>
-      <c r="G240" s="26"/>
-      <c r="H240" s="27"/>
+      <c r="H240" s="26">
+        <f ca="1">I239</f>
+        <v>20</v>
+      </c>
       <c r="I240" s="27"/>
       <c r="J240" s="29"/>
       <c r="K240" s="27"/>
@@ -24369,15 +24375,20 @@
       <c r="D241" s="37">
         <v>9</v>
       </c>
-      <c r="E241" s="158"/>
+      <c r="E241" s="158">
+        <v>4</v>
+      </c>
       <c r="F241" s="33">
         <f>IF(ISBLANK(E241),0,IF(E241=Answers!E241,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G241" s="159" t="s">
         <v>289</v>
       </c>
-      <c r="H241" s="27"/>
+      <c r="H241" s="27">
+        <f t="dataTable" ref="H241:H260" dt2D="0" dtr="0" r1="H239" ca="1"/>
+        <v>4</v>
+      </c>
       <c r="I241" s="27"/>
       <c r="J241" s="20"/>
       <c r="K241" s="27"/>
@@ -24394,15 +24405,19 @@
       <c r="D242" s="37">
         <v>9</v>
       </c>
-      <c r="E242" s="158"/>
+      <c r="E242" s="158">
+        <v>22</v>
+      </c>
       <c r="F242" s="33">
         <f>IF(ISBLANK(E242),0,IF(E242=Answers!E242,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G242" s="159" t="s">
         <v>290</v>
       </c>
-      <c r="H242" s="27"/>
+      <c r="H242" s="27">
+        <v>22</v>
+      </c>
       <c r="I242" s="27"/>
       <c r="J242" s="20"/>
       <c r="K242" s="27"/>
@@ -24419,15 +24434,19 @@
       <c r="D243" s="37">
         <v>9</v>
       </c>
-      <c r="E243" s="158"/>
+      <c r="E243" s="158">
+        <v>20</v>
+      </c>
       <c r="F243" s="33">
         <f>IF(ISBLANK(E243),0,IF(E243=Answers!E243,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G243" s="159" t="s">
         <v>291</v>
       </c>
-      <c r="H243" s="27"/>
+      <c r="H243" s="27">
+        <v>20</v>
+      </c>
       <c r="I243" s="27"/>
       <c r="J243" s="20"/>
       <c r="K243" s="27"/>
@@ -24444,15 +24463,19 @@
       <c r="D244" s="37">
         <v>9</v>
       </c>
-      <c r="E244" s="158"/>
+      <c r="E244" s="158">
+        <v>0</v>
+      </c>
       <c r="F244" s="33">
         <f>IF(ISBLANK(E244),0,IF(E244=Answers!E244,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G244" s="159" t="s">
         <v>292</v>
       </c>
-      <c r="H244" s="27"/>
+      <c r="H244" s="27">
+        <v>0</v>
+      </c>
       <c r="I244" s="27"/>
       <c r="J244" s="20"/>
       <c r="K244" s="27"/>
@@ -24469,15 +24492,19 @@
       <c r="D245" s="37">
         <v>9</v>
       </c>
-      <c r="E245" s="158"/>
+      <c r="E245" s="158">
+        <v>15</v>
+      </c>
       <c r="F245" s="33">
         <f>IF(ISBLANK(E245),0,IF(E245=Answers!E245,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G245" s="159" t="s">
         <v>293</v>
       </c>
-      <c r="H245" s="27"/>
+      <c r="H245" s="27">
+        <v>15</v>
+      </c>
       <c r="I245" s="27"/>
       <c r="J245" s="20"/>
       <c r="K245" s="27"/>
@@ -24494,15 +24521,19 @@
       <c r="D246" s="37">
         <v>9</v>
       </c>
-      <c r="E246" s="158"/>
+      <c r="E246" s="158">
+        <v>19</v>
+      </c>
       <c r="F246" s="33">
         <f>IF(ISBLANK(E246),0,IF(E246=Answers!E246,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G246" s="159" t="s">
         <v>294</v>
       </c>
-      <c r="H246" s="27"/>
+      <c r="H246" s="27">
+        <v>19</v>
+      </c>
       <c r="I246" s="27"/>
       <c r="J246" s="20"/>
       <c r="K246" s="27"/>
@@ -24519,15 +24550,19 @@
       <c r="D247" s="37">
         <v>9</v>
       </c>
-      <c r="E247" s="158"/>
+      <c r="E247" s="158">
+        <v>14</v>
+      </c>
       <c r="F247" s="33">
         <f>IF(ISBLANK(E247),0,IF(E247=Answers!E247,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G247" s="159" t="s">
         <v>295</v>
       </c>
-      <c r="H247" s="27"/>
+      <c r="H247" s="27">
+        <v>14</v>
+      </c>
       <c r="I247" s="27"/>
       <c r="J247" s="20"/>
       <c r="K247" s="27"/>
@@ -24544,15 +24579,19 @@
       <c r="D248" s="37">
         <v>9</v>
       </c>
-      <c r="E248" s="158"/>
+      <c r="E248" s="158">
+        <v>16</v>
+      </c>
       <c r="F248" s="33">
         <f>IF(ISBLANK(E248),0,IF(E248=Answers!E248,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G248" s="159" t="s">
         <v>296</v>
       </c>
-      <c r="H248" s="27"/>
+      <c r="H248" s="27">
+        <v>16</v>
+      </c>
       <c r="I248" s="27"/>
       <c r="J248" s="20"/>
       <c r="K248" s="27"/>
@@ -24569,15 +24608,19 @@
       <c r="D249" s="37">
         <v>9</v>
       </c>
-      <c r="E249" s="158"/>
+      <c r="E249" s="158">
+        <v>7</v>
+      </c>
       <c r="F249" s="33">
         <f>IF(ISBLANK(E249),0,IF(E249=Answers!E249,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G249" s="159" t="s">
         <v>297</v>
       </c>
-      <c r="H249" s="27"/>
+      <c r="H249" s="27">
+        <v>7</v>
+      </c>
       <c r="I249" s="27"/>
       <c r="J249" s="20"/>
       <c r="K249" s="27"/>
@@ -24594,15 +24637,19 @@
       <c r="D250" s="37">
         <v>9</v>
       </c>
-      <c r="E250" s="158"/>
+      <c r="E250" s="158">
+        <v>22</v>
+      </c>
       <c r="F250" s="33">
         <f>IF(ISBLANK(E250),0,IF(E250=Answers!E250,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G250" s="159" t="s">
         <v>298</v>
       </c>
-      <c r="H250" s="27"/>
+      <c r="H250" s="27">
+        <v>22</v>
+      </c>
       <c r="I250" s="27"/>
       <c r="J250" s="20"/>
       <c r="K250" s="27"/>
@@ -24619,15 +24666,19 @@
       <c r="D251" s="37">
         <v>9</v>
       </c>
-      <c r="E251" s="158"/>
+      <c r="E251" s="158">
+        <v>8</v>
+      </c>
       <c r="F251" s="33">
         <f>IF(ISBLANK(E251),0,IF(E251=Answers!E251,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G251" s="159" t="s">
         <v>299</v>
       </c>
-      <c r="H251" s="27"/>
+      <c r="H251" s="27">
+        <v>8</v>
+      </c>
       <c r="I251" s="27"/>
       <c r="J251" s="20"/>
       <c r="K251" s="27"/>
@@ -24644,15 +24695,19 @@
       <c r="D252" s="37">
         <v>9</v>
       </c>
-      <c r="E252" s="158"/>
+      <c r="E252" s="158">
+        <v>4</v>
+      </c>
       <c r="F252" s="33">
         <f>IF(ISBLANK(E252),0,IF(E252=Answers!E252,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G252" s="159" t="s">
         <v>300</v>
       </c>
-      <c r="H252" s="27"/>
+      <c r="H252" s="27">
+        <v>4</v>
+      </c>
       <c r="I252" s="27"/>
       <c r="J252" s="20"/>
       <c r="K252" s="27"/>
@@ -24669,15 +24724,19 @@
       <c r="D253" s="37">
         <v>9</v>
       </c>
-      <c r="E253" s="158"/>
+      <c r="E253" s="158">
+        <v>16</v>
+      </c>
       <c r="F253" s="33">
         <f>IF(ISBLANK(E253),0,IF(E253=Answers!E253,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G253" s="159" t="s">
         <v>301</v>
       </c>
-      <c r="H253" s="27"/>
+      <c r="H253" s="27">
+        <v>16</v>
+      </c>
       <c r="I253" s="27"/>
       <c r="J253" s="20"/>
       <c r="K253" s="27"/>
@@ -24694,15 +24753,19 @@
       <c r="D254" s="37">
         <v>9</v>
       </c>
-      <c r="E254" s="158"/>
+      <c r="E254" s="158">
+        <v>0</v>
+      </c>
       <c r="F254" s="33">
         <f>IF(ISBLANK(E254),0,IF(E254=Answers!E254,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G254" s="159" t="s">
         <v>302</v>
       </c>
-      <c r="H254" s="27"/>
+      <c r="H254" s="27">
+        <v>0</v>
+      </c>
       <c r="I254" s="27"/>
       <c r="J254" s="20"/>
       <c r="K254" s="27"/>
@@ -24719,15 +24782,19 @@
       <c r="D255" s="37">
         <v>9</v>
       </c>
-      <c r="E255" s="158"/>
+      <c r="E255" s="158">
+        <v>16</v>
+      </c>
       <c r="F255" s="33">
         <f>IF(ISBLANK(E255),0,IF(E255=Answers!E255,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G255" s="159" t="s">
         <v>303</v>
       </c>
-      <c r="H255" s="27"/>
+      <c r="H255" s="27">
+        <v>16</v>
+      </c>
       <c r="I255" s="27"/>
       <c r="J255" s="20"/>
       <c r="K255" s="27"/>
@@ -24744,15 +24811,19 @@
       <c r="D256" s="37">
         <v>9</v>
       </c>
-      <c r="E256" s="158"/>
+      <c r="E256" s="158">
+        <v>26</v>
+      </c>
       <c r="F256" s="33">
         <f>IF(ISBLANK(E256),0,IF(E256=Answers!E256,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G256" s="159" t="s">
         <v>304</v>
       </c>
-      <c r="H256" s="27"/>
+      <c r="H256" s="27">
+        <v>26</v>
+      </c>
       <c r="I256" s="27"/>
       <c r="J256" s="20"/>
       <c r="K256" s="27"/>
@@ -24769,15 +24840,19 @@
       <c r="D257" s="37">
         <v>9</v>
       </c>
-      <c r="E257" s="158"/>
+      <c r="E257" s="158">
+        <v>6</v>
+      </c>
       <c r="F257" s="33">
         <f>IF(ISBLANK(E257),0,IF(E257=Answers!E257,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G257" s="159" t="s">
         <v>305</v>
       </c>
-      <c r="H257" s="27"/>
+      <c r="H257" s="27">
+        <v>6</v>
+      </c>
       <c r="I257" s="27"/>
       <c r="J257" s="20"/>
       <c r="K257" s="27"/>
@@ -24794,15 +24869,19 @@
       <c r="D258" s="37">
         <v>9</v>
       </c>
-      <c r="E258" s="158"/>
+      <c r="E258" s="158">
+        <v>11</v>
+      </c>
       <c r="F258" s="33">
         <f>IF(ISBLANK(E258),0,IF(E258=Answers!E258,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G258" s="159" t="s">
         <v>306</v>
       </c>
-      <c r="H258" s="27"/>
+      <c r="H258" s="27">
+        <v>11</v>
+      </c>
       <c r="I258" s="27"/>
       <c r="J258" s="20"/>
       <c r="K258" s="27"/>
@@ -24819,15 +24898,19 @@
       <c r="D259" s="37">
         <v>9</v>
       </c>
-      <c r="E259" s="158"/>
+      <c r="E259" s="158">
+        <v>24</v>
+      </c>
       <c r="F259" s="33">
         <f>IF(ISBLANK(E259),0,IF(E259=Answers!E259,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G259" s="159" t="s">
         <v>307</v>
       </c>
-      <c r="H259" s="27"/>
+      <c r="H259" s="27">
+        <v>24</v>
+      </c>
       <c r="I259" s="27"/>
       <c r="J259" s="20"/>
       <c r="K259" s="27"/>
@@ -24844,15 +24927,19 @@
       <c r="D260" s="37">
         <v>9</v>
       </c>
-      <c r="E260" s="158"/>
+      <c r="E260" s="158">
+        <v>12</v>
+      </c>
       <c r="F260" s="33">
         <f>IF(ISBLANK(E260),0,IF(E260=Answers!E260,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G260" s="159" t="s">
         <v>308</v>
       </c>
-      <c r="H260" s="27"/>
+      <c r="H260" s="27">
+        <v>12</v>
+      </c>
       <c r="I260" s="27"/>
       <c r="J260" s="20"/>
       <c r="K260" s="27"/>
@@ -24886,129 +24973,337 @@
       <c r="K262" s="27"/>
       <c r="L262" s="27"/>
     </row>
-    <row r="263" spans="1:12">
-      <c r="B263" s="192" t="s">
+    <row r="263" spans="1:12" ht="15" customHeight="1">
+      <c r="A263" s="13"/>
+      <c r="B263" s="27"/>
+      <c r="C263" s="27"/>
+      <c r="D263" s="27"/>
+      <c r="E263" s="27"/>
+      <c r="F263" s="30"/>
+      <c r="G263" s="27"/>
+      <c r="H263" s="27"/>
+      <c r="I263" s="27"/>
+      <c r="J263" s="29"/>
+      <c r="K263" s="27"/>
+      <c r="L263" s="27"/>
+    </row>
+    <row r="264" spans="1:12" ht="15" customHeight="1">
+      <c r="A264" s="13"/>
+      <c r="B264" s="27"/>
+      <c r="C264" s="27"/>
+      <c r="D264" s="27"/>
+      <c r="E264" s="27"/>
+      <c r="F264" s="30"/>
+      <c r="G264" s="27"/>
+      <c r="H264" s="27"/>
+      <c r="I264" s="27"/>
+      <c r="J264" s="29"/>
+      <c r="K264" s="27"/>
+      <c r="L264" s="27"/>
+    </row>
+    <row r="265" spans="1:12" ht="15" customHeight="1">
+      <c r="A265" s="13"/>
+      <c r="B265" s="27"/>
+      <c r="C265" s="27"/>
+      <c r="D265" s="27"/>
+      <c r="E265" s="27"/>
+      <c r="F265" s="30"/>
+      <c r="G265" s="27"/>
+      <c r="H265" s="27"/>
+      <c r="I265" s="27"/>
+      <c r="J265" s="29"/>
+      <c r="K265" s="27"/>
+      <c r="L265" s="27"/>
+    </row>
+    <row r="266" spans="1:12" ht="15" customHeight="1">
+      <c r="A266" s="13"/>
+      <c r="B266" s="27"/>
+      <c r="C266" s="27"/>
+      <c r="D266" s="27"/>
+      <c r="E266" s="27"/>
+      <c r="F266" s="30"/>
+      <c r="G266" s="27"/>
+      <c r="H266" s="27"/>
+      <c r="I266" s="27"/>
+      <c r="J266" s="29"/>
+      <c r="K266" s="27"/>
+      <c r="L266" s="27"/>
+    </row>
+    <row r="267" spans="1:12" ht="15" customHeight="1">
+      <c r="A267" s="13"/>
+      <c r="B267" s="27"/>
+      <c r="C267" s="27"/>
+      <c r="D267" s="27"/>
+      <c r="E267" s="27"/>
+      <c r="F267" s="30"/>
+      <c r="G267" s="27"/>
+      <c r="H267" s="27"/>
+      <c r="I267" s="27"/>
+      <c r="J267" s="29"/>
+      <c r="K267" s="27"/>
+      <c r="L267" s="27"/>
+    </row>
+    <row r="268" spans="1:12" ht="15" customHeight="1">
+      <c r="A268" s="13"/>
+      <c r="B268" s="27"/>
+      <c r="C268" s="27"/>
+      <c r="D268" s="27"/>
+      <c r="E268" s="27"/>
+      <c r="F268" s="30"/>
+      <c r="G268" s="27"/>
+      <c r="H268" s="27"/>
+      <c r="I268" s="27"/>
+      <c r="J268" s="29"/>
+      <c r="K268" s="27"/>
+      <c r="L268" s="27"/>
+    </row>
+    <row r="269" spans="1:12" ht="15" customHeight="1">
+      <c r="A269" s="13"/>
+      <c r="B269" s="27"/>
+      <c r="C269" s="27"/>
+      <c r="D269" s="27"/>
+      <c r="E269" s="27"/>
+      <c r="F269" s="30"/>
+      <c r="G269" s="27"/>
+      <c r="H269" s="27"/>
+      <c r="I269" s="27"/>
+      <c r="J269" s="29"/>
+      <c r="K269" s="27"/>
+      <c r="L269" s="27"/>
+    </row>
+    <row r="270" spans="1:12" ht="15" customHeight="1">
+      <c r="A270" s="13"/>
+      <c r="B270" s="27"/>
+      <c r="C270" s="27"/>
+      <c r="D270" s="27"/>
+      <c r="E270" s="27"/>
+      <c r="F270" s="30"/>
+      <c r="G270" s="27"/>
+      <c r="H270" s="27"/>
+      <c r="I270" s="27"/>
+      <c r="J270" s="29"/>
+      <c r="K270" s="27"/>
+      <c r="L270" s="27"/>
+    </row>
+    <row r="271" spans="1:12" ht="15" customHeight="1">
+      <c r="A271" s="13"/>
+      <c r="B271" s="27"/>
+      <c r="C271" s="27"/>
+      <c r="D271" s="27"/>
+      <c r="E271" s="27"/>
+      <c r="F271" s="30"/>
+      <c r="G271" s="27"/>
+      <c r="H271" s="27"/>
+      <c r="I271" s="27"/>
+      <c r="J271" s="29"/>
+      <c r="K271" s="27"/>
+      <c r="L271" s="27"/>
+    </row>
+    <row r="272" spans="1:12" ht="15" customHeight="1">
+      <c r="A272" s="13"/>
+      <c r="B272" s="27"/>
+      <c r="C272" s="27"/>
+      <c r="D272" s="27"/>
+      <c r="E272" s="27"/>
+      <c r="F272" s="30"/>
+      <c r="G272" s="27"/>
+      <c r="H272" s="27"/>
+      <c r="I272" s="27"/>
+      <c r="J272" s="29"/>
+      <c r="K272" s="27"/>
+      <c r="L272" s="27"/>
+    </row>
+    <row r="273" spans="1:12" ht="15" customHeight="1">
+      <c r="A273" s="13"/>
+      <c r="B273" s="27"/>
+      <c r="C273" s="27"/>
+      <c r="D273" s="27"/>
+      <c r="E273" s="27"/>
+      <c r="F273" s="30"/>
+      <c r="G273" s="27"/>
+      <c r="H273" s="27"/>
+      <c r="I273" s="27"/>
+      <c r="J273" s="29"/>
+      <c r="K273" s="27"/>
+      <c r="L273" s="27"/>
+    </row>
+    <row r="274" spans="1:12" ht="15" customHeight="1">
+      <c r="A274" s="13"/>
+      <c r="B274" s="27"/>
+      <c r="C274" s="27"/>
+      <c r="D274" s="27"/>
+      <c r="E274" s="27"/>
+      <c r="F274" s="30"/>
+      <c r="G274" s="27"/>
+      <c r="H274" s="27"/>
+      <c r="I274" s="27"/>
+      <c r="J274" s="29"/>
+      <c r="K274" s="27"/>
+      <c r="L274" s="27"/>
+    </row>
+    <row r="275" spans="1:12" ht="15" customHeight="1">
+      <c r="A275" s="13"/>
+      <c r="B275" s="27"/>
+      <c r="C275" s="27"/>
+      <c r="D275" s="27"/>
+      <c r="E275" s="27"/>
+      <c r="F275" s="30"/>
+      <c r="G275" s="27"/>
+      <c r="H275" s="27"/>
+      <c r="I275" s="27"/>
+      <c r="J275" s="29"/>
+      <c r="K275" s="27"/>
+      <c r="L275" s="27"/>
+    </row>
+    <row r="276" spans="1:12" ht="15" customHeight="1">
+      <c r="A276" s="13"/>
+      <c r="B276" s="27"/>
+      <c r="C276" s="27"/>
+      <c r="D276" s="27"/>
+      <c r="E276" s="27"/>
+      <c r="F276" s="30"/>
+      <c r="G276" s="27"/>
+      <c r="H276" s="27"/>
+      <c r="I276" s="27"/>
+      <c r="J276" s="29"/>
+      <c r="K276" s="27"/>
+      <c r="L276" s="27"/>
+    </row>
+    <row r="277" spans="1:12">
+      <c r="B277" s="184" t="s">
         <v>22</v>
       </c>
-      <c r="C263" s="193"/>
-      <c r="D263" s="193"/>
-      <c r="E263" s="193"/>
-      <c r="F263" s="193"/>
-      <c r="G263" s="193"/>
-      <c r="H263" s="193"/>
-      <c r="I263" s="193"/>
-      <c r="J263" s="193"/>
-      <c r="K263" s="193"/>
-      <c r="L263" s="193"/>
-    </row>
-    <row r="264" spans="1:12">
-      <c r="B264" s="183" t="s">
+      <c r="C277" s="185"/>
+      <c r="D277" s="185"/>
+      <c r="E277" s="185"/>
+      <c r="F277" s="185"/>
+      <c r="G277" s="185"/>
+      <c r="H277" s="185"/>
+      <c r="I277" s="185"/>
+      <c r="J277" s="185"/>
+      <c r="K277" s="185"/>
+      <c r="L277" s="185"/>
+    </row>
+    <row r="278" spans="1:12">
+      <c r="B278" s="219" t="s">
         <v>317</v>
       </c>
-      <c r="C264" s="184"/>
-      <c r="D264" s="184"/>
-      <c r="E264" s="184"/>
-      <c r="F264" s="184"/>
-      <c r="G264" s="184"/>
-      <c r="H264" s="184"/>
-      <c r="I264" s="184"/>
-      <c r="J264" s="184"/>
-      <c r="K264" s="184"/>
-      <c r="L264" s="185"/>
-    </row>
-    <row r="265" spans="1:12">
-      <c r="B265" s="186"/>
-      <c r="C265" s="187"/>
-      <c r="D265" s="187"/>
-      <c r="E265" s="187"/>
-      <c r="F265" s="187"/>
-      <c r="G265" s="187"/>
-      <c r="H265" s="187"/>
-      <c r="I265" s="187"/>
-      <c r="J265" s="187"/>
-      <c r="K265" s="187"/>
-      <c r="L265" s="188"/>
-    </row>
-    <row r="266" spans="1:12">
-      <c r="B266" s="186"/>
-      <c r="C266" s="187"/>
-      <c r="D266" s="187"/>
-      <c r="E266" s="187"/>
-      <c r="F266" s="187"/>
-      <c r="G266" s="187"/>
-      <c r="H266" s="187"/>
-      <c r="I266" s="187"/>
-      <c r="J266" s="187"/>
-      <c r="K266" s="187"/>
-      <c r="L266" s="188"/>
-    </row>
-    <row r="267" spans="1:12">
-      <c r="B267" s="186"/>
-      <c r="C267" s="187"/>
-      <c r="D267" s="187"/>
-      <c r="E267" s="187"/>
-      <c r="F267" s="187"/>
-      <c r="G267" s="187"/>
-      <c r="H267" s="187"/>
-      <c r="I267" s="187"/>
-      <c r="J267" s="187"/>
-      <c r="K267" s="187"/>
-      <c r="L267" s="188"/>
-    </row>
-    <row r="268" spans="1:12">
-      <c r="B268" s="186"/>
-      <c r="C268" s="187"/>
-      <c r="D268" s="187"/>
-      <c r="E268" s="187"/>
-      <c r="F268" s="187"/>
-      <c r="G268" s="187"/>
-      <c r="H268" s="187"/>
-      <c r="I268" s="187"/>
-      <c r="J268" s="187"/>
-      <c r="K268" s="187"/>
-      <c r="L268" s="188"/>
-    </row>
-    <row r="269" spans="1:12">
-      <c r="B269" s="186"/>
-      <c r="C269" s="187"/>
-      <c r="D269" s="187"/>
-      <c r="E269" s="187"/>
-      <c r="F269" s="187"/>
-      <c r="G269" s="187"/>
-      <c r="H269" s="187"/>
-      <c r="I269" s="187"/>
-      <c r="J269" s="187"/>
-      <c r="K269" s="187"/>
-      <c r="L269" s="188"/>
-    </row>
-    <row r="270" spans="1:12">
-      <c r="B270" s="186"/>
-      <c r="C270" s="187"/>
-      <c r="D270" s="187"/>
-      <c r="E270" s="187"/>
-      <c r="F270" s="187"/>
-      <c r="G270" s="187"/>
-      <c r="H270" s="187"/>
-      <c r="I270" s="187"/>
-      <c r="J270" s="187"/>
-      <c r="K270" s="187"/>
-      <c r="L270" s="188"/>
-    </row>
-    <row r="271" spans="1:12">
-      <c r="B271" s="189"/>
-      <c r="C271" s="190"/>
-      <c r="D271" s="190"/>
-      <c r="E271" s="190"/>
-      <c r="F271" s="190"/>
-      <c r="G271" s="190"/>
-      <c r="H271" s="190"/>
-      <c r="I271" s="190"/>
-      <c r="J271" s="190"/>
-      <c r="K271" s="190"/>
-      <c r="L271" s="191"/>
+      <c r="C278" s="220"/>
+      <c r="D278" s="220"/>
+      <c r="E278" s="220"/>
+      <c r="F278" s="220"/>
+      <c r="G278" s="220"/>
+      <c r="H278" s="220"/>
+      <c r="I278" s="220"/>
+      <c r="J278" s="220"/>
+      <c r="K278" s="220"/>
+      <c r="L278" s="221"/>
+    </row>
+    <row r="279" spans="1:12">
+      <c r="B279" s="222"/>
+      <c r="C279" s="223"/>
+      <c r="D279" s="223"/>
+      <c r="E279" s="223"/>
+      <c r="F279" s="223"/>
+      <c r="G279" s="223"/>
+      <c r="H279" s="223"/>
+      <c r="I279" s="223"/>
+      <c r="J279" s="223"/>
+      <c r="K279" s="223"/>
+      <c r="L279" s="224"/>
+    </row>
+    <row r="280" spans="1:12">
+      <c r="B280" s="222"/>
+      <c r="C280" s="223"/>
+      <c r="D280" s="223"/>
+      <c r="E280" s="223"/>
+      <c r="F280" s="223"/>
+      <c r="G280" s="223"/>
+      <c r="H280" s="223"/>
+      <c r="I280" s="223"/>
+      <c r="J280" s="223"/>
+      <c r="K280" s="223"/>
+      <c r="L280" s="224"/>
+    </row>
+    <row r="281" spans="1:12">
+      <c r="B281" s="222"/>
+      <c r="C281" s="223"/>
+      <c r="D281" s="223"/>
+      <c r="E281" s="223"/>
+      <c r="F281" s="223"/>
+      <c r="G281" s="223"/>
+      <c r="H281" s="223"/>
+      <c r="I281" s="223"/>
+      <c r="J281" s="223"/>
+      <c r="K281" s="223"/>
+      <c r="L281" s="224"/>
+    </row>
+    <row r="282" spans="1:12">
+      <c r="B282" s="222"/>
+      <c r="C282" s="223"/>
+      <c r="D282" s="223"/>
+      <c r="E282" s="223"/>
+      <c r="F282" s="223"/>
+      <c r="G282" s="223"/>
+      <c r="H282" s="223"/>
+      <c r="I282" s="223"/>
+      <c r="J282" s="223"/>
+      <c r="K282" s="223"/>
+      <c r="L282" s="224"/>
+    </row>
+    <row r="283" spans="1:12">
+      <c r="B283" s="222"/>
+      <c r="C283" s="223"/>
+      <c r="D283" s="223"/>
+      <c r="E283" s="223"/>
+      <c r="F283" s="223"/>
+      <c r="G283" s="223"/>
+      <c r="H283" s="223"/>
+      <c r="I283" s="223"/>
+      <c r="J283" s="223"/>
+      <c r="K283" s="223"/>
+      <c r="L283" s="224"/>
+    </row>
+    <row r="284" spans="1:12">
+      <c r="B284" s="222"/>
+      <c r="C284" s="223"/>
+      <c r="D284" s="223"/>
+      <c r="E284" s="223"/>
+      <c r="F284" s="223"/>
+      <c r="G284" s="223"/>
+      <c r="H284" s="223"/>
+      <c r="I284" s="223"/>
+      <c r="J284" s="223"/>
+      <c r="K284" s="223"/>
+      <c r="L284" s="224"/>
+    </row>
+    <row r="285" spans="1:12">
+      <c r="B285" s="225"/>
+      <c r="C285" s="226"/>
+      <c r="D285" s="226"/>
+      <c r="E285" s="226"/>
+      <c r="F285" s="226"/>
+      <c r="G285" s="226"/>
+      <c r="H285" s="226"/>
+      <c r="I285" s="226"/>
+      <c r="J285" s="226"/>
+      <c r="K285" s="226"/>
+      <c r="L285" s="227"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B278:L285"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L36"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I63:J64"/>
+    <mergeCell ref="K63:L64"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="B100:L100"/>
+    <mergeCell ref="B101:L107"/>
+    <mergeCell ref="B109:L109"/>
+    <mergeCell ref="B118:C119"/>
+    <mergeCell ref="B277:L277"/>
     <mergeCell ref="B30:L30"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B4:L4"/>
@@ -25021,18 +25316,6 @@
     <mergeCell ref="G26:L26"/>
     <mergeCell ref="G27:L27"/>
     <mergeCell ref="G28:L28"/>
-    <mergeCell ref="B264:L271"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L36"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I63:J64"/>
-    <mergeCell ref="K63:L64"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="B100:L100"/>
-    <mergeCell ref="B101:L107"/>
-    <mergeCell ref="B109:L109"/>
-    <mergeCell ref="B118:C119"/>
-    <mergeCell ref="B263:L263"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -25088,15 +25371,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="22.8">
-      <c r="B2" s="192" t="s">
+      <c r="B2" s="184" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="193"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="185"/>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="179" t="s">
@@ -25386,15 +25669,15 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="22.8">
-      <c r="B18" s="192" t="s">
+      <c r="B18" s="184" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="193"/>
-      <c r="D18" s="193"/>
-      <c r="E18" s="193"/>
-      <c r="F18" s="193"/>
-      <c r="G18" s="193"/>
-      <c r="H18" s="193"/>
+      <c r="C18" s="185"/>
+      <c r="D18" s="185"/>
+      <c r="E18" s="185"/>
+      <c r="F18" s="185"/>
+      <c r="G18" s="185"/>
+      <c r="H18" s="185"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="U5:X14">
@@ -25417,9 +25700,9 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:XFD69"/>
+  <dimension ref="A1:XFC69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="N24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
@@ -26277,7 +26560,7 @@
       <c r="V27" s="105"/>
       <c r="W27" s="105"/>
       <c r="X27" s="105"/>
-      <c r="Y27" s="257">
+      <c r="Y27" s="183">
         <f ca="1">COUNTIFS(_xlfn.ANCHORARRAY(Y28),2)</f>
         <v>3</v>
       </c>
@@ -27669,171 +27952,171 @@
       <c r="Z63" s="103"/>
     </row>
     <row r="64" spans="1:26" hidden="1">
-      <c r="A64" s="256"/>
-      <c r="B64" s="256"/>
-      <c r="C64" s="256"/>
-      <c r="D64" s="256"/>
-      <c r="E64" s="256"/>
-      <c r="F64" s="256"/>
-      <c r="G64" s="256"/>
-      <c r="H64" s="256"/>
-      <c r="I64" s="256"/>
-      <c r="J64" s="256"/>
-      <c r="K64" s="256"/>
-      <c r="L64" s="256"/>
-      <c r="M64" s="256"/>
-      <c r="N64" s="256"/>
-      <c r="O64" s="256"/>
-      <c r="P64" s="256"/>
-      <c r="Q64" s="256"/>
-      <c r="R64" s="256"/>
-      <c r="S64" s="256"/>
-      <c r="T64" s="256"/>
-      <c r="U64" s="256"/>
-      <c r="V64" s="256"/>
-      <c r="W64" s="256"/>
-      <c r="X64" s="256"/>
-      <c r="Y64" s="256"/>
+      <c r="A64" s="257"/>
+      <c r="B64" s="257"/>
+      <c r="C64" s="257"/>
+      <c r="D64" s="257"/>
+      <c r="E64" s="257"/>
+      <c r="F64" s="257"/>
+      <c r="G64" s="257"/>
+      <c r="H64" s="257"/>
+      <c r="I64" s="257"/>
+      <c r="J64" s="257"/>
+      <c r="K64" s="257"/>
+      <c r="L64" s="257"/>
+      <c r="M64" s="257"/>
+      <c r="N64" s="257"/>
+      <c r="O64" s="257"/>
+      <c r="P64" s="257"/>
+      <c r="Q64" s="257"/>
+      <c r="R64" s="257"/>
+      <c r="S64" s="257"/>
+      <c r="T64" s="257"/>
+      <c r="U64" s="257"/>
+      <c r="V64" s="257"/>
+      <c r="W64" s="257"/>
+      <c r="X64" s="257"/>
+      <c r="Y64" s="257"/>
       <c r="Z64" s="104"/>
     </row>
     <row r="65" spans="1:26" hidden="1">
-      <c r="A65" s="256"/>
-      <c r="B65" s="256"/>
-      <c r="C65" s="256"/>
-      <c r="D65" s="256"/>
-      <c r="E65" s="256"/>
-      <c r="F65" s="256"/>
-      <c r="G65" s="256"/>
-      <c r="H65" s="256"/>
-      <c r="I65" s="256"/>
-      <c r="J65" s="256"/>
-      <c r="K65" s="256"/>
-      <c r="L65" s="256"/>
-      <c r="M65" s="256"/>
-      <c r="N65" s="256"/>
-      <c r="O65" s="256"/>
-      <c r="P65" s="256"/>
-      <c r="Q65" s="256"/>
-      <c r="R65" s="256"/>
-      <c r="S65" s="256"/>
-      <c r="T65" s="256"/>
-      <c r="U65" s="256"/>
-      <c r="V65" s="256"/>
-      <c r="W65" s="256"/>
-      <c r="X65" s="256"/>
-      <c r="Y65" s="256"/>
+      <c r="A65" s="257"/>
+      <c r="B65" s="257"/>
+      <c r="C65" s="257"/>
+      <c r="D65" s="257"/>
+      <c r="E65" s="257"/>
+      <c r="F65" s="257"/>
+      <c r="G65" s="257"/>
+      <c r="H65" s="257"/>
+      <c r="I65" s="257"/>
+      <c r="J65" s="257"/>
+      <c r="K65" s="257"/>
+      <c r="L65" s="257"/>
+      <c r="M65" s="257"/>
+      <c r="N65" s="257"/>
+      <c r="O65" s="257"/>
+      <c r="P65" s="257"/>
+      <c r="Q65" s="257"/>
+      <c r="R65" s="257"/>
+      <c r="S65" s="257"/>
+      <c r="T65" s="257"/>
+      <c r="U65" s="257"/>
+      <c r="V65" s="257"/>
+      <c r="W65" s="257"/>
+      <c r="X65" s="257"/>
+      <c r="Y65" s="257"/>
       <c r="Z65" s="104"/>
     </row>
     <row r="66" spans="1:26" hidden="1">
-      <c r="A66" s="256"/>
-      <c r="B66" s="256"/>
-      <c r="C66" s="256"/>
-      <c r="D66" s="256"/>
-      <c r="E66" s="256"/>
-      <c r="F66" s="256"/>
-      <c r="G66" s="256"/>
-      <c r="H66" s="256"/>
-      <c r="I66" s="256"/>
-      <c r="J66" s="256"/>
-      <c r="K66" s="256"/>
-      <c r="L66" s="256"/>
-      <c r="M66" s="256"/>
-      <c r="N66" s="256"/>
-      <c r="O66" s="256"/>
-      <c r="P66" s="256"/>
-      <c r="Q66" s="256"/>
-      <c r="R66" s="256"/>
-      <c r="S66" s="256"/>
-      <c r="T66" s="256"/>
-      <c r="U66" s="256"/>
-      <c r="V66" s="256"/>
-      <c r="W66" s="256"/>
-      <c r="X66" s="256"/>
-      <c r="Y66" s="256"/>
+      <c r="A66" s="257"/>
+      <c r="B66" s="257"/>
+      <c r="C66" s="257"/>
+      <c r="D66" s="257"/>
+      <c r="E66" s="257"/>
+      <c r="F66" s="257"/>
+      <c r="G66" s="257"/>
+      <c r="H66" s="257"/>
+      <c r="I66" s="257"/>
+      <c r="J66" s="257"/>
+      <c r="K66" s="257"/>
+      <c r="L66" s="257"/>
+      <c r="M66" s="257"/>
+      <c r="N66" s="257"/>
+      <c r="O66" s="257"/>
+      <c r="P66" s="257"/>
+      <c r="Q66" s="257"/>
+      <c r="R66" s="257"/>
+      <c r="S66" s="257"/>
+      <c r="T66" s="257"/>
+      <c r="U66" s="257"/>
+      <c r="V66" s="257"/>
+      <c r="W66" s="257"/>
+      <c r="X66" s="257"/>
+      <c r="Y66" s="257"/>
       <c r="Z66" s="104"/>
     </row>
     <row r="67" spans="1:26" hidden="1">
-      <c r="A67" s="256"/>
-      <c r="B67" s="256"/>
-      <c r="C67" s="256"/>
-      <c r="D67" s="256"/>
-      <c r="E67" s="256"/>
-      <c r="F67" s="256"/>
-      <c r="G67" s="256"/>
-      <c r="H67" s="256"/>
-      <c r="I67" s="256"/>
-      <c r="J67" s="256"/>
-      <c r="K67" s="256"/>
-      <c r="L67" s="256"/>
-      <c r="M67" s="256"/>
-      <c r="N67" s="256"/>
-      <c r="O67" s="256"/>
-      <c r="P67" s="256"/>
-      <c r="Q67" s="256"/>
-      <c r="R67" s="256"/>
-      <c r="S67" s="256"/>
-      <c r="T67" s="256"/>
-      <c r="U67" s="256"/>
-      <c r="V67" s="256"/>
-      <c r="W67" s="256"/>
-      <c r="X67" s="256"/>
-      <c r="Y67" s="256"/>
+      <c r="A67" s="257"/>
+      <c r="B67" s="257"/>
+      <c r="C67" s="257"/>
+      <c r="D67" s="257"/>
+      <c r="E67" s="257"/>
+      <c r="F67" s="257"/>
+      <c r="G67" s="257"/>
+      <c r="H67" s="257"/>
+      <c r="I67" s="257"/>
+      <c r="J67" s="257"/>
+      <c r="K67" s="257"/>
+      <c r="L67" s="257"/>
+      <c r="M67" s="257"/>
+      <c r="N67" s="257"/>
+      <c r="O67" s="257"/>
+      <c r="P67" s="257"/>
+      <c r="Q67" s="257"/>
+      <c r="R67" s="257"/>
+      <c r="S67" s="257"/>
+      <c r="T67" s="257"/>
+      <c r="U67" s="257"/>
+      <c r="V67" s="257"/>
+      <c r="W67" s="257"/>
+      <c r="X67" s="257"/>
+      <c r="Y67" s="257"/>
       <c r="Z67" s="104"/>
     </row>
     <row r="68" spans="1:26" hidden="1">
-      <c r="A68" s="256"/>
-      <c r="B68" s="256"/>
-      <c r="C68" s="256"/>
-      <c r="D68" s="256"/>
-      <c r="E68" s="256"/>
-      <c r="F68" s="256"/>
-      <c r="G68" s="256"/>
-      <c r="H68" s="256"/>
-      <c r="I68" s="256"/>
-      <c r="J68" s="256"/>
-      <c r="K68" s="256"/>
-      <c r="L68" s="256"/>
-      <c r="M68" s="256"/>
-      <c r="N68" s="256"/>
-      <c r="O68" s="256"/>
-      <c r="P68" s="256"/>
-      <c r="Q68" s="256"/>
-      <c r="R68" s="256"/>
-      <c r="S68" s="256"/>
-      <c r="T68" s="256"/>
-      <c r="U68" s="256"/>
-      <c r="V68" s="256"/>
-      <c r="W68" s="256"/>
-      <c r="X68" s="256"/>
-      <c r="Y68" s="256"/>
+      <c r="A68" s="257"/>
+      <c r="B68" s="257"/>
+      <c r="C68" s="257"/>
+      <c r="D68" s="257"/>
+      <c r="E68" s="257"/>
+      <c r="F68" s="257"/>
+      <c r="G68" s="257"/>
+      <c r="H68" s="257"/>
+      <c r="I68" s="257"/>
+      <c r="J68" s="257"/>
+      <c r="K68" s="257"/>
+      <c r="L68" s="257"/>
+      <c r="M68" s="257"/>
+      <c r="N68" s="257"/>
+      <c r="O68" s="257"/>
+      <c r="P68" s="257"/>
+      <c r="Q68" s="257"/>
+      <c r="R68" s="257"/>
+      <c r="S68" s="257"/>
+      <c r="T68" s="257"/>
+      <c r="U68" s="257"/>
+      <c r="V68" s="257"/>
+      <c r="W68" s="257"/>
+      <c r="X68" s="257"/>
+      <c r="Y68" s="257"/>
       <c r="Z68" s="104"/>
     </row>
     <row r="69" spans="1:26" hidden="1">
-      <c r="A69" s="256"/>
-      <c r="B69" s="256"/>
-      <c r="C69" s="256"/>
-      <c r="D69" s="256"/>
-      <c r="E69" s="256"/>
-      <c r="F69" s="256"/>
-      <c r="G69" s="256"/>
-      <c r="H69" s="256"/>
-      <c r="I69" s="256"/>
-      <c r="J69" s="256"/>
-      <c r="K69" s="256"/>
-      <c r="L69" s="256"/>
-      <c r="M69" s="256"/>
-      <c r="N69" s="256"/>
-      <c r="O69" s="256"/>
-      <c r="P69" s="256"/>
-      <c r="Q69" s="256"/>
-      <c r="R69" s="256"/>
-      <c r="S69" s="256"/>
-      <c r="T69" s="256"/>
-      <c r="U69" s="256"/>
-      <c r="V69" s="256"/>
-      <c r="W69" s="256"/>
-      <c r="X69" s="256"/>
-      <c r="Y69" s="256"/>
+      <c r="A69" s="257"/>
+      <c r="B69" s="257"/>
+      <c r="C69" s="257"/>
+      <c r="D69" s="257"/>
+      <c r="E69" s="257"/>
+      <c r="F69" s="257"/>
+      <c r="G69" s="257"/>
+      <c r="H69" s="257"/>
+      <c r="I69" s="257"/>
+      <c r="J69" s="257"/>
+      <c r="K69" s="257"/>
+      <c r="L69" s="257"/>
+      <c r="M69" s="257"/>
+      <c r="N69" s="257"/>
+      <c r="O69" s="257"/>
+      <c r="P69" s="257"/>
+      <c r="Q69" s="257"/>
+      <c r="R69" s="257"/>
+      <c r="S69" s="257"/>
+      <c r="T69" s="257"/>
+      <c r="U69" s="257"/>
+      <c r="V69" s="257"/>
+      <c r="W69" s="257"/>
+      <c r="X69" s="257"/>
+      <c r="Y69" s="257"/>
       <c r="Z69" s="104"/>
     </row>
   </sheetData>
@@ -27854,7 +28137,7 @@
   </sheetPr>
   <dimension ref="A1:AN40"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="AA3" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="25.2" zeroHeight="1"/>
   <cols>
@@ -30231,19 +30514,19 @@
       <c r="A1"/>
     </row>
     <row r="2" spans="1:12" ht="59.25" customHeight="1">
-      <c r="B2" s="223" t="s">
+      <c r="B2" s="186" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
-      <c r="L2" s="224"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" outlineLevel="1">
       <c r="A3"/>
@@ -30260,19 +30543,19 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" ht="75" customHeight="1" outlineLevel="1">
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="188" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="225"/>
-      <c r="D4" s="225"/>
-      <c r="E4" s="225"/>
-      <c r="F4" s="225"/>
-      <c r="G4" s="225"/>
-      <c r="H4" s="225"/>
-      <c r="I4" s="225"/>
-      <c r="J4" s="225"/>
-      <c r="K4" s="225"/>
-      <c r="L4" s="225"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="188"/>
+      <c r="K4" s="188"/>
+      <c r="L4" s="188"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="B5" s="2"/>
@@ -30288,112 +30571,112 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="33" customHeight="1">
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="184" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="193"/>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="193"/>
-      <c r="H6" s="193"/>
-      <c r="I6" s="226"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="185"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="189"/>
       <c r="J6"/>
-      <c r="K6" s="227" t="s">
+      <c r="K6" s="190" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="228"/>
+      <c r="L6" s="191"/>
     </row>
     <row r="7" spans="1:12" ht="25.95" customHeight="1">
-      <c r="B7" s="229" t="s">
+      <c r="B7" s="192" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="230"/>
-      <c r="D7" s="230"/>
-      <c r="E7" s="230"/>
-      <c r="F7" s="230"/>
-      <c r="G7" s="230"/>
-      <c r="H7" s="230"/>
-      <c r="I7" s="231"/>
+      <c r="C7" s="193"/>
+      <c r="D7" s="193"/>
+      <c r="E7" s="193"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="193"/>
+      <c r="I7" s="194"/>
       <c r="K7" s="5"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="232"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233"/>
-      <c r="H8" s="233"/>
-      <c r="I8" s="234"/>
+      <c r="B8" s="195"/>
+      <c r="C8" s="196"/>
+      <c r="D8" s="196"/>
+      <c r="E8" s="196"/>
+      <c r="F8" s="196"/>
+      <c r="G8" s="196"/>
+      <c r="H8" s="196"/>
+      <c r="I8" s="197"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="232"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
-      <c r="G9" s="233"/>
-      <c r="H9" s="233"/>
-      <c r="I9" s="234"/>
+      <c r="B9" s="195"/>
+      <c r="C9" s="196"/>
+      <c r="D9" s="196"/>
+      <c r="E9" s="196"/>
+      <c r="F9" s="196"/>
+      <c r="G9" s="196"/>
+      <c r="H9" s="196"/>
+      <c r="I9" s="197"/>
       <c r="J9"/>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="B10" s="232"/>
-      <c r="C10" s="233"/>
-      <c r="D10" s="233"/>
-      <c r="E10" s="233"/>
-      <c r="F10" s="233"/>
-      <c r="G10" s="233"/>
-      <c r="H10" s="233"/>
-      <c r="I10" s="234"/>
+      <c r="B10" s="195"/>
+      <c r="C10" s="196"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="196"/>
+      <c r="H10" s="196"/>
+      <c r="I10" s="197"/>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="B11" s="232"/>
-      <c r="C11" s="233"/>
-      <c r="D11" s="233"/>
-      <c r="E11" s="233"/>
-      <c r="F11" s="233"/>
-      <c r="G11" s="233"/>
-      <c r="H11" s="233"/>
-      <c r="I11" s="234"/>
+      <c r="B11" s="195"/>
+      <c r="C11" s="196"/>
+      <c r="D11" s="196"/>
+      <c r="E11" s="196"/>
+      <c r="F11" s="196"/>
+      <c r="G11" s="196"/>
+      <c r="H11" s="196"/>
+      <c r="I11" s="197"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="B12" s="232"/>
-      <c r="C12" s="233"/>
-      <c r="D12" s="233"/>
-      <c r="E12" s="233"/>
-      <c r="F12" s="233"/>
-      <c r="G12" s="233"/>
-      <c r="H12" s="233"/>
-      <c r="I12" s="234"/>
+      <c r="B12" s="195"/>
+      <c r="C12" s="196"/>
+      <c r="D12" s="196"/>
+      <c r="E12" s="196"/>
+      <c r="F12" s="196"/>
+      <c r="G12" s="196"/>
+      <c r="H12" s="196"/>
+      <c r="I12" s="197"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:12" ht="23.25" customHeight="1">
-      <c r="B13" s="232"/>
-      <c r="C13" s="233"/>
-      <c r="D13" s="233"/>
-      <c r="E13" s="233"/>
-      <c r="F13" s="233"/>
-      <c r="G13" s="233"/>
-      <c r="H13" s="233"/>
-      <c r="I13" s="234"/>
+      <c r="B13" s="195"/>
+      <c r="C13" s="196"/>
+      <c r="D13" s="196"/>
+      <c r="E13" s="196"/>
+      <c r="F13" s="196"/>
+      <c r="G13" s="196"/>
+      <c r="H13" s="196"/>
+      <c r="I13" s="197"/>
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:12" ht="33" customHeight="1">
-      <c r="B14" s="235"/>
-      <c r="C14" s="236"/>
-      <c r="D14" s="236"/>
-      <c r="E14" s="236"/>
-      <c r="F14" s="236"/>
-      <c r="G14" s="236"/>
-      <c r="H14" s="236"/>
-      <c r="I14" s="237"/>
+      <c r="B14" s="198"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="199"/>
+      <c r="F14" s="199"/>
+      <c r="G14" s="199"/>
+      <c r="H14" s="199"/>
+      <c r="I14" s="200"/>
       <c r="K14" s="34" t="s">
         <v>0</v>
       </c>
@@ -30407,60 +30690,60 @@
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B16" s="192" t="s">
+      <c r="B16" s="184" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="193"/>
-      <c r="D16" s="193"/>
-      <c r="E16" s="193"/>
-      <c r="F16" s="193"/>
-      <c r="G16" s="193"/>
-      <c r="H16" s="193"/>
-      <c r="I16" s="193"/>
-      <c r="J16" s="193"/>
-      <c r="K16" s="193"/>
-      <c r="L16" s="193"/>
+      <c r="C16" s="185"/>
+      <c r="D16" s="185"/>
+      <c r="E16" s="185"/>
+      <c r="F16" s="185"/>
+      <c r="G16" s="185"/>
+      <c r="H16" s="185"/>
+      <c r="I16" s="185"/>
+      <c r="J16" s="185"/>
+      <c r="K16" s="185"/>
+      <c r="L16" s="185"/>
     </row>
     <row r="17" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B17" s="238" t="s">
+      <c r="B17" s="201" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="239"/>
-      <c r="D17" s="239"/>
-      <c r="E17" s="239"/>
-      <c r="F17" s="239"/>
-      <c r="G17" s="239"/>
-      <c r="H17" s="239"/>
-      <c r="I17" s="239"/>
-      <c r="J17" s="239"/>
-      <c r="K17" s="239"/>
-      <c r="L17" s="240"/>
+      <c r="C17" s="202"/>
+      <c r="D17" s="202"/>
+      <c r="E17" s="202"/>
+      <c r="F17" s="202"/>
+      <c r="G17" s="202"/>
+      <c r="H17" s="202"/>
+      <c r="I17" s="202"/>
+      <c r="J17" s="202"/>
+      <c r="K17" s="202"/>
+      <c r="L17" s="203"/>
     </row>
     <row r="18" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B18" s="241"/>
-      <c r="C18" s="242"/>
-      <c r="D18" s="242"/>
-      <c r="E18" s="242"/>
-      <c r="F18" s="242"/>
-      <c r="G18" s="242"/>
-      <c r="H18" s="242"/>
-      <c r="I18" s="242"/>
-      <c r="J18" s="242"/>
-      <c r="K18" s="242"/>
-      <c r="L18" s="243"/>
+      <c r="B18" s="204"/>
+      <c r="C18" s="205"/>
+      <c r="D18" s="205"/>
+      <c r="E18" s="205"/>
+      <c r="F18" s="205"/>
+      <c r="G18" s="205"/>
+      <c r="H18" s="205"/>
+      <c r="I18" s="205"/>
+      <c r="J18" s="205"/>
+      <c r="K18" s="205"/>
+      <c r="L18" s="206"/>
     </row>
     <row r="19" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B19" s="244"/>
-      <c r="C19" s="245"/>
-      <c r="D19" s="245"/>
-      <c r="E19" s="245"/>
-      <c r="F19" s="245"/>
-      <c r="G19" s="245"/>
-      <c r="H19" s="245"/>
-      <c r="I19" s="245"/>
-      <c r="J19" s="245"/>
-      <c r="K19" s="245"/>
-      <c r="L19" s="246"/>
+      <c r="B19" s="207"/>
+      <c r="C19" s="208"/>
+      <c r="D19" s="208"/>
+      <c r="E19" s="208"/>
+      <c r="F19" s="208"/>
+      <c r="G19" s="208"/>
+      <c r="H19" s="208"/>
+      <c r="I19" s="208"/>
+      <c r="J19" s="208"/>
+      <c r="K19" s="208"/>
+      <c r="L19" s="209"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="B20" s="8"/>
@@ -30476,19 +30759,19 @@
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B21" s="192" t="s">
+      <c r="B21" s="184" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="193"/>
-      <c r="D21" s="193"/>
-      <c r="E21" s="193"/>
-      <c r="F21" s="193"/>
-      <c r="G21" s="193"/>
-      <c r="H21" s="193"/>
-      <c r="I21" s="193"/>
-      <c r="J21" s="193"/>
-      <c r="K21" s="193"/>
-      <c r="L21" s="193"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="185"/>
+      <c r="E21" s="185"/>
+      <c r="F21" s="185"/>
+      <c r="G21" s="185"/>
+      <c r="H21" s="185"/>
+      <c r="I21" s="185"/>
+      <c r="J21" s="185"/>
+      <c r="K21" s="185"/>
+      <c r="L21" s="185"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="B22" s="9"/>
@@ -30569,14 +30852,14 @@
         <v>2</v>
       </c>
       <c r="F26" s="33"/>
-      <c r="G26" s="247" t="s">
+      <c r="G26" s="210" t="s">
         <v>187</v>
       </c>
-      <c r="H26" s="248"/>
-      <c r="I26" s="248"/>
-      <c r="J26" s="248"/>
-      <c r="K26" s="248"/>
-      <c r="L26" s="249"/>
+      <c r="H26" s="211"/>
+      <c r="I26" s="211"/>
+      <c r="J26" s="211"/>
+      <c r="K26" s="211"/>
+      <c r="L26" s="212"/>
     </row>
     <row r="27" spans="1:12" ht="33.75" customHeight="1">
       <c r="B27" s="36" t="s">
@@ -30592,14 +30875,14 @@
         <v>360360</v>
       </c>
       <c r="F27" s="33"/>
-      <c r="G27" s="250" t="s">
+      <c r="G27" s="213" t="s">
         <v>186</v>
       </c>
-      <c r="H27" s="251"/>
-      <c r="I27" s="251"/>
-      <c r="J27" s="251"/>
-      <c r="K27" s="251"/>
-      <c r="L27" s="252"/>
+      <c r="H27" s="214"/>
+      <c r="I27" s="214"/>
+      <c r="J27" s="214"/>
+      <c r="K27" s="214"/>
+      <c r="L27" s="215"/>
     </row>
     <row r="28" spans="1:12" ht="54" customHeight="1">
       <c r="B28" s="36" t="s">
@@ -30615,14 +30898,14 @@
         <v>312</v>
       </c>
       <c r="F28" s="33"/>
-      <c r="G28" s="253" t="s">
+      <c r="G28" s="216" t="s">
         <v>345</v>
       </c>
-      <c r="H28" s="254"/>
-      <c r="I28" s="254"/>
-      <c r="J28" s="254"/>
-      <c r="K28" s="254"/>
-      <c r="L28" s="255"/>
+      <c r="H28" s="217"/>
+      <c r="I28" s="217"/>
+      <c r="J28" s="217"/>
+      <c r="K28" s="217"/>
+      <c r="L28" s="218"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="B29" s="2"/>
@@ -30638,19 +30921,19 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="B30" s="192" t="s">
+      <c r="B30" s="184" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="193"/>
-      <c r="D30" s="193"/>
-      <c r="E30" s="193"/>
-      <c r="F30" s="193"/>
-      <c r="G30" s="193"/>
-      <c r="H30" s="193"/>
-      <c r="I30" s="193"/>
-      <c r="J30" s="193"/>
-      <c r="K30" s="193"/>
-      <c r="L30" s="193"/>
+      <c r="C30" s="185"/>
+      <c r="D30" s="185"/>
+      <c r="E30" s="185"/>
+      <c r="F30" s="185"/>
+      <c r="G30" s="185"/>
+      <c r="H30" s="185"/>
+      <c r="I30" s="185"/>
+      <c r="J30" s="185"/>
+      <c r="K30" s="185"/>
+      <c r="L30" s="185"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="B31" s="16"/>
@@ -30880,10 +31163,10 @@
         <v>122</v>
       </c>
       <c r="F45" s="18"/>
-      <c r="G45" s="200" t="s">
+      <c r="G45" s="234" t="s">
         <v>324</v>
       </c>
-      <c r="H45" s="201"/>
+      <c r="H45" s="235"/>
       <c r="I45" s="91" t="s">
         <v>52</v>
       </c>
@@ -31276,14 +31559,14 @@
       <c r="F63" s="18"/>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
-      <c r="I63" s="202" t="s">
+      <c r="I63" s="236" t="s">
         <v>138</v>
       </c>
-      <c r="J63" s="203"/>
-      <c r="K63" s="206" t="s">
+      <c r="J63" s="237"/>
+      <c r="K63" s="240" t="s">
         <v>141</v>
       </c>
-      <c r="L63" s="207"/>
+      <c r="L63" s="241"/>
     </row>
     <row r="64" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A64" s="13"/>
@@ -31296,10 +31579,10 @@
       <c r="F64" s="18"/>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
-      <c r="I64" s="204"/>
-      <c r="J64" s="205"/>
-      <c r="K64" s="208"/>
-      <c r="L64" s="209"/>
+      <c r="I64" s="238"/>
+      <c r="J64" s="239"/>
+      <c r="K64" s="242"/>
+      <c r="L64" s="243"/>
     </row>
     <row r="65" spans="1:12" ht="15" customHeight="1">
       <c r="A65" s="13"/>
@@ -31468,16 +31751,16 @@
         <v>349</v>
       </c>
       <c r="F75" s="85"/>
-      <c r="G75" s="210" t="s">
+      <c r="G75" s="244" t="s">
         <v>136</v>
       </c>
-      <c r="H75" s="211"/>
-      <c r="I75" s="211"/>
-      <c r="J75" s="212"/>
-      <c r="K75" s="210" t="s">
+      <c r="H75" s="245"/>
+      <c r="I75" s="245"/>
+      <c r="J75" s="246"/>
+      <c r="K75" s="244" t="s">
         <v>135</v>
       </c>
-      <c r="L75" s="212"/>
+      <c r="L75" s="246"/>
     </row>
     <row r="76" spans="1:12" ht="15" customHeight="1">
       <c r="A76" s="13"/>
@@ -32068,119 +32351,119 @@
       <c r="L99" s="20"/>
     </row>
     <row r="100" spans="1:12">
-      <c r="B100" s="192" t="s">
+      <c r="B100" s="184" t="s">
         <v>21</v>
       </c>
-      <c r="C100" s="193"/>
-      <c r="D100" s="193"/>
-      <c r="E100" s="193"/>
-      <c r="F100" s="193"/>
-      <c r="G100" s="193"/>
-      <c r="H100" s="193"/>
-      <c r="I100" s="193"/>
-      <c r="J100" s="193"/>
-      <c r="K100" s="193"/>
-      <c r="L100" s="193"/>
+      <c r="C100" s="185"/>
+      <c r="D100" s="185"/>
+      <c r="E100" s="185"/>
+      <c r="F100" s="185"/>
+      <c r="G100" s="185"/>
+      <c r="H100" s="185"/>
+      <c r="I100" s="185"/>
+      <c r="J100" s="185"/>
+      <c r="K100" s="185"/>
+      <c r="L100" s="185"/>
     </row>
     <row r="101" spans="1:12" ht="15" customHeight="1">
       <c r="A101" s="13"/>
-      <c r="B101" s="183" t="s">
+      <c r="B101" s="219" t="s">
         <v>198</v>
       </c>
-      <c r="C101" s="213"/>
-      <c r="D101" s="213"/>
-      <c r="E101" s="213"/>
-      <c r="F101" s="213"/>
-      <c r="G101" s="213"/>
-      <c r="H101" s="213"/>
-      <c r="I101" s="213"/>
-      <c r="J101" s="213"/>
-      <c r="K101" s="213"/>
-      <c r="L101" s="214"/>
+      <c r="C101" s="247"/>
+      <c r="D101" s="247"/>
+      <c r="E101" s="247"/>
+      <c r="F101" s="247"/>
+      <c r="G101" s="247"/>
+      <c r="H101" s="247"/>
+      <c r="I101" s="247"/>
+      <c r="J101" s="247"/>
+      <c r="K101" s="247"/>
+      <c r="L101" s="248"/>
     </row>
     <row r="102" spans="1:12" ht="15" customHeight="1">
       <c r="A102" s="13"/>
-      <c r="B102" s="215"/>
-      <c r="C102" s="216"/>
-      <c r="D102" s="216"/>
-      <c r="E102" s="216"/>
-      <c r="F102" s="216"/>
-      <c r="G102" s="216"/>
-      <c r="H102" s="216"/>
-      <c r="I102" s="216"/>
-      <c r="J102" s="216"/>
-      <c r="K102" s="216"/>
-      <c r="L102" s="217"/>
+      <c r="B102" s="249"/>
+      <c r="C102" s="250"/>
+      <c r="D102" s="250"/>
+      <c r="E102" s="250"/>
+      <c r="F102" s="250"/>
+      <c r="G102" s="250"/>
+      <c r="H102" s="250"/>
+      <c r="I102" s="250"/>
+      <c r="J102" s="250"/>
+      <c r="K102" s="250"/>
+      <c r="L102" s="251"/>
     </row>
     <row r="103" spans="1:12" ht="15" customHeight="1">
       <c r="A103" s="13"/>
-      <c r="B103" s="215"/>
-      <c r="C103" s="216"/>
-      <c r="D103" s="216"/>
-      <c r="E103" s="216"/>
-      <c r="F103" s="216"/>
-      <c r="G103" s="216"/>
-      <c r="H103" s="216"/>
-      <c r="I103" s="216"/>
-      <c r="J103" s="216"/>
-      <c r="K103" s="216"/>
-      <c r="L103" s="217"/>
+      <c r="B103" s="249"/>
+      <c r="C103" s="250"/>
+      <c r="D103" s="250"/>
+      <c r="E103" s="250"/>
+      <c r="F103" s="250"/>
+      <c r="G103" s="250"/>
+      <c r="H103" s="250"/>
+      <c r="I103" s="250"/>
+      <c r="J103" s="250"/>
+      <c r="K103" s="250"/>
+      <c r="L103" s="251"/>
     </row>
     <row r="104" spans="1:12" ht="15" customHeight="1">
       <c r="A104" s="13"/>
-      <c r="B104" s="215"/>
-      <c r="C104" s="216"/>
-      <c r="D104" s="216"/>
-      <c r="E104" s="216"/>
-      <c r="F104" s="216"/>
-      <c r="G104" s="216"/>
-      <c r="H104" s="216"/>
-      <c r="I104" s="216"/>
-      <c r="J104" s="216"/>
-      <c r="K104" s="216"/>
-      <c r="L104" s="217"/>
+      <c r="B104" s="249"/>
+      <c r="C104" s="250"/>
+      <c r="D104" s="250"/>
+      <c r="E104" s="250"/>
+      <c r="F104" s="250"/>
+      <c r="G104" s="250"/>
+      <c r="H104" s="250"/>
+      <c r="I104" s="250"/>
+      <c r="J104" s="250"/>
+      <c r="K104" s="250"/>
+      <c r="L104" s="251"/>
     </row>
     <row r="105" spans="1:12" ht="15" customHeight="1">
       <c r="A105" s="13"/>
-      <c r="B105" s="215"/>
-      <c r="C105" s="216"/>
-      <c r="D105" s="216"/>
-      <c r="E105" s="216"/>
-      <c r="F105" s="216"/>
-      <c r="G105" s="216"/>
-      <c r="H105" s="216"/>
-      <c r="I105" s="216"/>
-      <c r="J105" s="216"/>
-      <c r="K105" s="216"/>
-      <c r="L105" s="217"/>
+      <c r="B105" s="249"/>
+      <c r="C105" s="250"/>
+      <c r="D105" s="250"/>
+      <c r="E105" s="250"/>
+      <c r="F105" s="250"/>
+      <c r="G105" s="250"/>
+      <c r="H105" s="250"/>
+      <c r="I105" s="250"/>
+      <c r="J105" s="250"/>
+      <c r="K105" s="250"/>
+      <c r="L105" s="251"/>
     </row>
     <row r="106" spans="1:12" ht="15" customHeight="1">
       <c r="A106" s="13"/>
-      <c r="B106" s="215"/>
-      <c r="C106" s="216"/>
-      <c r="D106" s="216"/>
-      <c r="E106" s="216"/>
-      <c r="F106" s="216"/>
-      <c r="G106" s="216"/>
-      <c r="H106" s="216"/>
-      <c r="I106" s="216"/>
-      <c r="J106" s="216"/>
-      <c r="K106" s="216"/>
-      <c r="L106" s="217"/>
+      <c r="B106" s="249"/>
+      <c r="C106" s="250"/>
+      <c r="D106" s="250"/>
+      <c r="E106" s="250"/>
+      <c r="F106" s="250"/>
+      <c r="G106" s="250"/>
+      <c r="H106" s="250"/>
+      <c r="I106" s="250"/>
+      <c r="J106" s="250"/>
+      <c r="K106" s="250"/>
+      <c r="L106" s="251"/>
     </row>
     <row r="107" spans="1:12" ht="15" customHeight="1">
       <c r="A107" s="13"/>
-      <c r="B107" s="218"/>
-      <c r="C107" s="219"/>
-      <c r="D107" s="219"/>
-      <c r="E107" s="219"/>
-      <c r="F107" s="219"/>
-      <c r="G107" s="219"/>
-      <c r="H107" s="219"/>
-      <c r="I107" s="219"/>
-      <c r="J107" s="219"/>
-      <c r="K107" s="219"/>
-      <c r="L107" s="220"/>
+      <c r="B107" s="252"/>
+      <c r="C107" s="253"/>
+      <c r="D107" s="253"/>
+      <c r="E107" s="253"/>
+      <c r="F107" s="253"/>
+      <c r="G107" s="253"/>
+      <c r="H107" s="253"/>
+      <c r="I107" s="253"/>
+      <c r="J107" s="253"/>
+      <c r="K107" s="253"/>
+      <c r="L107" s="254"/>
     </row>
     <row r="108" spans="1:12" ht="15" customHeight="1">
       <c r="A108" s="13"/>
@@ -32197,19 +32480,19 @@
       <c r="L108" s="20"/>
     </row>
     <row r="109" spans="1:12">
-      <c r="B109" s="192" t="s">
+      <c r="B109" s="184" t="s">
         <v>118</v>
       </c>
-      <c r="C109" s="193"/>
-      <c r="D109" s="193"/>
-      <c r="E109" s="193"/>
-      <c r="F109" s="193"/>
-      <c r="G109" s="193"/>
-      <c r="H109" s="193"/>
-      <c r="I109" s="193"/>
-      <c r="J109" s="193"/>
-      <c r="K109" s="193"/>
-      <c r="L109" s="193"/>
+      <c r="C109" s="185"/>
+      <c r="D109" s="185"/>
+      <c r="E109" s="185"/>
+      <c r="F109" s="185"/>
+      <c r="G109" s="185"/>
+      <c r="H109" s="185"/>
+      <c r="I109" s="185"/>
+      <c r="J109" s="185"/>
+      <c r="K109" s="185"/>
+      <c r="L109" s="185"/>
     </row>
     <row r="110" spans="1:12" ht="15" customHeight="1">
       <c r="A110" s="13"/>
@@ -32333,8 +32616,8 @@
     </row>
     <row r="118" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A118" s="13"/>
-      <c r="B118" s="221"/>
-      <c r="C118" s="222"/>
+      <c r="B118" s="255"/>
+      <c r="C118" s="256"/>
       <c r="D118" s="63"/>
       <c r="E118" s="63"/>
       <c r="F118" s="62"/>
@@ -32347,8 +32630,8 @@
     </row>
     <row r="119" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A119" s="13"/>
-      <c r="B119" s="221"/>
-      <c r="C119" s="222"/>
+      <c r="B119" s="255"/>
+      <c r="C119" s="256"/>
       <c r="D119" s="63"/>
       <c r="E119" s="63"/>
       <c r="F119" s="62"/>
@@ -35230,128 +35513,136 @@
       <c r="L262" s="27"/>
     </row>
     <row r="263" spans="1:12">
-      <c r="B263" s="192" t="s">
+      <c r="B263" s="184" t="s">
         <v>22</v>
       </c>
-      <c r="C263" s="193"/>
-      <c r="D263" s="193"/>
-      <c r="E263" s="193"/>
-      <c r="F263" s="193"/>
-      <c r="G263" s="193"/>
-      <c r="H263" s="193"/>
-      <c r="I263" s="193"/>
-      <c r="J263" s="193"/>
-      <c r="K263" s="193"/>
-      <c r="L263" s="193"/>
+      <c r="C263" s="185"/>
+      <c r="D263" s="185"/>
+      <c r="E263" s="185"/>
+      <c r="F263" s="185"/>
+      <c r="G263" s="185"/>
+      <c r="H263" s="185"/>
+      <c r="I263" s="185"/>
+      <c r="J263" s="185"/>
+      <c r="K263" s="185"/>
+      <c r="L263" s="185"/>
     </row>
     <row r="264" spans="1:12">
-      <c r="B264" s="183" t="s">
+      <c r="B264" s="219" t="s">
         <v>317</v>
       </c>
-      <c r="C264" s="184"/>
-      <c r="D264" s="184"/>
-      <c r="E264" s="184"/>
-      <c r="F264" s="184"/>
-      <c r="G264" s="184"/>
-      <c r="H264" s="184"/>
-      <c r="I264" s="184"/>
-      <c r="J264" s="184"/>
-      <c r="K264" s="184"/>
-      <c r="L264" s="185"/>
+      <c r="C264" s="220"/>
+      <c r="D264" s="220"/>
+      <c r="E264" s="220"/>
+      <c r="F264" s="220"/>
+      <c r="G264" s="220"/>
+      <c r="H264" s="220"/>
+      <c r="I264" s="220"/>
+      <c r="J264" s="220"/>
+      <c r="K264" s="220"/>
+      <c r="L264" s="221"/>
     </row>
     <row r="265" spans="1:12">
-      <c r="B265" s="186"/>
-      <c r="C265" s="187"/>
-      <c r="D265" s="187"/>
-      <c r="E265" s="187"/>
-      <c r="F265" s="187"/>
-      <c r="G265" s="187"/>
-      <c r="H265" s="187"/>
-      <c r="I265" s="187"/>
-      <c r="J265" s="187"/>
-      <c r="K265" s="187"/>
-      <c r="L265" s="188"/>
+      <c r="B265" s="222"/>
+      <c r="C265" s="223"/>
+      <c r="D265" s="223"/>
+      <c r="E265" s="223"/>
+      <c r="F265" s="223"/>
+      <c r="G265" s="223"/>
+      <c r="H265" s="223"/>
+      <c r="I265" s="223"/>
+      <c r="J265" s="223"/>
+      <c r="K265" s="223"/>
+      <c r="L265" s="224"/>
     </row>
     <row r="266" spans="1:12">
-      <c r="B266" s="186"/>
-      <c r="C266" s="187"/>
-      <c r="D266" s="187"/>
-      <c r="E266" s="187"/>
-      <c r="F266" s="187"/>
-      <c r="G266" s="187"/>
-      <c r="H266" s="187"/>
-      <c r="I266" s="187"/>
-      <c r="J266" s="187"/>
-      <c r="K266" s="187"/>
-      <c r="L266" s="188"/>
+      <c r="B266" s="222"/>
+      <c r="C266" s="223"/>
+      <c r="D266" s="223"/>
+      <c r="E266" s="223"/>
+      <c r="F266" s="223"/>
+      <c r="G266" s="223"/>
+      <c r="H266" s="223"/>
+      <c r="I266" s="223"/>
+      <c r="J266" s="223"/>
+      <c r="K266" s="223"/>
+      <c r="L266" s="224"/>
     </row>
     <row r="267" spans="1:12">
-      <c r="B267" s="186"/>
-      <c r="C267" s="187"/>
-      <c r="D267" s="187"/>
-      <c r="E267" s="187"/>
-      <c r="F267" s="187"/>
-      <c r="G267" s="187"/>
-      <c r="H267" s="187"/>
-      <c r="I267" s="187"/>
-      <c r="J267" s="187"/>
-      <c r="K267" s="187"/>
-      <c r="L267" s="188"/>
+      <c r="B267" s="222"/>
+      <c r="C267" s="223"/>
+      <c r="D267" s="223"/>
+      <c r="E267" s="223"/>
+      <c r="F267" s="223"/>
+      <c r="G267" s="223"/>
+      <c r="H267" s="223"/>
+      <c r="I267" s="223"/>
+      <c r="J267" s="223"/>
+      <c r="K267" s="223"/>
+      <c r="L267" s="224"/>
     </row>
     <row r="268" spans="1:12">
-      <c r="B268" s="186"/>
-      <c r="C268" s="187"/>
-      <c r="D268" s="187"/>
-      <c r="E268" s="187"/>
-      <c r="F268" s="187"/>
-      <c r="G268" s="187"/>
-      <c r="H268" s="187"/>
-      <c r="I268" s="187"/>
-      <c r="J268" s="187"/>
-      <c r="K268" s="187"/>
-      <c r="L268" s="188"/>
+      <c r="B268" s="222"/>
+      <c r="C268" s="223"/>
+      <c r="D268" s="223"/>
+      <c r="E268" s="223"/>
+      <c r="F268" s="223"/>
+      <c r="G268" s="223"/>
+      <c r="H268" s="223"/>
+      <c r="I268" s="223"/>
+      <c r="J268" s="223"/>
+      <c r="K268" s="223"/>
+      <c r="L268" s="224"/>
     </row>
     <row r="269" spans="1:12">
-      <c r="B269" s="186"/>
-      <c r="C269" s="187"/>
-      <c r="D269" s="187"/>
-      <c r="E269" s="187"/>
-      <c r="F269" s="187"/>
-      <c r="G269" s="187"/>
-      <c r="H269" s="187"/>
-      <c r="I269" s="187"/>
-      <c r="J269" s="187"/>
-      <c r="K269" s="187"/>
-      <c r="L269" s="188"/>
+      <c r="B269" s="222"/>
+      <c r="C269" s="223"/>
+      <c r="D269" s="223"/>
+      <c r="E269" s="223"/>
+      <c r="F269" s="223"/>
+      <c r="G269" s="223"/>
+      <c r="H269" s="223"/>
+      <c r="I269" s="223"/>
+      <c r="J269" s="223"/>
+      <c r="K269" s="223"/>
+      <c r="L269" s="224"/>
     </row>
     <row r="270" spans="1:12">
-      <c r="B270" s="186"/>
-      <c r="C270" s="187"/>
-      <c r="D270" s="187"/>
-      <c r="E270" s="187"/>
-      <c r="F270" s="187"/>
-      <c r="G270" s="187"/>
-      <c r="H270" s="187"/>
-      <c r="I270" s="187"/>
-      <c r="J270" s="187"/>
-      <c r="K270" s="187"/>
-      <c r="L270" s="188"/>
+      <c r="B270" s="222"/>
+      <c r="C270" s="223"/>
+      <c r="D270" s="223"/>
+      <c r="E270" s="223"/>
+      <c r="F270" s="223"/>
+      <c r="G270" s="223"/>
+      <c r="H270" s="223"/>
+      <c r="I270" s="223"/>
+      <c r="J270" s="223"/>
+      <c r="K270" s="223"/>
+      <c r="L270" s="224"/>
     </row>
     <row r="271" spans="1:12">
-      <c r="B271" s="189"/>
-      <c r="C271" s="190"/>
-      <c r="D271" s="190"/>
-      <c r="E271" s="190"/>
-      <c r="F271" s="190"/>
-      <c r="G271" s="190"/>
-      <c r="H271" s="190"/>
-      <c r="I271" s="190"/>
-      <c r="J271" s="190"/>
-      <c r="K271" s="190"/>
-      <c r="L271" s="191"/>
+      <c r="B271" s="225"/>
+      <c r="C271" s="226"/>
+      <c r="D271" s="226"/>
+      <c r="E271" s="226"/>
+      <c r="F271" s="226"/>
+      <c r="G271" s="226"/>
+      <c r="H271" s="226"/>
+      <c r="I271" s="226"/>
+      <c r="J271" s="226"/>
+      <c r="K271" s="226"/>
+      <c r="L271" s="227"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B16:L16"/>
+    <mergeCell ref="B17:L19"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B4:L4"/>
     <mergeCell ref="B264:L271"/>
     <mergeCell ref="B109:L109"/>
     <mergeCell ref="B7:I14"/>
@@ -35367,14 +35658,6 @@
     <mergeCell ref="K75:L75"/>
     <mergeCell ref="B263:L263"/>
     <mergeCell ref="B101:L107"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B17:L19"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B4:L4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Did a better job on last bonus
</commit_message>
<xml_diff>
--- a/AllsWellThatEndsExcel_Case_and_Answers.xlsx
+++ b/AllsWellThatEndsExcel_Case_and_Answers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29113"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592D41AD-A30D-4D8D-8464-ECF4EBC2C1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8527F6-038C-43F3-9071-B7E52ACDDC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{14CF381A-4175-4F53-B406-22934FD6CEB0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{14CF381A-4175-4F53-B406-22934FD6CEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="16" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="378">
   <si>
     <t>Harry Gross</t>
   </si>
@@ -11579,8 +11579,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6726002" y="25062196"/>
-          <a:ext cx="701364" cy="209696"/>
+          <a:off x="6752224" y="24916520"/>
+          <a:ext cx="699795" cy="205886"/>
           <a:chOff x="5262929" y="18783301"/>
           <a:chExt cx="663493" cy="205886"/>
         </a:xfrm>
@@ -11719,8 +11719,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6714582" y="25340487"/>
-          <a:ext cx="928119" cy="214865"/>
+          <a:off x="6735089" y="25192233"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -11859,8 +11859,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6724263" y="25636746"/>
-          <a:ext cx="726278" cy="216770"/>
+          <a:off x="6742865" y="25484010"/>
+          <a:ext cx="736139" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="698638" cy="211055"/>
         </a:xfrm>
@@ -11999,8 +11999,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6721022" y="25946052"/>
-          <a:ext cx="937644" cy="207245"/>
+          <a:off x="6747244" y="25785024"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -12139,8 +12139,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6723293" y="26243014"/>
-          <a:ext cx="689934" cy="200171"/>
+          <a:off x="6741895" y="26075598"/>
+          <a:ext cx="699795" cy="205886"/>
           <a:chOff x="5262929" y="18783301"/>
           <a:chExt cx="663493" cy="205886"/>
         </a:xfrm>
@@ -12279,8 +12279,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6728083" y="26498362"/>
-          <a:ext cx="930024" cy="207245"/>
+          <a:off x="6746685" y="26326464"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -12419,8 +12419,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6728239" y="26787001"/>
-          <a:ext cx="737708" cy="214865"/>
+          <a:off x="6754461" y="26618240"/>
+          <a:ext cx="736139" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="698638" cy="211055"/>
         </a:xfrm>
@@ -12559,8 +12559,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6734522" y="27109419"/>
-          <a:ext cx="939549" cy="207245"/>
+          <a:off x="6758839" y="26930461"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -12699,8 +12699,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6727268" y="27404476"/>
-          <a:ext cx="701364" cy="200171"/>
+          <a:off x="6753490" y="27221036"/>
+          <a:ext cx="699795" cy="205886"/>
           <a:chOff x="5262929" y="18783301"/>
           <a:chExt cx="663493" cy="205886"/>
         </a:xfrm>
@@ -15234,8 +15234,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6723641" y="21394205"/>
-          <a:ext cx="937644" cy="207245"/>
+          <a:off x="6749863" y="21300748"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -15374,8 +15374,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6725917" y="21886981"/>
-          <a:ext cx="930024" cy="216770"/>
+          <a:off x="6744519" y="21792515"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -15514,8 +15514,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6724159" y="22437371"/>
-          <a:ext cx="937644" cy="207245"/>
+          <a:off x="6750381" y="22332036"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -15654,8 +15654,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6721228" y="22742352"/>
-          <a:ext cx="937644" cy="207245"/>
+          <a:off x="6747450" y="22630629"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -15794,8 +15794,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6727089" y="23004543"/>
-          <a:ext cx="939549" cy="216770"/>
+          <a:off x="6753311" y="22894053"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -15934,8 +15934,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6725917" y="23312895"/>
-          <a:ext cx="930024" cy="207245"/>
+          <a:off x="6744519" y="23194112"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16074,8 +16074,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6724452" y="23612014"/>
-          <a:ext cx="930024" cy="205340"/>
+          <a:off x="6743054" y="23486844"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16214,8 +16214,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6722689" y="23907071"/>
-          <a:ext cx="699459" cy="200171"/>
+          <a:off x="6748911" y="23777418"/>
+          <a:ext cx="699795" cy="205886"/>
           <a:chOff x="5262929" y="18783301"/>
           <a:chExt cx="663493" cy="205886"/>
         </a:xfrm>
@@ -16354,8 +16354,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6732307" y="24206398"/>
-          <a:ext cx="937644" cy="216770"/>
+          <a:off x="6756624" y="24077979"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16494,8 +16494,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6721610" y="24514750"/>
-          <a:ext cx="937644" cy="207245"/>
+          <a:off x="6747832" y="24378039"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16634,8 +16634,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6727765" y="24813868"/>
-          <a:ext cx="930024" cy="209150"/>
+          <a:off x="6746367" y="24670769"/>
+          <a:ext cx="936075" cy="206573"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16774,8 +16774,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6726779" y="20905965"/>
-          <a:ext cx="930024" cy="207245"/>
+          <a:off x="6745381" y="20818896"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -16914,8 +16914,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6721434" y="22186962"/>
-          <a:ext cx="928119" cy="207245"/>
+          <a:off x="6740036" y="22086109"/>
+          <a:ext cx="936075" cy="211055"/>
           <a:chOff x="5262929" y="18778132"/>
           <a:chExt cx="899785" cy="211055"/>
         </a:xfrm>
@@ -18166,8 +18166,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5793262" y="1230390"/>
-          <a:ext cx="16326246" cy="14397387"/>
+          <a:off x="5763942" y="1243145"/>
+          <a:ext cx="16277958" cy="14444267"/>
           <a:chOff x="5611090" y="1281546"/>
           <a:chExt cx="15831149" cy="14356773"/>
         </a:xfrm>
@@ -18324,13 +18324,13 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>928689</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>1200149</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>250506</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -18374,13 +18374,13 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>866776</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>319087</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>1124901</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>95248</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -18424,14 +18424,14 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>257176</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>42863</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>1447801</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>169544</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>169545</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -18530,8 +18530,8 @@
           <xdr:rowOff>2747964</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>152400</xdr:colOff>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>4594656</xdr:rowOff>
         </xdr:to>
@@ -18548,7 +18548,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4479"/>
+                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4489"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -18599,7 +18599,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>25</xdr:col>
-          <xdr:colOff>475297</xdr:colOff>
+          <xdr:colOff>31952</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>4590846</xdr:rowOff>
         </xdr:to>
@@ -18616,7 +18616,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4480"/>
+                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4490"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -18660,13 +18660,13 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>71438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>628649</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>91441</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -18721,13 +18721,13 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>309564</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>666749</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>309564</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -18811,7 +18811,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>551496</xdr:colOff>
+      <xdr:colOff>108150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>2607421</xdr:rowOff>
     </xdr:to>
@@ -24343,8 +24343,8 @@
         <v>L24</v>
       </c>
       <c r="I239" s="27" cm="1">
-        <f t="array" aca="1" ref="I239" ca="1">SUM(_xlfn.XLOOKUP(_xlfn.TOCOL(OFFSET(INDIRECT("'Birnam Forest'!"&amp;H239),-2,-2,5,5)),'Birnam Forest'!$AK$7:$AK$13,'Birnam Forest'!AM7:$AM$13,0))</f>
-        <v>20</v>
+        <f t="array" aca="1" ref="I239" ca="1">SUM(_xlfn.XLOOKUP(_xlfn.TOCOL(OFFSET(INDIRECT("'Birnam Forest'!"&amp;H239),-2,-2,5,5)),'Birnam Forest'!$AK$8:$AK$14,'Birnam Forest'!AM8:$AM$14,0))</f>
+        <v>13</v>
       </c>
       <c r="J239" s="20"/>
       <c r="K239" s="27"/>
@@ -24359,7 +24359,7 @@
       <c r="F240" s="18"/>
       <c r="H240" s="26">
         <f ca="1">I239</f>
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I240" s="27"/>
       <c r="J240" s="29"/>
@@ -24389,7 +24389,7 @@
       </c>
       <c r="H241" s="27">
         <f t="dataTable" ref="H241:H260" dt2D="0" dtr="0" r1="H239" ca="1"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I241" s="27"/>
       <c r="J241" s="20"/>
@@ -24505,7 +24505,7 @@
         <v>293</v>
       </c>
       <c r="H245" s="27">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I245" s="27"/>
       <c r="J245" s="20"/>
@@ -24534,7 +24534,7 @@
         <v>294</v>
       </c>
       <c r="H246" s="27">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I246" s="27"/>
       <c r="J246" s="20"/>
@@ -24563,7 +24563,7 @@
         <v>295</v>
       </c>
       <c r="H247" s="27">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I247" s="27"/>
       <c r="J247" s="20"/>
@@ -24621,7 +24621,7 @@
         <v>297</v>
       </c>
       <c r="H249" s="27">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I249" s="27"/>
       <c r="J249" s="20"/>
@@ -24650,7 +24650,7 @@
         <v>298</v>
       </c>
       <c r="H250" s="27">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I250" s="27"/>
       <c r="J250" s="20"/>
@@ -24679,7 +24679,7 @@
         <v>299</v>
       </c>
       <c r="H251" s="27">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I251" s="27"/>
       <c r="J251" s="20"/>
@@ -24737,7 +24737,7 @@
         <v>301</v>
       </c>
       <c r="H253" s="27">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I253" s="27"/>
       <c r="J253" s="20"/>
@@ -24795,7 +24795,7 @@
         <v>303</v>
       </c>
       <c r="H255" s="27">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I255" s="27"/>
       <c r="J255" s="20"/>
@@ -24824,7 +24824,7 @@
         <v>304</v>
       </c>
       <c r="H256" s="27">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I256" s="27"/>
       <c r="J256" s="20"/>
@@ -24853,7 +24853,7 @@
         <v>305</v>
       </c>
       <c r="H257" s="27">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I257" s="27"/>
       <c r="J257" s="20"/>
@@ -24882,7 +24882,7 @@
         <v>306</v>
       </c>
       <c r="H258" s="27">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I258" s="27"/>
       <c r="J258" s="20"/>
@@ -24940,7 +24940,7 @@
         <v>308</v>
       </c>
       <c r="H260" s="27">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I260" s="27"/>
       <c r="J260" s="20"/>
@@ -28137,20 +28137,28 @@
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AN40"/>
+  <dimension ref="A1:AN41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6:AH12"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="25.2" zeroHeight="1"/>
   <cols>
     <col min="1" max="1" width="6" style="138" customWidth="1"/>
-    <col min="2" max="10" width="9.88671875" style="138" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="138" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="138" customWidth="1"/>
+    <col min="4" max="5" width="9.88671875" style="138" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="138" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="138" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="138" customWidth="1"/>
+    <col min="9" max="10" width="9.88671875" style="138" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.88671875" style="138" customWidth="1"/>
     <col min="13" max="13" width="18.77734375" style="138" customWidth="1"/>
     <col min="14" max="17" width="9.88671875" style="138" customWidth="1"/>
-    <col min="18" max="25" width="9.88671875" style="138" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" style="138" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.33203125" style="138" customWidth="1"/>
+    <col min="20" max="25" width="9.88671875" style="138" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14.5546875" style="138" bestFit="1" customWidth="1"/>
     <col min="27" max="34" width="9.88671875" style="138" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="6" style="138" customWidth="1"/>
@@ -28206,93 +28214,34 @@
       <c r="AN1" s="152"/>
     </row>
     <row r="2" spans="1:40">
-      <c r="A2" s="140" cm="1">
-        <f t="array" ref="A2:G2">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(M$14:M$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(M$14:M$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>7</v>
-      </c>
-      <c r="B2" s="140">
-        <v>6</v>
-      </c>
-      <c r="C2" s="151">
-        <v>8</v>
-      </c>
-      <c r="D2" s="151">
-        <v>9</v>
-      </c>
-      <c r="E2" s="151">
-        <v>12</v>
-      </c>
-      <c r="F2" s="151">
-        <v>11</v>
-      </c>
-      <c r="G2" s="151">
-        <v>10</v>
-      </c>
+      <c r="A2" s="140"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
       <c r="H2" s="151"/>
-      <c r="I2" s="140" cm="1">
-        <f t="array" ref="I2:O2">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(Q$14:Q$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(Q$14:Q$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>7</v>
-      </c>
-      <c r="J2" s="151">
-        <v>6</v>
-      </c>
-      <c r="K2" s="151">
-        <v>8</v>
-      </c>
-      <c r="L2" s="151">
-        <v>9</v>
-      </c>
-      <c r="M2" s="138">
-        <v>12</v>
-      </c>
-      <c r="N2" s="138">
-        <v>11</v>
-      </c>
-      <c r="O2" s="138">
-        <v>10</v>
-      </c>
-      <c r="P2" s="140" cm="1">
-        <f t="array" ref="P2">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(P$14:P$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(P$14:P$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>11</v>
-      </c>
+      <c r="I2" s="140"/>
+      <c r="J2" s="151"/>
+      <c r="K2" s="151"/>
+      <c r="L2" s="151"/>
+      <c r="P2" s="140"/>
       <c r="T2" s="151"/>
-      <c r="U2" s="140" cm="1">
-        <f t="array" ref="U2:V2">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(U$14:U$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(U$14:U$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>6</v>
-      </c>
-      <c r="V2" s="151">
-        <v>12</v>
-      </c>
+      <c r="U2" s="140"/>
+      <c r="V2" s="151"/>
       <c r="W2" s="151"/>
       <c r="X2" s="151"/>
-      <c r="Y2" s="140" cm="1">
-        <f t="array" ref="Y2:AD2">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(Y$14:Y$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(Y$14:Y$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>7</v>
-      </c>
-      <c r="Z2" s="151">
-        <v>6</v>
-      </c>
-      <c r="AA2" s="151">
-        <v>11</v>
-      </c>
-      <c r="AB2" s="151">
-        <v>9</v>
-      </c>
-      <c r="AC2" s="151">
-        <v>8</v>
-      </c>
-      <c r="AD2" s="151">
-        <v>10</v>
-      </c>
+      <c r="Y2" s="140"/>
+      <c r="Z2" s="151"/>
+      <c r="AA2" s="151"/>
+      <c r="AB2" s="151"/>
+      <c r="AC2" s="151"/>
+      <c r="AD2" s="151"/>
       <c r="AE2" s="151"/>
       <c r="AF2" s="151"/>
-      <c r="AG2" s="140" cm="1">
-        <f t="array" ref="AG2:AH2">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW($AG$14:$AG$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP($AG$14:$AG$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>8</v>
-      </c>
-      <c r="AH2" s="151">
-        <v>10</v>
-      </c>
+      <c r="AG2" s="140"/>
+      <c r="AH2" s="151"/>
       <c r="AI2" s="151"/>
       <c r="AJ2" s="151"/>
       <c r="AK2" s="151"/>
@@ -28302,84 +28251,40 @@
     </row>
     <row r="3" spans="1:40">
       <c r="A3" s="151"/>
-      <c r="B3" s="140" cm="1">
-        <f t="array" ref="B3">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(N$14:N$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(N$14:N$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>11</v>
-      </c>
+      <c r="B3" s="140"/>
       <c r="C3" s="151"/>
       <c r="D3" s="151"/>
       <c r="E3" s="151"/>
       <c r="F3" s="151"/>
       <c r="G3" s="151"/>
       <c r="H3" s="151"/>
-      <c r="I3" s="140" cm="1">
-        <f t="array" ref="I3:M3">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(S$14:S$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(S$14:S$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>7</v>
-      </c>
-      <c r="J3" s="151">
-        <v>8</v>
-      </c>
-      <c r="K3" s="151">
-        <v>9</v>
-      </c>
-      <c r="L3" s="151">
-        <v>11</v>
-      </c>
-      <c r="M3" s="151">
-        <v>10</v>
-      </c>
+      <c r="I3" s="140"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="151"/>
+      <c r="L3" s="151"/>
+      <c r="M3" s="151"/>
       <c r="O3" s="140"/>
       <c r="P3" s="151"/>
       <c r="Q3" s="151"/>
       <c r="R3" s="151"/>
       <c r="S3" s="151"/>
       <c r="T3" s="151"/>
-      <c r="U3" s="140" cm="1">
-        <f t="array" ref="U3:V3">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(V$14:V$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(V$14:V$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>12</v>
-      </c>
-      <c r="V3" s="151">
-        <v>6</v>
-      </c>
+      <c r="U3" s="140"/>
+      <c r="V3" s="151"/>
       <c r="W3" s="151"/>
       <c r="X3" s="151"/>
-      <c r="Y3" s="140" cm="1">
-        <f t="array" ref="Y3">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(Z$14:Z$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(Z$14:Z$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>12</v>
-      </c>
-      <c r="Z3" s="140" cm="1">
-        <f t="array" ref="Z3:AE3">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(AC$14:AC$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(AC$14:AC$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>6</v>
-      </c>
-      <c r="AA3" s="151">
-        <v>10</v>
-      </c>
-      <c r="AB3" s="151">
-        <v>7</v>
-      </c>
-      <c r="AC3" s="151">
-        <v>9</v>
-      </c>
-      <c r="AD3" s="151">
-        <v>8</v>
-      </c>
-      <c r="AE3" s="151">
-        <v>11</v>
-      </c>
+      <c r="Y3" s="140"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="151"/>
+      <c r="AB3" s="151"/>
+      <c r="AC3" s="151"/>
+      <c r="AD3" s="151"/>
+      <c r="AE3" s="151"/>
       <c r="AF3" s="151"/>
-      <c r="AG3" s="140" cm="1">
-        <f t="array" ref="AG3:AJ3">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW($AH$14:$AH$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP($AH$14:$AH$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>6</v>
-      </c>
-      <c r="AH3" s="151">
-        <v>7</v>
-      </c>
-      <c r="AI3" s="151">
-        <v>11</v>
-      </c>
-      <c r="AJ3" s="151">
-        <v>12</v>
-      </c>
+      <c r="AG3" s="140"/>
+      <c r="AH3" s="151"/>
+      <c r="AI3" s="151"/>
+      <c r="AJ3" s="151"/>
       <c r="AK3" s="151"/>
       <c r="AL3" s="151"/>
       <c r="AM3" s="151"/>
@@ -28388,22 +28293,14 @@
     <row r="4" spans="1:40">
       <c r="A4" s="151"/>
       <c r="B4" s="151"/>
-      <c r="C4" s="140" cm="1">
-        <f t="array" ref="C4">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(O$14:O$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(O$14:O$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>10</v>
-      </c>
+      <c r="C4" s="140"/>
       <c r="D4" s="151"/>
       <c r="E4" s="151"/>
       <c r="F4" s="151"/>
       <c r="G4" s="151"/>
       <c r="H4" s="151"/>
-      <c r="I4" s="140" cm="1">
-        <f t="array" ref="I4:J4">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(T$14:T$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(T$14:T$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>6</v>
-      </c>
-      <c r="J4" s="151">
-        <v>12</v>
-      </c>
+      <c r="I4" s="140"/>
+      <c r="J4" s="151"/>
       <c r="K4" s="151"/>
       <c r="L4" s="151"/>
       <c r="M4" s="151"/>
@@ -28417,32 +28314,14 @@
       <c r="V4" s="151"/>
       <c r="W4" s="151"/>
       <c r="X4" s="151"/>
-      <c r="Y4" s="140" cm="1">
-        <f t="array" ref="Y4">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(AA$14:AA$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(AA$14:AA$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>12</v>
-      </c>
-      <c r="Z4" s="140" cm="1">
-        <f t="array" ref="Z4:AF4">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(AE$14:AE$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(AE$14:AE$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>6</v>
-      </c>
-      <c r="AA4" s="151">
-        <v>12</v>
-      </c>
-      <c r="AB4" s="151">
-        <v>8</v>
-      </c>
-      <c r="AC4" s="151">
-        <v>11</v>
-      </c>
-      <c r="AD4" s="151">
-        <v>10</v>
-      </c>
-      <c r="AE4" s="151">
-        <v>7</v>
-      </c>
-      <c r="AF4" s="151">
-        <v>9</v>
-      </c>
+      <c r="Y4" s="140"/>
+      <c r="Z4" s="140"/>
+      <c r="AA4" s="151"/>
+      <c r="AB4" s="151"/>
+      <c r="AC4" s="151"/>
+      <c r="AD4" s="151"/>
+      <c r="AE4" s="151"/>
+      <c r="AF4" s="151"/>
       <c r="AG4" s="151"/>
       <c r="AH4" s="151"/>
       <c r="AI4" s="151"/>
@@ -28453,7 +28332,7 @@
       <c r="AN4" s="151"/>
     </row>
     <row r="5" spans="1:40">
-      <c r="B5" s="140"/>
+      <c r="B5" s="169"/>
       <c r="C5" s="140"/>
       <c r="D5" s="140"/>
       <c r="E5" s="140"/>
@@ -28476,12 +28355,12 @@
       <c r="W5" s="140"/>
       <c r="X5" s="140"/>
       <c r="Y5" s="140" cm="1">
-        <f t="array" ref="Y5">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(AB$14:AB$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(AB$14:AB$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>12</v>
+        <f t="array" ref="Y5">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(AB$15:AB$36))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(AB$15:AB$36,$AK$8:$AK$14,$AM$8:$AM$14,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
+        <v>13</v>
       </c>
       <c r="Z5" s="140" cm="1">
-        <f t="array" ref="Z5">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(AF$14:AF$35))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(AF$14:AF$35,$AK$7:$AK$13,$AM$7:$AM$13,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>9</v>
+        <f t="array" ref="Z5">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(AF$15:AF$36))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(AF$15:AF$36,$AK$8:$AK$14,$AM$8:$AM$14,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
+        <v>10</v>
       </c>
       <c r="AA5" s="140"/>
       <c r="AB5" s="140"/>
@@ -28496,920 +28375,1027 @@
       <c r="AM5" s="168"/>
       <c r="AN5" s="168"/>
     </row>
-    <row r="6" spans="1:40" ht="25.8">
-      <c r="B6" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="C6" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="D6" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="E6" s="140" t="s">
-        <v>271</v>
-      </c>
+    <row r="6" spans="1:40">
+      <c r="B6" s="169"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
       <c r="F6" s="140"/>
-      <c r="G6" s="140" t="s">
-        <v>272</v>
-      </c>
+      <c r="G6" s="140"/>
       <c r="H6" s="140"/>
       <c r="I6" s="140"/>
       <c r="J6" s="140"/>
-      <c r="K6" s="140" t="s">
-        <v>272</v>
-      </c>
+      <c r="K6" s="140"/>
       <c r="L6" s="140"/>
-      <c r="M6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($A$2),ROW()),"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="N6" s="138" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($B$3),ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="O6" s="140" t="str">
-        <f>IF(COUNTIFS($C$4,ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="P6" s="140" t="str">
-        <f>IF(COUNTIFS($P$2,ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="Q6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($I$2),ROW()),"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="S6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($I$3),ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="T6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($I$4),ROW()),"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="U6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($U$2),ROW()),"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="V6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($U$3),ROW()),"*","")</f>
-        <v>*</v>
-      </c>
+      <c r="N6" s="140"/>
+      <c r="O6" s="140"/>
+      <c r="P6" s="140"/>
+      <c r="Q6" s="140"/>
+      <c r="R6" s="140"/>
+      <c r="S6" s="140"/>
+      <c r="T6" s="140"/>
+      <c r="U6" s="140"/>
+      <c r="V6" s="140"/>
       <c r="W6" s="140"/>
       <c r="X6" s="140"/>
-      <c r="Y6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($Y$2),ROW()),"*","")</f>
+      <c r="Y6" s="140"/>
+      <c r="Z6" s="140"/>
+      <c r="AA6" s="140"/>
+      <c r="AB6" s="140"/>
+      <c r="AC6" s="140"/>
+      <c r="AD6" s="140"/>
+      <c r="AE6" s="140"/>
+      <c r="AF6" s="140"/>
+      <c r="AG6" s="140"/>
+      <c r="AH6" s="140"/>
+      <c r="AK6" s="168"/>
+      <c r="AL6" s="168"/>
+      <c r="AM6" s="168"/>
+      <c r="AN6" s="168"/>
+    </row>
+    <row r="7" spans="1:40" ht="25.8">
+      <c r="B7" s="140" t="str" cm="1">
+        <f t="array" ref="B7:B13">_xlfn.LET(_xlpm.grd,B15:B36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     _xlpm.z)</f>
         <v>*</v>
       </c>
-      <c r="Z6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($Y$3),ROW()),"*","")</f>
+      <c r="C7" s="140" t="str" cm="1">
+        <f t="array" ref="C7:C13">_xlfn.LET(_xlpm.grd,C15:C36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     _xlpm.z)</f>
+        <v>*</v>
+      </c>
+      <c r="D7" s="140" t="str" cm="1">
+        <f t="array" ref="D7:D13">_xlfn.LET(_xlpm.grd,D15:D36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     _xlpm.z)</f>
+        <v>*</v>
+      </c>
+      <c r="E7" s="140" t="str" cm="1">
+        <f t="array" ref="E7:E13">_xlfn.LET(_xlpm.grd,E15:E36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     _xlpm.z)</f>
+        <v>*</v>
+      </c>
+      <c r="F7" s="140" t="str" cm="1">
+        <f t="array" ref="F7">_xlfn.LET(_xlpm.grd,F15:F36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
         <v/>
       </c>
-      <c r="AA6" s="140" t="str">
-        <f>IF(COUNTIFS($Y$4,ROW()),"*","")</f>
+      <c r="G7" s="140" t="str" cm="1">
+        <f t="array" ref="G7:G13">_xlfn.LET(_xlpm.grd,G15:G36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v>*</v>
+      </c>
+      <c r="H7" s="140" t="str" cm="1">
+        <f t="array" ref="H7:H13">_xlfn.LET(_xlpm.grd,H15:H36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
         <v/>
       </c>
-      <c r="AB6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($Y$5),ROW()),"*","")</f>
+      <c r="I7" s="140" t="str" cm="1">
+        <f t="array" ref="I7:I13">_xlfn.LET(_xlpm.grd,I15:I36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
         <v/>
       </c>
-      <c r="AC6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($Z$3),ROW()),"*","")</f>
+      <c r="J7" s="140" t="str" cm="1">
+        <f t="array" ref="J7:J13">_xlfn.LET(_xlpm.grd,J15:J36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="K7" s="140" t="str" cm="1">
+        <f t="array" ref="K7:K13">_xlfn.LET(_xlpm.grd,K15:K36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
         <v>*</v>
       </c>
-      <c r="AD6" s="140"/>
-      <c r="AE6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($Z$4),ROW()),"*","")</f>
+      <c r="L7" s="140" t="str" cm="1">
+        <f t="array" ref="L7">_xlfn.LET(_xlpm.grd,L15:L36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="M7" s="140" t="str" cm="1">
+        <f t="array" ref="M7:M13">_xlfn.LET(_xlpm.grd,M15:M36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
         <v>*</v>
       </c>
-      <c r="AF6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($Z$5),ROW()),"*","")</f>
+      <c r="N7" s="140" t="str" cm="1">
+        <f t="array" ref="N7:N13">_xlfn.LET(_xlpm.grd,N15:N36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
         <v/>
       </c>
-      <c r="AG6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($AG$2),ROW()),"*","")</f>
+      <c r="O7" s="140" t="str" cm="1">
+        <f t="array" ref="O7:O13">_xlfn.LET(_xlpm.grd,O15:O36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
         <v/>
       </c>
-      <c r="AH6" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($AG$3),ROW()),"*","")</f>
+      <c r="P7" s="140" t="str" cm="1">
+        <f t="array" ref="P7:P13">_xlfn.LET(_xlpm.grd,P15:P36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="Q7" s="140" t="str" cm="1">
+        <f t="array" ref="Q7:Q13">_xlfn.LET(_xlpm.grd,Q15:Q36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
         <v>*</v>
       </c>
-      <c r="AK6" s="164" t="s">
+      <c r="R7" s="140" t="str" cm="1">
+        <f t="array" ref="R7">_xlfn.LET(_xlpm.grd,R15:R36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="S7" s="140" t="str" cm="1">
+        <f t="array" ref="S7:S13">_xlfn.LET(_xlpm.grd,S15:S36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="T7" s="140" t="str" cm="1">
+        <f t="array" ref="T7:T13">_xlfn.LET(_xlpm.grd,T15:T36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v>*</v>
+      </c>
+      <c r="U7" s="140" t="str" cm="1">
+        <f t="array" ref="U7:U13">_xlfn.LET(_xlpm.grd,U15:U36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v>*</v>
+      </c>
+      <c r="V7" s="140" t="str" cm="1">
+        <f t="array" ref="V7:V13">_xlfn.LET(_xlpm.grd,V15:V36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v>*</v>
+      </c>
+      <c r="W7" s="140" t="str" cm="1">
+        <f t="array" ref="W7">_xlfn.LET(_xlpm.grd,W15:W36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="X7" s="140" t="str" cm="1">
+        <f t="array" ref="X7">_xlfn.LET(_xlpm.grd,X15:X36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="Y7" s="140" t="str" cm="1">
+        <f t="array" ref="Y7:Y13">_xlfn.LET(_xlpm.grd,Y15:Y36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v>*</v>
+      </c>
+      <c r="Z7" s="140" t="str" cm="1">
+        <f t="array" ref="Z7:Z13">_xlfn.LET(_xlpm.grd,Z15:Z36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="AA7" s="140" t="str" cm="1">
+        <f t="array" ref="AA7:AA13">_xlfn.LET(_xlpm.grd,AA15:AA36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="AB7" s="140" t="str" cm="1">
+        <f t="array" ref="AB7:AB13">_xlfn.LET(_xlpm.grd,AB15:AB36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="AC7" s="140" t="str" cm="1">
+        <f t="array" ref="AC7:AC13">_xlfn.LET(_xlpm.grd,AC15:AC36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v>*</v>
+      </c>
+      <c r="AD7" s="140" t="str" cm="1">
+        <f t="array" ref="AD7">_xlfn.LET(_xlpm.grd,AD15:AD36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="AE7" s="140" t="str" cm="1">
+        <f t="array" ref="AE7:AE13">_xlfn.LET(_xlpm.grd,AE15:AE36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v>*</v>
+      </c>
+      <c r="AF7" s="140" t="str" cm="1">
+        <f t="array" ref="AF7:AF13">_xlfn.LET(_xlpm.grd,AF15:AF36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="AG7" s="140" t="str" cm="1">
+        <f t="array" ref="AG7:AG13">_xlfn.LET(_xlpm.grd,AG15:AG36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v/>
+      </c>
+      <c r="AH7" s="140" t="str" cm="1">
+        <f t="array" ref="AH7:AH13">_xlfn.LET(_xlpm.grd,AH15:AH36,
+     _xlpm.chr,_xlfn.XLOOKUP(_xlpm.grd,$AK$8:$AK$14,$AM$8:$AM$14,NA()),
+     _xlpm.off,TRANSPOSE(ROW(_xlpm.grd))-3*TRANSPOSE(_xlpm.chr),
+     _xlpm.of,_xlfn._xlws.FILTER(_xlpm.off,ISNUMBER(_xlpm.off))-6,
+     _xlpm.z,TRANSPOSE(_xlfn.DROP(_xlfn.REDUCE("0",_xlfn.SEQUENCE(7),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,IF(OR(_xlpm.v=_xlpm.of),"*","")))),,1)),
+     IFERROR(_xlpm.z,""))</f>
+        <v>*</v>
+      </c>
+      <c r="AK7" s="164" t="s">
         <v>281</v>
       </c>
-      <c r="AL6" s="164" t="s">
+      <c r="AL7" s="164" t="s">
         <v>32</v>
       </c>
-      <c r="AM6" s="164" t="s">
+      <c r="AM7" s="164" t="s">
         <v>280</v>
       </c>
-      <c r="AN6" s="168"/>
-    </row>
-    <row r="7" spans="1:40">
-      <c r="B7" s="140" t="s">
-        <v>272</v>
-      </c>
-      <c r="C7" s="140"/>
-      <c r="D7" s="140"/>
-      <c r="F7" s="140"/>
-      <c r="G7" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="H7" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="I7" s="140"/>
-      <c r="J7" s="140" t="s">
-        <v>268</v>
-      </c>
-      <c r="K7" s="140" t="s">
-        <v>267</v>
-      </c>
-      <c r="L7" s="140"/>
-      <c r="M7" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($A$2),ROW()),"*","")</f>
+      <c r="AN7" s="168"/>
+    </row>
+    <row r="8" spans="1:40">
+      <c r="B8" s="140" t="str">
         <v>*</v>
       </c>
-      <c r="N7" s="138" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($B$3),ROW()),"*","")</f>
+      <c r="C8" s="140" t="str">
         <v/>
       </c>
-      <c r="O7" s="140" t="str">
-        <f>IF(COUNTIFS($C$4,ROW()),"*","")</f>
+      <c r="D8" s="140" t="str">
         <v/>
       </c>
-      <c r="P7" s="140" t="str">
-        <f t="shared" ref="P7:P11" si="0">IF(COUNTIFS($P$2,ROW()),"*","")</f>
+      <c r="E8" s="138" t="str">
         <v/>
       </c>
-      <c r="Q7" s="140" t="str">
-        <f t="shared" ref="Q7:Q12" si="1">IF(COUNTIFS(_xlfn.ANCHORARRAY($I$2),ROW()),"*","")</f>
+      <c r="F8" s="140"/>
+      <c r="G8" s="140" t="str">
         <v>*</v>
       </c>
-      <c r="R7" s="140"/>
-      <c r="S7" s="140" t="str">
-        <f t="shared" ref="S7:S12" si="2">IF(COUNTIFS(_xlfn.ANCHORARRAY($I$3),ROW()),"*","")</f>
+      <c r="H8" s="140" t="str">
         <v>*</v>
       </c>
-      <c r="T7" s="140" t="str">
-        <f t="shared" ref="T7:T12" si="3">IF(COUNTIFS(_xlfn.ANCHORARRAY($I$4),ROW()),"*","")</f>
+      <c r="I8" s="140" t="str">
         <v/>
       </c>
-      <c r="U7" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($U$2),ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="V7" s="140" t="str">
-        <f t="shared" ref="V7:V12" si="4">IF(COUNTIFS(_xlfn.ANCHORARRAY($U$3),ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="W7" s="140"/>
-      <c r="X7" s="140"/>
-      <c r="Y7" s="140" t="str">
-        <f t="shared" ref="Y7:Y11" si="5">IF(COUNTIFS(_xlfn.ANCHORARRAY($Y$2),ROW()),"*","")</f>
+      <c r="J8" s="140" t="str">
         <v>*</v>
       </c>
-      <c r="Z7" s="140" t="str">
-        <f t="shared" ref="Z7:Z12" si="6">IF(COUNTIFS(_xlfn.ANCHORARRAY($Y$3),ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="AA7" s="140" t="str">
-        <f t="shared" ref="AA7:AA12" si="7">IF(COUNTIFS($Y$4,ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="AB7" s="140" t="str">
-        <f t="shared" ref="AB7:AB12" si="8">IF(COUNTIFS(_xlfn.ANCHORARRAY($Y$5),ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="AC7" s="140" t="str">
-        <f t="shared" ref="AC7:AC12" si="9">IF(COUNTIFS(_xlfn.ANCHORARRAY($Z$3),ROW()),"*","")</f>
+      <c r="K8" s="140" t="str">
         <v>*</v>
-      </c>
-      <c r="AD7" s="140"/>
-      <c r="AE7" s="140" t="str">
-        <f t="shared" ref="AE7:AE12" si="10">IF(COUNTIFS(_xlfn.ANCHORARRAY($Z$4),ROW()),"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="AF7" s="140" t="str">
-        <f t="shared" ref="AF7:AF12" si="11">IF(COUNTIFS(_xlfn.ANCHORARRAY($Z$5),ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="AG7" s="140" t="str">
-        <f t="shared" ref="AG7:AG12" si="12">IF(COUNTIFS(_xlfn.ANCHORARRAY($AG$2),ROW()),"*","")</f>
-        <v/>
-      </c>
-      <c r="AH7" s="140" t="str">
-        <f t="shared" ref="AH7:AH12" si="13">IF(COUNTIFS(_xlfn.ANCHORARRAY($AG$3),ROW()),"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="AK7" s="150" t="s">
-        <v>272</v>
-      </c>
-      <c r="AL7" s="149" t="s">
-        <v>279</v>
-      </c>
-      <c r="AM7" s="148">
-        <v>3</v>
-      </c>
-      <c r="AN7" s="168"/>
-    </row>
-    <row r="8" spans="1:40">
-      <c r="B8" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="C8" s="140"/>
-      <c r="D8" s="140"/>
-      <c r="E8" s="140"/>
-      <c r="F8" s="140"/>
-      <c r="G8" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="I8" s="140" t="s">
-        <v>266</v>
-      </c>
-      <c r="J8" s="140"/>
-      <c r="K8" s="140" t="s">
-        <v>270</v>
       </c>
       <c r="L8" s="140"/>
       <c r="M8" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($A$2),ROW()),"*","")</f>
         <v>*</v>
       </c>
-      <c r="N8" s="138" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($B$3),ROW()),"*","")</f>
+      <c r="N8" s="140" t="str">
         <v/>
       </c>
       <c r="O8" s="140" t="str">
-        <f>IF(COUNTIFS($C$4,ROW()),"*","")</f>
         <v/>
       </c>
       <c r="P8" s="140" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q8" s="140" t="str">
-        <f t="shared" si="1"/>
         <v>*</v>
       </c>
       <c r="R8" s="140"/>
       <c r="S8" s="140" t="str">
-        <f t="shared" si="2"/>
         <v>*</v>
       </c>
       <c r="T8" s="140" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="U8" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($U$2),ROW()),"*","")</f>
         <v/>
       </c>
       <c r="V8" s="140" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W8" s="140"/>
       <c r="X8" s="140"/>
       <c r="Y8" s="140" t="str">
-        <f t="shared" si="5"/>
         <v>*</v>
       </c>
       <c r="Z8" s="140" t="str">
-        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AA8" s="140" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB8" s="140" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AC8" s="140" t="str">
-        <f t="shared" si="9"/>
         <v>*</v>
       </c>
       <c r="AD8" s="140"/>
       <c r="AE8" s="140" t="str">
-        <f t="shared" si="10"/>
         <v>*</v>
       </c>
       <c r="AF8" s="140" t="str">
-        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AG8" s="140" t="str">
-        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="AH8" s="140" t="str">
         <v>*</v>
       </c>
-      <c r="AH8" s="140" t="str">
-        <f t="shared" si="13"/>
+      <c r="AK8" s="150" t="s">
+        <v>272</v>
+      </c>
+      <c r="AL8" s="149" t="s">
+        <v>279</v>
+      </c>
+      <c r="AM8" s="148">
+        <v>3</v>
+      </c>
+      <c r="AN8" s="168"/>
+    </row>
+    <row r="9" spans="1:40">
+      <c r="B9" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="C9" s="140" t="str">
         <v/>
       </c>
-      <c r="AK8" s="147" t="s">
-        <v>271</v>
-      </c>
-      <c r="AL8" s="146" t="s">
-        <v>278</v>
-      </c>
-      <c r="AM8" s="145">
-        <v>4</v>
-      </c>
-      <c r="AN8" s="168"/>
-    </row>
-    <row r="9" spans="1:40">
-      <c r="B9" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="C9" s="140" t="s">
-        <v>268</v>
-      </c>
-      <c r="D9" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="E9" s="140"/>
+      <c r="D9" s="140" t="str">
+        <v/>
+      </c>
+      <c r="E9" s="140" t="str">
+        <v/>
+      </c>
       <c r="F9" s="140"/>
-      <c r="G9" s="138" t="s">
-        <v>268</v>
-      </c>
-      <c r="H9" s="140"/>
-      <c r="I9" s="140"/>
-      <c r="J9" s="140"/>
-      <c r="K9" s="140" t="s">
-        <v>267</v>
+      <c r="G9" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="H9" s="140" t="str">
+        <v/>
+      </c>
+      <c r="I9" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="J9" s="140" t="str">
+        <v/>
+      </c>
+      <c r="K9" s="140" t="str">
+        <v>*</v>
       </c>
       <c r="L9" s="140"/>
       <c r="M9" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($A$2),ROW()),"*","")</f>
         <v>*</v>
       </c>
-      <c r="N9" s="138" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($B$3),ROW()),"*","")</f>
+      <c r="N9" s="140" t="str">
         <v/>
       </c>
       <c r="O9" s="140" t="str">
-        <f>IF(COUNTIFS($C$4,ROW()),"*","")</f>
         <v/>
       </c>
       <c r="P9" s="140" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q9" s="140" t="str">
-        <f t="shared" si="1"/>
         <v>*</v>
       </c>
       <c r="R9" s="140"/>
       <c r="S9" s="140" t="str">
-        <f t="shared" si="2"/>
         <v>*</v>
       </c>
       <c r="T9" s="140" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="U9" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($U$2),ROW()),"*","")</f>
         <v/>
       </c>
       <c r="V9" s="140" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W9" s="140"/>
       <c r="X9" s="140"/>
       <c r="Y9" s="140" t="str">
-        <f t="shared" si="5"/>
         <v>*</v>
       </c>
       <c r="Z9" s="140" t="str">
-        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AA9" s="140" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB9" s="140" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AC9" s="140" t="str">
-        <f t="shared" si="9"/>
         <v>*</v>
       </c>
       <c r="AD9" s="140"/>
       <c r="AE9" s="140" t="str">
-        <f t="shared" si="10"/>
         <v>*</v>
       </c>
       <c r="AF9" s="140" t="str">
-        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AG9" s="140" t="str">
         <v>*</v>
       </c>
-      <c r="AG9" s="140" t="str">
-        <f t="shared" si="12"/>
+      <c r="AH9" s="140" t="str">
         <v/>
       </c>
-      <c r="AH9" s="140" t="str">
-        <f t="shared" si="13"/>
+      <c r="AK9" s="147" t="s">
+        <v>271</v>
+      </c>
+      <c r="AL9" s="146" t="s">
+        <v>278</v>
+      </c>
+      <c r="AM9" s="145">
+        <v>4</v>
+      </c>
+      <c r="AN9" s="168"/>
+    </row>
+    <row r="10" spans="1:40">
+      <c r="B10" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="C10" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="D10" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="E10" s="140" t="str">
         <v/>
       </c>
-      <c r="AK9" s="147" t="s">
-        <v>270</v>
-      </c>
-      <c r="AL9" s="146" t="s">
-        <v>277</v>
-      </c>
-      <c r="AM9" s="145">
-        <v>5</v>
-      </c>
-      <c r="AN9" s="168"/>
-    </row>
-    <row r="10" spans="1:40">
-      <c r="B10" s="140" t="s">
-        <v>267</v>
-      </c>
-      <c r="C10" s="140"/>
-      <c r="D10" s="140"/>
-      <c r="E10" s="140"/>
       <c r="F10" s="140"/>
-      <c r="G10" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="H10" s="140"/>
-      <c r="I10" s="140"/>
-      <c r="J10" s="140"/>
-      <c r="K10" s="140" t="s">
-        <v>269</v>
+      <c r="G10" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="H10" s="140" t="str">
+        <v/>
+      </c>
+      <c r="I10" s="140" t="str">
+        <v/>
+      </c>
+      <c r="J10" s="140" t="str">
+        <v/>
+      </c>
+      <c r="K10" s="140" t="str">
+        <v>*</v>
       </c>
       <c r="L10" s="140"/>
       <c r="M10" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($A$2),ROW()),"*","")</f>
         <v>*</v>
       </c>
-      <c r="N10" s="138" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($B$3),ROW()),"*","")</f>
+      <c r="N10" s="140" t="str">
         <v/>
       </c>
       <c r="O10" s="140" t="str">
-        <f>IF(COUNTIFS($C$4,ROW()),"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="P10" s="140" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Q10" s="140" t="str">
-        <f t="shared" si="1"/>
         <v>*</v>
       </c>
       <c r="R10" s="140"/>
       <c r="S10" s="140" t="str">
-        <f t="shared" si="2"/>
         <v>*</v>
       </c>
       <c r="T10" s="140" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="U10" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($U$2),ROW()),"*","")</f>
         <v/>
       </c>
       <c r="V10" s="140" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W10" s="140"/>
       <c r="X10" s="140"/>
       <c r="Y10" s="140" t="str">
-        <f t="shared" si="5"/>
         <v>*</v>
       </c>
       <c r="Z10" s="140" t="str">
-        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AA10" s="140" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB10" s="140" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AC10" s="140" t="str">
-        <f t="shared" si="9"/>
         <v>*</v>
       </c>
       <c r="AD10" s="140"/>
       <c r="AE10" s="140" t="str">
-        <f t="shared" si="10"/>
         <v>*</v>
       </c>
       <c r="AF10" s="140" t="str">
-        <f t="shared" si="11"/>
+        <v>*</v>
+      </c>
+      <c r="AG10" s="140" t="str">
         <v/>
       </c>
-      <c r="AG10" s="140" t="str">
-        <f t="shared" si="12"/>
+      <c r="AH10" s="140" t="str">
+        <v/>
+      </c>
+      <c r="AK10" s="147" t="s">
+        <v>270</v>
+      </c>
+      <c r="AL10" s="146" t="s">
+        <v>277</v>
+      </c>
+      <c r="AM10" s="145">
+        <v>5</v>
+      </c>
+      <c r="AN10" s="168"/>
+    </row>
+    <row r="11" spans="1:40">
+      <c r="B11" s="140" t="str">
         <v>*</v>
       </c>
-      <c r="AH10" s="140" t="str">
-        <f t="shared" si="13"/>
+      <c r="C11" s="140" t="str">
         <v/>
       </c>
-      <c r="AK10" s="147" t="s">
-        <v>269</v>
-      </c>
-      <c r="AL10" s="146" t="s">
-        <v>276</v>
-      </c>
-      <c r="AM10" s="145">
-        <v>6</v>
-      </c>
-      <c r="AN10" s="168"/>
-    </row>
-    <row r="11" spans="1:40">
-      <c r="B11" s="140" t="s">
-        <v>268</v>
-      </c>
-      <c r="C11" s="140"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="140"/>
+      <c r="D11" s="140" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="140" t="str">
+        <v/>
+      </c>
       <c r="F11" s="140"/>
-      <c r="G11" s="138" t="s">
-        <v>267</v>
-      </c>
-      <c r="H11" s="140"/>
-      <c r="I11" s="140"/>
-      <c r="J11" s="140"/>
-      <c r="K11" s="140" t="s">
-        <v>270</v>
+      <c r="G11" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="H11" s="140" t="str">
+        <v/>
+      </c>
+      <c r="I11" s="140" t="str">
+        <v/>
+      </c>
+      <c r="J11" s="140" t="str">
+        <v/>
+      </c>
+      <c r="K11" s="140" t="str">
+        <v>*</v>
       </c>
       <c r="L11" s="140"/>
       <c r="M11" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($A$2),ROW()),"*","")</f>
         <v>*</v>
       </c>
       <c r="N11" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($B$3),ROW()),"*","")</f>
+        <v/>
+      </c>
+      <c r="O11" s="140" t="str">
         <v>*</v>
       </c>
-      <c r="O11" s="140" t="str">
-        <f>IF(COUNTIFS($C$4,ROW()),"*","")</f>
+      <c r="P11" s="140" t="str">
         <v/>
       </c>
-      <c r="P11" s="140" t="str">
-        <f t="shared" si="0"/>
-        <v>*</v>
-      </c>
       <c r="Q11" s="140" t="str">
-        <f t="shared" si="1"/>
         <v>*</v>
       </c>
       <c r="R11" s="140"/>
       <c r="S11" s="140" t="str">
-        <f t="shared" si="2"/>
         <v>*</v>
       </c>
       <c r="T11" s="140" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="U11" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($U$2),ROW()),"*","")</f>
         <v/>
       </c>
       <c r="V11" s="140" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W11" s="140"/>
       <c r="X11" s="140"/>
       <c r="Y11" s="140" t="str">
-        <f t="shared" si="5"/>
         <v>*</v>
       </c>
       <c r="Z11" s="140" t="str">
-        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AA11" s="140" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB11" s="140" t="str">
-        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AC11" s="140" t="str">
-        <f t="shared" si="9"/>
         <v>*</v>
       </c>
       <c r="AD11" s="140"/>
       <c r="AE11" s="140" t="str">
-        <f t="shared" si="10"/>
         <v>*</v>
       </c>
       <c r="AF11" s="140" t="str">
-        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AG11" s="140" t="str">
-        <f t="shared" si="12"/>
+        <v>*</v>
+      </c>
+      <c r="AH11" s="140" t="str">
         <v/>
       </c>
-      <c r="AH11" s="140" t="str">
-        <f t="shared" si="13"/>
+      <c r="AK11" s="147" t="s">
+        <v>269</v>
+      </c>
+      <c r="AL11" s="146" t="s">
+        <v>276</v>
+      </c>
+      <c r="AM11" s="145">
+        <v>6</v>
+      </c>
+      <c r="AN11" s="168"/>
+    </row>
+    <row r="12" spans="1:40">
+      <c r="B12" s="140" t="str">
         <v>*</v>
       </c>
-      <c r="AK11" s="147" t="s">
-        <v>268</v>
-      </c>
-      <c r="AL11" s="146" t="s">
-        <v>275</v>
-      </c>
-      <c r="AM11" s="145">
-        <v>7</v>
-      </c>
-      <c r="AN11" s="168"/>
-    </row>
-    <row r="12" spans="1:40">
-      <c r="B12" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="141" t="s">
-        <v>265</v>
+      <c r="C12" s="140" t="str">
+        <v/>
+      </c>
+      <c r="D12" s="140" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="140" t="str">
+        <v/>
       </c>
       <c r="F12" s="140"/>
-      <c r="G12" s="138" t="s">
-        <v>272</v>
-      </c>
-      <c r="H12" s="140"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="K12" s="140" t="s">
-        <v>272</v>
+      <c r="G12" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="H12" s="140" t="str">
+        <v/>
+      </c>
+      <c r="I12" s="140" t="str">
+        <v/>
+      </c>
+      <c r="J12" s="140" t="str">
+        <v/>
+      </c>
+      <c r="K12" s="140" t="str">
+        <v>*</v>
       </c>
       <c r="L12" s="140"/>
       <c r="M12" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($A$2),ROW()),"*","")</f>
         <v>*</v>
       </c>
-      <c r="N12" s="138" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($B$3),ROW()),"*","")</f>
+      <c r="N12" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="O12" s="140" t="str">
         <v/>
       </c>
-      <c r="O12" s="140"/>
       <c r="P12" s="140" t="str">
-        <f>IF(COUNTIFS($P$2,ROW()),"*","")</f>
-        <v/>
+        <v>*</v>
       </c>
       <c r="Q12" s="140" t="str">
-        <f t="shared" si="1"/>
         <v>*</v>
       </c>
       <c r="R12" s="140"/>
       <c r="S12" s="140" t="str">
-        <f t="shared" si="2"/>
+        <v>*</v>
+      </c>
+      <c r="T12" s="140" t="str">
         <v/>
       </c>
-      <c r="T12" s="140" t="str">
-        <f t="shared" si="3"/>
-        <v>*</v>
-      </c>
       <c r="U12" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($U$2),ROW()),"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="V12" s="140" t="str">
-        <f t="shared" si="4"/>
-        <v>*</v>
+        <v/>
       </c>
       <c r="W12" s="140"/>
       <c r="X12" s="140"/>
       <c r="Y12" s="140" t="str">
-        <f>IF(COUNTIFS(_xlfn.ANCHORARRAY($Y$2),ROW()),"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="Z12" s="140" t="str">
         <v/>
       </c>
-      <c r="Z12" s="140" t="str">
-        <f t="shared" si="6"/>
+      <c r="AA12" s="140" t="str">
+        <v/>
+      </c>
+      <c r="AB12" s="140" t="str">
+        <v/>
+      </c>
+      <c r="AC12" s="140" t="str">
         <v>*</v>
-      </c>
-      <c r="AA12" s="140" t="str">
-        <f t="shared" si="7"/>
-        <v>*</v>
-      </c>
-      <c r="AB12" s="140" t="str">
-        <f t="shared" si="8"/>
-        <v>*</v>
-      </c>
-      <c r="AC12" s="140" t="str">
-        <f t="shared" si="9"/>
-        <v/>
       </c>
       <c r="AD12" s="140"/>
       <c r="AE12" s="140" t="str">
-        <f t="shared" si="10"/>
         <v>*</v>
       </c>
       <c r="AF12" s="140" t="str">
-        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AG12" s="140" t="str">
-        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AH12" s="140" t="str">
-        <f t="shared" si="13"/>
         <v>*</v>
       </c>
       <c r="AK12" s="147" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AL12" s="146" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AM12" s="145">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AN12" s="168"/>
     </row>
     <row r="13" spans="1:40">
-      <c r="B13" s="140"/>
-      <c r="C13" s="140"/>
-      <c r="D13" s="140"/>
-      <c r="E13" s="140"/>
+      <c r="B13" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="C13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="D13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="E13" s="141" t="str">
+        <v/>
+      </c>
       <c r="F13" s="140"/>
-      <c r="G13" s="140"/>
-      <c r="H13" s="140"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="140"/>
-      <c r="K13" s="140"/>
+      <c r="G13" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="H13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="I13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="J13" s="139" t="str">
+        <v/>
+      </c>
+      <c r="K13" s="140" t="str">
+        <v>*</v>
+      </c>
       <c r="L13" s="140"/>
-      <c r="M13" s="140"/>
-      <c r="N13" s="140"/>
-      <c r="O13" s="140"/>
-      <c r="P13" s="140"/>
-      <c r="Q13" s="140"/>
+      <c r="M13" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="N13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="O13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="P13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="Q13" s="140" t="str">
+        <v>*</v>
+      </c>
       <c r="R13" s="140"/>
-      <c r="S13" s="140"/>
-      <c r="T13" s="140"/>
-      <c r="U13" s="140"/>
-      <c r="V13" s="140"/>
+      <c r="S13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="T13" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="U13" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="V13" s="140" t="str">
+        <v>*</v>
+      </c>
       <c r="W13" s="140"/>
       <c r="X13" s="140"/>
-      <c r="Y13" s="140"/>
-      <c r="Z13" s="140"/>
-      <c r="AA13" s="140"/>
-      <c r="AB13" s="140"/>
-      <c r="AC13" s="140"/>
+      <c r="Y13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="Z13" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="AA13" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="AB13" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="AC13" s="140" t="str">
+        <v/>
+      </c>
       <c r="AD13" s="140"/>
-      <c r="AE13" s="140"/>
-      <c r="AF13" s="140"/>
-      <c r="AG13" s="140"/>
-      <c r="AH13" s="140"/>
-      <c r="AK13" s="144" t="s">
+      <c r="AE13" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="AF13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="AG13" s="140" t="str">
+        <v/>
+      </c>
+      <c r="AH13" s="140" t="str">
+        <v>*</v>
+      </c>
+      <c r="AK13" s="147" t="s">
+        <v>267</v>
+      </c>
+      <c r="AL13" s="146" t="s">
+        <v>274</v>
+      </c>
+      <c r="AM13" s="145">
+        <v>8</v>
+      </c>
+      <c r="AN13" s="168"/>
+    </row>
+    <row r="14" spans="1:40">
+      <c r="B14" s="140"/>
+      <c r="C14" s="140"/>
+      <c r="D14" s="140"/>
+      <c r="E14" s="140"/>
+      <c r="F14" s="140"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="140"/>
+      <c r="I14" s="140"/>
+      <c r="J14" s="140"/>
+      <c r="K14" s="140"/>
+      <c r="L14" s="140"/>
+      <c r="M14" s="140"/>
+      <c r="N14" s="140"/>
+      <c r="O14" s="140"/>
+      <c r="P14" s="140"/>
+      <c r="Q14" s="140"/>
+      <c r="R14" s="140"/>
+      <c r="S14" s="140"/>
+      <c r="T14" s="140"/>
+      <c r="U14" s="140"/>
+      <c r="V14" s="140"/>
+      <c r="W14" s="140"/>
+      <c r="X14" s="140"/>
+      <c r="Y14" s="140"/>
+      <c r="Z14" s="140"/>
+      <c r="AA14" s="140"/>
+      <c r="AB14" s="140"/>
+      <c r="AC14" s="140"/>
+      <c r="AD14" s="140"/>
+      <c r="AE14" s="140"/>
+      <c r="AF14" s="140"/>
+      <c r="AG14" s="140"/>
+      <c r="AH14" s="140"/>
+      <c r="AK14" s="144" t="s">
         <v>266</v>
       </c>
-      <c r="AL13" s="143" t="s">
+      <c r="AL14" s="143" t="s">
         <v>273</v>
       </c>
-      <c r="AM13" s="142">
+      <c r="AM14" s="142">
         <v>9</v>
       </c>
-      <c r="AN13" s="168"/>
-    </row>
-    <row r="14" spans="1:40">
-      <c r="B14" s="141"/>
-      <c r="C14" s="141" t="s">
+      <c r="AN14" s="168"/>
+    </row>
+    <row r="15" spans="1:40">
+      <c r="B15" s="141"/>
+      <c r="C15" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="D14" s="139"/>
-      <c r="E14" s="139"/>
-      <c r="F14" s="139"/>
-      <c r="G14" s="141" t="s">
+      <c r="D15" s="139"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139"/>
+      <c r="G15" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="H14" s="139"/>
-      <c r="I14" s="139"/>
-      <c r="J14" s="139"/>
-      <c r="K14" s="141" t="s">
+      <c r="H15" s="139"/>
+      <c r="I15" s="139"/>
+      <c r="J15" s="139"/>
+      <c r="K15" s="141" t="s">
         <v>265</v>
-      </c>
-      <c r="L14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="M14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="N14" s="139"/>
-      <c r="O14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="P14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q14" s="139"/>
-      <c r="R14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="S14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="T14" s="139"/>
-      <c r="U14" s="139"/>
-      <c r="V14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="W14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="X14" s="139"/>
-      <c r="Y14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="Z14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AA14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AB14" s="139"/>
-      <c r="AC14" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="AD14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AE14" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="AF14" s="139"/>
-      <c r="AG14" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AH14" s="139"/>
-      <c r="AK14" s="168"/>
-      <c r="AL14" s="168"/>
-      <c r="AM14" s="168"/>
-      <c r="AN14" s="168"/>
-    </row>
-    <row r="15" spans="1:40">
-      <c r="B15" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="C15" s="139"/>
-      <c r="D15" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="E15" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="F15" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="G15" s="140" t="s">
-        <v>272</v>
-      </c>
-      <c r="H15" s="139"/>
-      <c r="I15" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="J15" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="K15" s="140" t="s">
-        <v>272</v>
       </c>
       <c r="L15" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="M15" s="141" t="s">
+      <c r="M15" s="139" t="s">
         <v>265</v>
       </c>
       <c r="N15" s="139"/>
       <c r="O15" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="P15" s="139"/>
-      <c r="Q15" s="141" t="s">
+      <c r="P15" s="139" t="s">
         <v>265</v>
       </c>
+      <c r="Q15" s="139"/>
       <c r="R15" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="S15" s="141" t="s">
+      <c r="S15" s="139" t="s">
         <v>265</v>
       </c>
       <c r="T15" s="139"/>
@@ -29417,26 +29403,28 @@
       <c r="V15" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="W15" s="139"/>
-      <c r="X15" s="139" t="s">
+      <c r="W15" s="139" t="s">
         <v>265</v>
       </c>
+      <c r="X15" s="139"/>
       <c r="Y15" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Z15" s="139"/>
+      <c r="Z15" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="AA15" s="139" t="s">
         <v>265</v>
       </c>
       <c r="AB15" s="139"/>
-      <c r="AC15" s="140" t="s">
-        <v>272</v>
+      <c r="AC15" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="AD15" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AE15" s="140" t="s">
-        <v>272</v>
+      <c r="AE15" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="AF15" s="139"/>
       <c r="AG15" s="139" t="s">
@@ -29449,12 +29437,10 @@
       <c r="AN15" s="168"/>
     </row>
     <row r="16" spans="1:40">
-      <c r="B16" s="140" t="s">
-        <v>272</v>
-      </c>
-      <c r="C16" s="139" t="s">
+      <c r="B16" s="141" t="s">
         <v>265</v>
       </c>
+      <c r="C16" s="139"/>
       <c r="D16" s="139" t="s">
         <v>265</v>
       </c>
@@ -29464,28 +29450,38 @@
       <c r="F16" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="G16" s="139" t="s">
+      <c r="G16" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="H16" s="139"/>
+      <c r="I16" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="H16" s="139"/>
-      <c r="I16" s="139"/>
-      <c r="J16" s="139"/>
-      <c r="K16" s="139"/>
+      <c r="J16" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="K16" s="140" t="s">
+        <v>272</v>
+      </c>
       <c r="L16" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="M16" s="140" t="s">
-        <v>272</v>
+      <c r="M16" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="N16" s="139"/>
-      <c r="O16" s="139"/>
+      <c r="O16" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="P16" s="139"/>
-      <c r="Q16" s="140" t="s">
-        <v>272</v>
-      </c>
-      <c r="R16" s="139"/>
-      <c r="S16" s="140" t="s">
-        <v>272</v>
+      <c r="Q16" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="R16" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="S16" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="T16" s="139"/>
       <c r="U16" s="139"/>
@@ -29504,34 +29500,36 @@
         <v>265</v>
       </c>
       <c r="AB16" s="139"/>
-      <c r="AC16" s="139"/>
+      <c r="AC16" s="140" t="s">
+        <v>272</v>
+      </c>
       <c r="AD16" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AE16" s="139" t="s">
-        <v>265</v>
+      <c r="AE16" s="140" t="s">
+        <v>272</v>
       </c>
       <c r="AF16" s="139"/>
       <c r="AG16" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AH16" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="AH16" s="139"/>
       <c r="AK16" s="168"/>
       <c r="AL16" s="168"/>
       <c r="AM16" s="168"/>
       <c r="AN16" s="168"/>
     </row>
     <row r="17" spans="2:40">
-      <c r="B17" s="141" t="s">
+      <c r="B17" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="C17" s="139"/>
       <c r="D17" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="E17" s="141" t="s">
+      <c r="E17" s="139" t="s">
         <v>265</v>
       </c>
       <c r="F17" s="139" t="s">
@@ -29540,55 +29538,55 @@
       <c r="G17" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="H17" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="H17" s="139"/>
       <c r="I17" s="139"/>
       <c r="J17" s="139"/>
       <c r="K17" s="139"/>
       <c r="L17" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="M17" s="141" t="s">
-        <v>265</v>
+      <c r="M17" s="140" t="s">
+        <v>272</v>
       </c>
       <c r="N17" s="139"/>
       <c r="O17" s="139"/>
       <c r="P17" s="139"/>
-      <c r="Q17" s="141" t="s">
+      <c r="Q17" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="R17" s="139"/>
+      <c r="S17" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="T17" s="139"/>
+      <c r="U17" s="139"/>
+      <c r="V17" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="R17" s="139"/>
-      <c r="S17" s="139"/>
-      <c r="T17" s="141" t="s">
+      <c r="W17" s="139"/>
+      <c r="X17" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="U17" s="139" t="s">
+      <c r="Y17" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="V17" s="139"/>
-      <c r="W17" s="139"/>
-      <c r="X17" s="139"/>
-      <c r="Y17" s="139"/>
-      <c r="Z17" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="Z17" s="139"/>
       <c r="AA17" s="139" t="s">
         <v>265</v>
       </c>
       <c r="AB17" s="139"/>
       <c r="AC17" s="139"/>
-      <c r="AD17" s="139"/>
+      <c r="AD17" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="AE17" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AF17" s="141" t="s">
-        <v>265</v>
-      </c>
+      <c r="AF17" s="139"/>
       <c r="AG17" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AH17" s="141" t="s">
+      <c r="AH17" s="139" t="s">
         <v>265</v>
       </c>
       <c r="AK17" s="168"/>
@@ -29597,78 +29595,72 @@
       <c r="AN17" s="168"/>
     </row>
     <row r="18" spans="2:40">
-      <c r="B18" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="C18" s="139" t="s">
+      <c r="B18" s="141" t="s">
         <v>265</v>
       </c>
+      <c r="C18" s="139"/>
       <c r="D18" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="E18" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="F18" s="139"/>
-      <c r="G18" s="141" t="s">
+      <c r="E18" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="H18" s="139"/>
+      <c r="F18" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="G18" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="H18" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="I18" s="139"/>
       <c r="J18" s="139"/>
       <c r="K18" s="139"/>
-      <c r="L18" s="139"/>
-      <c r="M18" s="140" t="s">
-        <v>271</v>
+      <c r="L18" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="M18" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="N18" s="139"/>
-      <c r="O18" s="139" t="s">
+      <c r="O18" s="139"/>
+      <c r="P18" s="139"/>
+      <c r="Q18" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="P18" s="139" t="s">
+      <c r="R18" s="139"/>
+      <c r="S18" s="139"/>
+      <c r="T18" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="Q18" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="R18" s="139" t="s">
+      <c r="U18" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="S18" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="T18" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="U18" s="139"/>
-      <c r="V18" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="V18" s="139"/>
       <c r="W18" s="139"/>
       <c r="X18" s="139"/>
-      <c r="Y18" s="141" t="s">
+      <c r="Y18" s="139"/>
+      <c r="Z18" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Z18" s="139"/>
       <c r="AA18" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AB18" s="139" t="s">
+      <c r="AB18" s="139"/>
+      <c r="AC18" s="139"/>
+      <c r="AD18" s="139"/>
+      <c r="AE18" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AC18" s="141" t="s">
+      <c r="AF18" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="AD18" s="139" t="s">
+      <c r="AG18" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AE18" s="139"/>
-      <c r="AF18" s="140" t="s">
-        <v>272</v>
-      </c>
-      <c r="AG18" s="139"/>
-      <c r="AH18" s="140" t="s">
-        <v>271</v>
+      <c r="AH18" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="AK18" s="168"/>
       <c r="AL18" s="168"/>
@@ -29676,28 +29668,30 @@
       <c r="AN18" s="168"/>
     </row>
     <row r="19" spans="2:40">
-      <c r="B19" s="139"/>
-      <c r="C19" s="139"/>
+      <c r="B19" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="C19" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="D19" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="E19" s="139" t="s">
+      <c r="E19" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="F19" s="139"/>
+      <c r="G19" s="141" t="s">
         <v>265</v>
-      </c>
-      <c r="F19" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="G19" s="140" t="s">
-        <v>271</v>
       </c>
       <c r="H19" s="139"/>
       <c r="I19" s="139"/>
       <c r="J19" s="139"/>
       <c r="K19" s="139"/>
-      <c r="L19" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="M19" s="139"/>
+      <c r="L19" s="139"/>
+      <c r="M19" s="140" t="s">
+        <v>271</v>
+      </c>
       <c r="N19" s="139"/>
       <c r="O19" s="139" t="s">
         <v>265</v>
@@ -29705,50 +29699,48 @@
       <c r="P19" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Q19" s="141" t="s">
-        <v>265</v>
+      <c r="Q19" s="140" t="s">
+        <v>271</v>
       </c>
       <c r="R19" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="S19" s="141" t="s">
+      <c r="S19" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="T19" s="139"/>
-      <c r="U19" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="T19" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="U19" s="139"/>
       <c r="V19" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="W19" s="139" t="s">
+      <c r="W19" s="139"/>
+      <c r="X19" s="139"/>
+      <c r="Y19" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="X19" s="139"/>
-      <c r="Y19" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="Z19" s="139" t="s">
+      <c r="Z19" s="139"/>
+      <c r="AA19" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AA19" s="139"/>
       <c r="AB19" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AC19" s="140" t="s">
-        <v>272</v>
+      <c r="AC19" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="AD19" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AE19" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AF19" s="139"/>
-      <c r="AG19" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="AH19" s="139"/>
+      <c r="AE19" s="139"/>
+      <c r="AF19" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="AG19" s="139"/>
+      <c r="AH19" s="140" t="s">
+        <v>271</v>
+      </c>
       <c r="AK19" s="168"/>
       <c r="AL19" s="168"/>
       <c r="AM19" s="168"/>
@@ -29756,29 +29748,27 @@
     </row>
     <row r="20" spans="2:40">
       <c r="B20" s="139"/>
-      <c r="C20" s="141" t="s">
+      <c r="C20" s="139"/>
+      <c r="D20" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="D20" s="141" t="s">
+      <c r="E20" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="E20" s="139"/>
-      <c r="F20" s="139"/>
-      <c r="G20" s="141" t="s">
+      <c r="F20" s="139" t="s">
         <v>265</v>
+      </c>
+      <c r="G20" s="140" t="s">
+        <v>271</v>
       </c>
       <c r="H20" s="139"/>
       <c r="I20" s="139"/>
       <c r="J20" s="139"/>
-      <c r="K20" s="141" t="s">
-        <v>265</v>
-      </c>
+      <c r="K20" s="139"/>
       <c r="L20" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="M20" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="M20" s="139"/>
       <c r="N20" s="139"/>
       <c r="O20" s="139" t="s">
         <v>265</v>
@@ -29786,42 +29776,48 @@
       <c r="P20" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Q20" s="140" t="s">
-        <v>271</v>
+      <c r="Q20" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="R20" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="S20" s="140" t="s">
+      <c r="S20" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="T20" s="139"/>
+      <c r="U20" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="V20" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="W20" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="X20" s="139"/>
+      <c r="Y20" s="140" t="s">
         <v>271</v>
       </c>
-      <c r="T20" s="141" t="s">
+      <c r="Z20" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="U20" s="139"/>
-      <c r="V20" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="W20" s="139"/>
-      <c r="X20" s="139"/>
-      <c r="Y20" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="Z20" s="139"/>
-      <c r="AA20" s="141" t="s">
-        <v>265</v>
-      </c>
+      <c r="AA20" s="139"/>
       <c r="AB20" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AC20" s="139"/>
-      <c r="AD20" s="139"/>
-      <c r="AE20" s="141" t="s">
+      <c r="AC20" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD20" s="139" t="s">
         <v>265</v>
       </c>
+      <c r="AE20" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="AF20" s="139"/>
-      <c r="AG20" s="140" t="s">
-        <v>271</v>
+      <c r="AG20" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="AH20" s="139"/>
       <c r="AK20" s="168"/>
@@ -29831,28 +29827,22 @@
     </row>
     <row r="21" spans="2:40">
       <c r="B21" s="139"/>
-      <c r="C21" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="D21" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="E21" s="139" t="s">
+      <c r="C21" s="141" t="s">
         <v>265</v>
       </c>
+      <c r="D21" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="E21" s="139"/>
       <c r="F21" s="139"/>
-      <c r="G21" s="140" t="s">
-        <v>272</v>
-      </c>
-      <c r="H21" s="139" t="s">
+      <c r="G21" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="I21" s="139" t="s">
+      <c r="H21" s="139"/>
+      <c r="I21" s="139"/>
+      <c r="J21" s="139"/>
+      <c r="K21" s="141" t="s">
         <v>265</v>
-      </c>
-      <c r="J21" s="139"/>
-      <c r="K21" s="140" t="s">
-        <v>272</v>
       </c>
       <c r="L21" s="139" t="s">
         <v>265</v>
@@ -29860,76 +29850,70 @@
       <c r="M21" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="N21" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="O21" s="141" t="s">
+      <c r="N21" s="139"/>
+      <c r="O21" s="139" t="s">
         <v>265</v>
       </c>
       <c r="P21" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Q21" s="139"/>
-      <c r="R21" s="139"/>
-      <c r="S21" s="139"/>
-      <c r="T21" s="140" t="s">
-        <v>272</v>
+      <c r="Q21" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="R21" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="S21" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="T21" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="U21" s="139"/>
-      <c r="V21" s="140" t="s">
-        <v>272</v>
-      </c>
-      <c r="W21" s="139" t="s">
+      <c r="V21" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="X21" s="139" t="s">
+      <c r="W21" s="139"/>
+      <c r="X21" s="139"/>
+      <c r="Y21" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="Y21" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="Z21" s="139" t="s">
+      <c r="Z21" s="139"/>
+      <c r="AA21" s="141" t="s">
         <v>265</v>
-      </c>
-      <c r="AA21" s="140" t="s">
-        <v>272</v>
       </c>
       <c r="AB21" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AC21" s="141" t="s">
+      <c r="AC21" s="139"/>
+      <c r="AD21" s="139"/>
+      <c r="AE21" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="AD21" s="139"/>
-      <c r="AE21" s="140" t="s">
-        <v>272</v>
-      </c>
-      <c r="AF21" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AG21" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AH21" s="141" t="s">
-        <v>265</v>
-      </c>
+      <c r="AF21" s="139"/>
+      <c r="AG21" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="AH21" s="139"/>
       <c r="AK21" s="168"/>
       <c r="AL21" s="168"/>
       <c r="AM21" s="168"/>
       <c r="AN21" s="168"/>
     </row>
     <row r="22" spans="2:40">
-      <c r="B22" s="141" t="s">
+      <c r="B22" s="139"/>
+      <c r="C22" s="140" t="s">
+        <v>270</v>
+      </c>
+      <c r="D22" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="E22" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="C22" s="139"/>
-      <c r="D22" s="139"/>
-      <c r="E22" s="139"/>
-      <c r="F22" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="G22" s="141" t="s">
-        <v>265</v>
+      <c r="F22" s="139"/>
+      <c r="G22" s="140" t="s">
+        <v>272</v>
       </c>
       <c r="H22" s="139" t="s">
         <v>265</v>
@@ -29938,61 +29922,67 @@
         <v>265</v>
       </c>
       <c r="J22" s="139"/>
-      <c r="K22" s="141" t="s">
+      <c r="K22" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="L22" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="L22" s="139"/>
-      <c r="M22" s="141" t="s">
+      <c r="M22" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="N22" s="139"/>
-      <c r="O22" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="P22" s="139"/>
+      <c r="N22" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="O22" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="P22" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="Q22" s="139"/>
-      <c r="R22" s="139" t="s">
+      <c r="R22" s="139"/>
+      <c r="S22" s="139"/>
+      <c r="T22" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="U22" s="139"/>
+      <c r="V22" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="W22" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="S22" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="T22" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="U22" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="V22" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="W22" s="139"/>
       <c r="X22" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Y22" s="141" t="s">
-        <v>265</v>
+      <c r="Y22" s="140" t="s">
+        <v>270</v>
       </c>
       <c r="Z22" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AA22" s="139"/>
+      <c r="AA22" s="140" t="s">
+        <v>272</v>
+      </c>
       <c r="AB22" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AC22" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="AD22" s="139" t="s">
+      <c r="AC22" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="AE22" s="141" t="s">
+      <c r="AD22" s="139"/>
+      <c r="AE22" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="AF22" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AF22" s="139"/>
-      <c r="AG22" s="139"/>
-      <c r="AH22" s="140" t="s">
-        <v>270</v>
+      <c r="AG22" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AH22" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="AK22" s="168"/>
       <c r="AL22" s="168"/>
@@ -30000,153 +29990,159 @@
       <c r="AN22" s="168"/>
     </row>
     <row r="23" spans="2:40">
-      <c r="B23" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="C23" s="139" t="s">
+      <c r="B23" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="D23" s="141" t="s">
-        <v>265</v>
-      </c>
+      <c r="C23" s="139"/>
+      <c r="D23" s="139"/>
       <c r="E23" s="139"/>
       <c r="F23" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="G23" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="H23" s="139"/>
-      <c r="I23" s="139"/>
+      <c r="G23" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="H23" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="I23" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="J23" s="139"/>
-      <c r="K23" s="140" t="s">
-        <v>270</v>
+      <c r="K23" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="L23" s="139"/>
-      <c r="M23" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="N23" s="139" t="s">
+      <c r="M23" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="O23" s="139" t="s">
-        <v>265</v>
+      <c r="N23" s="139"/>
+      <c r="O23" s="140" t="s">
+        <v>271</v>
       </c>
       <c r="P23" s="139"/>
-      <c r="Q23" s="141" t="s">
-        <v>265</v>
-      </c>
+      <c r="Q23" s="139"/>
       <c r="R23" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="S23" s="141" t="s">
+      <c r="S23" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="T23" s="139"/>
-      <c r="U23" s="141" t="s">
+      <c r="T23" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="U23" s="139" t="s">
         <v>265</v>
       </c>
       <c r="V23" s="139" t="s">
         <v>265</v>
       </c>
       <c r="W23" s="139"/>
-      <c r="X23" s="139"/>
-      <c r="Y23" s="140" t="s">
-        <v>271</v>
+      <c r="X23" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="Y23" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="Z23" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AA23" s="139" t="s">
+      <c r="AA23" s="139"/>
+      <c r="AB23" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AB23" s="141" t="s">
+      <c r="AC23" s="140" t="s">
+        <v>270</v>
+      </c>
+      <c r="AD23" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AC23" s="139" t="s">
+      <c r="AE23" s="141" t="s">
         <v>265</v>
-      </c>
-      <c r="AD23" s="139"/>
-      <c r="AE23" s="140" t="s">
-        <v>270</v>
       </c>
       <c r="AF23" s="139"/>
       <c r="AG23" s="139"/>
-      <c r="AH23" s="139"/>
+      <c r="AH23" s="140" t="s">
+        <v>270</v>
+      </c>
       <c r="AK23" s="168"/>
       <c r="AL23" s="168"/>
       <c r="AM23" s="168"/>
       <c r="AN23" s="168"/>
     </row>
     <row r="24" spans="2:40">
-      <c r="B24" s="139" t="s">
+      <c r="B24" s="140" t="s">
+        <v>270</v>
+      </c>
+      <c r="C24" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="C24" s="139"/>
-      <c r="D24" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="E24" s="139" t="s">
+      <c r="D24" s="141" t="s">
         <v>265</v>
       </c>
+      <c r="E24" s="139"/>
       <c r="F24" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="G24" s="139"/>
-      <c r="H24" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="I24" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="G24" s="140" t="s">
+        <v>270</v>
+      </c>
+      <c r="H24" s="139"/>
+      <c r="I24" s="139"/>
       <c r="J24" s="139"/>
-      <c r="K24" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="L24" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="M24" s="139"/>
+      <c r="K24" s="140" t="s">
+        <v>270</v>
+      </c>
+      <c r="L24" s="139"/>
+      <c r="M24" s="140" t="s">
+        <v>270</v>
+      </c>
       <c r="N24" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="O24" s="139"/>
-      <c r="P24" s="139" t="s">
+      <c r="O24" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Q24" s="140" t="s">
-        <v>270</v>
+      <c r="P24" s="139"/>
+      <c r="Q24" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="R24" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="S24" s="140" t="s">
+      <c r="S24" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="T24" s="139"/>
+      <c r="U24" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="V24" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="W24" s="139"/>
+      <c r="X24" s="139"/>
+      <c r="Y24" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z24" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AA24" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AB24" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="AC24" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AD24" s="139"/>
+      <c r="AE24" s="140" t="s">
         <v>270</v>
       </c>
-      <c r="T24" s="139"/>
-      <c r="U24" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="V24" s="139"/>
-      <c r="W24" s="139"/>
-      <c r="X24" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="Y24" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="Z24" s="139"/>
-      <c r="AA24" s="139"/>
-      <c r="AB24" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="AC24" s="139"/>
-      <c r="AD24" s="139"/>
-      <c r="AE24" s="139"/>
       <c r="AF24" s="139"/>
-      <c r="AG24" s="141" t="s">
-        <v>265</v>
-      </c>
+      <c r="AG24" s="139"/>
       <c r="AH24" s="139"/>
       <c r="AK24" s="168"/>
       <c r="AL24" s="168"/>
@@ -30154,67 +30150,73 @@
       <c r="AN24" s="168"/>
     </row>
     <row r="25" spans="2:40">
-      <c r="B25" s="139"/>
+      <c r="B25" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="C25" s="139"/>
-      <c r="D25" s="139"/>
+      <c r="D25" s="140" t="s">
+        <v>269</v>
+      </c>
       <c r="E25" s="139" t="s">
         <v>265</v>
       </c>
       <c r="F25" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="G25" s="139" t="s">
+      <c r="G25" s="139"/>
+      <c r="H25" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="H25" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="I25" s="139"/>
-      <c r="J25" s="139" t="s">
+      <c r="I25" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="K25" s="141" t="s">
+      <c r="J25" s="139"/>
+      <c r="K25" s="139" t="s">
         <v>265</v>
       </c>
       <c r="L25" s="139" t="s">
         <v>265</v>
       </c>
       <c r="M25" s="139"/>
-      <c r="N25" s="141" t="s">
+      <c r="N25" s="139" t="s">
         <v>265</v>
       </c>
       <c r="O25" s="139"/>
-      <c r="P25" s="139"/>
-      <c r="Q25" s="139"/>
-      <c r="R25" s="139"/>
-      <c r="S25" s="141" t="s">
+      <c r="P25" s="139" t="s">
         <v>265</v>
       </c>
+      <c r="Q25" s="140" t="s">
+        <v>270</v>
+      </c>
+      <c r="R25" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="S25" s="140" t="s">
+        <v>270</v>
+      </c>
       <c r="T25" s="139"/>
-      <c r="U25" s="139"/>
-      <c r="V25" s="139" t="s">
+      <c r="U25" s="140" t="s">
+        <v>269</v>
+      </c>
+      <c r="V25" s="139"/>
+      <c r="W25" s="139"/>
+      <c r="X25" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="W25" s="139"/>
-      <c r="X25" s="139"/>
-      <c r="Y25" s="139"/>
+      <c r="Y25" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="Z25" s="139"/>
-      <c r="AA25" s="139" t="s">
+      <c r="AA25" s="139"/>
+      <c r="AB25" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="AC25" s="139"/>
+      <c r="AD25" s="139"/>
+      <c r="AE25" s="139"/>
+      <c r="AF25" s="139"/>
+      <c r="AG25" s="141" t="s">
         <v>265</v>
-      </c>
-      <c r="AB25" s="139"/>
-      <c r="AC25" s="139"/>
-      <c r="AD25" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AE25" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="AF25" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AG25" s="140" t="s">
-        <v>270</v>
       </c>
       <c r="AH25" s="139"/>
       <c r="AK25" s="168"/>
@@ -30223,78 +30225,68 @@
       <c r="AN25" s="168"/>
     </row>
     <row r="26" spans="2:40">
-      <c r="B26" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="C26" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="D26" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="B26" s="139"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="139"/>
       <c r="E26" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="F26" s="139"/>
-      <c r="G26" s="139"/>
-      <c r="H26" s="139"/>
+      <c r="F26" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="G26" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="H26" s="140" t="s">
+        <v>269</v>
+      </c>
       <c r="I26" s="139"/>
       <c r="J26" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="K26" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="L26" s="139"/>
-      <c r="M26" s="141" t="s">
+      <c r="K26" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="N26" s="140" t="s">
-        <v>270</v>
+      <c r="L26" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="M26" s="139"/>
+      <c r="N26" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="O26" s="139"/>
       <c r="P26" s="139"/>
-      <c r="Q26" s="141" t="s">
+      <c r="Q26" s="139"/>
+      <c r="R26" s="139"/>
+      <c r="S26" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="R26" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="S26" s="140" t="s">
-        <v>270</v>
-      </c>
-      <c r="T26" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="T26" s="139"/>
       <c r="U26" s="139"/>
       <c r="V26" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="W26" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="X26" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="Y26" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="Z26" s="141" t="s">
-        <v>265</v>
-      </c>
+      <c r="W26" s="139"/>
+      <c r="X26" s="139"/>
+      <c r="Y26" s="139"/>
+      <c r="Z26" s="139"/>
       <c r="AA26" s="139" t="s">
         <v>265</v>
       </c>
       <c r="AB26" s="139"/>
-      <c r="AC26" s="141" t="s">
+      <c r="AC26" s="139"/>
+      <c r="AD26" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AD26" s="139"/>
-      <c r="AE26" s="140" t="s">
+      <c r="AE26" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="AF26" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AG26" s="140" t="s">
         <v>270</v>
       </c>
-      <c r="AF26" s="139"/>
-      <c r="AG26" s="139"/>
       <c r="AH26" s="139"/>
       <c r="AK26" s="168"/>
       <c r="AL26" s="168"/>
@@ -30302,8 +30294,8 @@
       <c r="AN26" s="168"/>
     </row>
     <row r="27" spans="2:40">
-      <c r="B27" s="140" t="s">
-        <v>269</v>
+      <c r="B27" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="C27" s="139" t="s">
         <v>265</v>
@@ -30311,71 +30303,69 @@
       <c r="D27" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="E27" s="139"/>
-      <c r="F27" s="139" t="s">
+      <c r="E27" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="G27" s="141" t="s">
-        <v>265</v>
-      </c>
+      <c r="F27" s="139"/>
+      <c r="G27" s="139"/>
       <c r="H27" s="139"/>
       <c r="I27" s="139"/>
-      <c r="J27" s="141" t="s">
+      <c r="J27" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="K27" s="141" t="s">
+      <c r="K27" s="140" t="s">
+        <v>270</v>
+      </c>
+      <c r="L27" s="139"/>
+      <c r="M27" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="L27" s="139"/>
-      <c r="M27" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="N27" s="139" t="s">
+      <c r="N27" s="140" t="s">
+        <v>270</v>
+      </c>
+      <c r="O27" s="139"/>
+      <c r="P27" s="139"/>
+      <c r="Q27" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="O27" s="139"/>
-      <c r="P27" s="139" t="s">
+      <c r="R27" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Q27" s="140" t="s">
+      <c r="S27" s="140" t="s">
         <v>270</v>
       </c>
-      <c r="R27" s="139"/>
-      <c r="S27" s="141" t="s">
+      <c r="T27" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="T27" s="139"/>
       <c r="U27" s="139"/>
-      <c r="V27" s="139"/>
-      <c r="W27" s="139"/>
+      <c r="V27" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="W27" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="X27" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Y27" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="Z27" s="140" t="s">
-        <v>270</v>
+      <c r="Y27" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z27" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="AA27" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AB27" s="139" t="s">
+      <c r="AB27" s="139"/>
+      <c r="AC27" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="AC27" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="AD27" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AE27" s="141" t="s">
-        <v>265</v>
+      <c r="AD27" s="139"/>
+      <c r="AE27" s="140" t="s">
+        <v>270</v>
       </c>
       <c r="AF27" s="139"/>
-      <c r="AG27" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="AG27" s="139"/>
       <c r="AH27" s="139"/>
       <c r="AK27" s="168"/>
       <c r="AL27" s="168"/>
@@ -30383,161 +30373,161 @@
       <c r="AN27" s="168"/>
     </row>
     <row r="28" spans="2:40">
-      <c r="B28" s="139" t="s">
+      <c r="B28" s="140" t="s">
+        <v>269</v>
+      </c>
+      <c r="C28" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="C28" s="139"/>
-      <c r="D28" s="139"/>
+      <c r="D28" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="E28" s="139"/>
       <c r="F28" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="G28" s="140" t="s">
+      <c r="G28" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="H28" s="139"/>
+      <c r="I28" s="139"/>
+      <c r="J28" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="K28" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="L28" s="139"/>
+      <c r="M28" s="140" t="s">
         <v>269</v>
       </c>
-      <c r="H28" s="139"/>
-      <c r="I28" s="139" t="s">
+      <c r="N28" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="J28" s="140" t="s">
-        <v>268</v>
-      </c>
-      <c r="K28" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="L28" s="139"/>
-      <c r="M28" s="139" t="s">
+      <c r="O28" s="139"/>
+      <c r="P28" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="N28" s="139"/>
-      <c r="O28" s="139" t="s">
+      <c r="Q28" s="140" t="s">
+        <v>270</v>
+      </c>
+      <c r="R28" s="139"/>
+      <c r="S28" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="P28" s="139"/>
-      <c r="Q28" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="R28" s="139"/>
-      <c r="S28" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="T28" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="U28" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="T28" s="139"/>
+      <c r="U28" s="139"/>
       <c r="V28" s="139"/>
       <c r="W28" s="139"/>
       <c r="X28" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Y28" s="141" t="s">
+      <c r="Y28" s="140" t="s">
+        <v>269</v>
+      </c>
+      <c r="Z28" s="140" t="s">
+        <v>270</v>
+      </c>
+      <c r="AA28" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Z28" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AA28" s="139"/>
       <c r="AB28" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AC28" s="141" t="s">
-        <v>265</v>
+      <c r="AC28" s="140" t="s">
+        <v>269</v>
       </c>
       <c r="AD28" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AE28" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="AF28" s="139" t="s">
+      <c r="AE28" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="AG28" s="139"/>
-      <c r="AH28" s="141" t="s">
+      <c r="AF28" s="139"/>
+      <c r="AG28" s="139" t="s">
         <v>265</v>
       </c>
+      <c r="AH28" s="139"/>
       <c r="AK28" s="168"/>
       <c r="AL28" s="168"/>
       <c r="AM28" s="168"/>
       <c r="AN28" s="168"/>
     </row>
     <row r="29" spans="2:40">
-      <c r="B29" s="141" t="s">
+      <c r="B29" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="C29" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="D29" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="C29" s="139"/>
+      <c r="D29" s="139"/>
       <c r="E29" s="139"/>
       <c r="F29" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="G29" s="141" t="s">
-        <v>265</v>
+      <c r="G29" s="140" t="s">
+        <v>269</v>
       </c>
       <c r="H29" s="139"/>
       <c r="I29" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="J29" s="139"/>
-      <c r="K29" s="139"/>
-      <c r="L29" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="M29" s="141" t="s">
+      <c r="J29" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="K29" s="140" t="s">
+        <v>269</v>
+      </c>
+      <c r="L29" s="139"/>
+      <c r="M29" s="139" t="s">
         <v>265</v>
       </c>
       <c r="N29" s="139"/>
       <c r="O29" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="P29" s="139" t="s">
+      <c r="P29" s="139"/>
+      <c r="Q29" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="Q29" s="140" t="s">
+      <c r="R29" s="139"/>
+      <c r="S29" s="140" t="s">
         <v>269</v>
       </c>
-      <c r="R29" s="139" t="s">
+      <c r="T29" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="S29" s="139"/>
-      <c r="T29" s="139"/>
-      <c r="U29" s="139"/>
-      <c r="V29" s="141" t="s">
+      <c r="U29" s="139" t="s">
         <v>265</v>
       </c>
+      <c r="V29" s="139"/>
       <c r="W29" s="139"/>
       <c r="X29" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Y29" s="140" t="s">
-        <v>268</v>
+      <c r="Y29" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="Z29" s="139" t="s">
         <v>265</v>
       </c>
       <c r="AA29" s="139"/>
-      <c r="AB29" s="139"/>
-      <c r="AC29" s="140" t="s">
-        <v>268</v>
+      <c r="AB29" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AC29" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="AD29" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AE29" s="139" t="s">
-        <v>265</v>
+      <c r="AE29" s="140" t="s">
+        <v>269</v>
       </c>
       <c r="AF29" s="139" t="s">
         <v>265</v>
       </c>
       <c r="AG29" s="139"/>
-      <c r="AH29" s="140" t="s">
-        <v>269</v>
+      <c r="AH29" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="AK29" s="168"/>
       <c r="AL29" s="168"/>
@@ -30545,45 +30535,43 @@
       <c r="AN29" s="168"/>
     </row>
     <row r="30" spans="2:40">
-      <c r="B30" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="C30" s="140" t="s">
-        <v>268</v>
+      <c r="B30" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="C30" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="D30" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="E30" s="139" t="s">
+      <c r="E30" s="139"/>
+      <c r="F30" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="F30" s="139"/>
-      <c r="G30" s="140" t="s">
-        <v>268</v>
+      <c r="G30" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="H30" s="139"/>
       <c r="I30" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="J30" s="139" t="s">
+      <c r="J30" s="139"/>
+      <c r="K30" s="139"/>
+      <c r="L30" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="K30" s="141" t="s">
+      <c r="M30" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="L30" s="139"/>
-      <c r="M30" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="N30" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="N30" s="139"/>
       <c r="O30" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="P30" s="139"/>
-      <c r="Q30" s="139" t="s">
+      <c r="P30" s="139" t="s">
         <v>265</v>
+      </c>
+      <c r="Q30" s="140" t="s">
+        <v>269</v>
       </c>
       <c r="R30" s="139" t="s">
         <v>265</v>
@@ -30591,38 +30579,36 @@
       <c r="S30" s="139"/>
       <c r="T30" s="139"/>
       <c r="U30" s="139"/>
-      <c r="V30" s="140" t="s">
-        <v>267</v>
+      <c r="V30" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="W30" s="139"/>
       <c r="X30" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Y30" s="139" t="s">
-        <v>265</v>
+      <c r="Y30" s="140" t="s">
+        <v>268</v>
       </c>
       <c r="Z30" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AA30" s="139" t="s">
+      <c r="AA30" s="139"/>
+      <c r="AB30" s="139"/>
+      <c r="AC30" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD30" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AB30" s="139"/>
-      <c r="AC30" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AD30" s="139"/>
-      <c r="AE30" s="141" t="s">
+      <c r="AE30" s="139" t="s">
         <v>265</v>
       </c>
       <c r="AF30" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AG30" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="AH30" s="139" t="s">
-        <v>265</v>
+      <c r="AG30" s="139"/>
+      <c r="AH30" s="140" t="s">
+        <v>269</v>
       </c>
       <c r="AK30" s="168"/>
       <c r="AL30" s="168"/>
@@ -30630,210 +30616,214 @@
       <c r="AN30" s="168"/>
     </row>
     <row r="31" spans="2:40">
-      <c r="B31" s="141" t="s">
+      <c r="B31" s="140" t="s">
+        <v>269</v>
+      </c>
+      <c r="C31" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="D31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="C31" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="D31" s="139"/>
       <c r="E31" s="139" t="s">
         <v>265</v>
       </c>
       <c r="F31" s="139"/>
-      <c r="G31" s="139" t="s">
+      <c r="G31" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="H31" s="139"/>
+      <c r="I31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="H31" s="139" t="s">
+      <c r="J31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="I31" s="139"/>
-      <c r="J31" s="139"/>
-      <c r="K31" s="140" t="s">
-        <v>267</v>
+      <c r="K31" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="L31" s="139"/>
-      <c r="M31" s="141" t="s">
-        <v>265</v>
+      <c r="M31" s="140" t="s">
+        <v>269</v>
       </c>
       <c r="N31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="O31" s="139"/>
-      <c r="P31" s="141" t="s">
+      <c r="O31" s="139" t="s">
         <v>265</v>
       </c>
+      <c r="P31" s="139"/>
       <c r="Q31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="R31" s="139"/>
+      <c r="R31" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="S31" s="139"/>
       <c r="T31" s="139"/>
-      <c r="U31" s="139" t="s">
+      <c r="U31" s="139"/>
+      <c r="V31" s="140" t="s">
+        <v>267</v>
+      </c>
+      <c r="W31" s="139"/>
+      <c r="X31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="V31" s="139"/>
-      <c r="W31" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="X31" s="139"/>
       <c r="Y31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Z31" s="139"/>
-      <c r="AA31" s="139"/>
-      <c r="AB31" s="139" t="s">
+      <c r="Z31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AC31" s="141" t="s">
+      <c r="AA31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AD31" s="139" t="s">
+      <c r="AB31" s="139"/>
+      <c r="AC31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AE31" s="140" t="s">
-        <v>267</v>
-      </c>
-      <c r="AF31" s="139"/>
+      <c r="AD31" s="139"/>
+      <c r="AE31" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="AF31" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="AG31" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AH31" s="139"/>
+      <c r="AH31" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="AK31" s="168"/>
       <c r="AL31" s="168"/>
       <c r="AM31" s="168"/>
       <c r="AN31" s="168"/>
     </row>
     <row r="32" spans="2:40">
-      <c r="B32" s="140" t="s">
-        <v>268</v>
-      </c>
-      <c r="C32" s="139"/>
+      <c r="B32" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="C32" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="D32" s="139"/>
       <c r="E32" s="139" t="s">
         <v>265</v>
       </c>
       <c r="F32" s="139"/>
-      <c r="G32" s="139"/>
+      <c r="G32" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="H32" s="139" t="s">
         <v>265</v>
       </c>
       <c r="I32" s="139"/>
       <c r="J32" s="139"/>
-      <c r="K32" s="141" t="s">
+      <c r="K32" s="140" t="s">
+        <v>267</v>
+      </c>
+      <c r="L32" s="139"/>
+      <c r="M32" s="141" t="s">
         <v>265</v>
-      </c>
-      <c r="L32" s="139"/>
-      <c r="M32" s="140" t="s">
-        <v>268</v>
       </c>
       <c r="N32" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="O32" s="139" t="s">
+      <c r="O32" s="139"/>
+      <c r="P32" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="P32" s="140" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q32" s="139"/>
+      <c r="Q32" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="R32" s="139"/>
-      <c r="S32" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="S32" s="139"/>
       <c r="T32" s="139"/>
-      <c r="U32" s="141" t="s">
+      <c r="U32" s="139" t="s">
         <v>265</v>
       </c>
       <c r="V32" s="139"/>
       <c r="W32" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="X32" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="X32" s="139"/>
       <c r="Y32" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Z32" s="139" t="s">
+      <c r="Z32" s="139"/>
+      <c r="AA32" s="139"/>
+      <c r="AB32" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AA32" s="139" t="s">
+      <c r="AC32" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="AB32" s="139"/>
-      <c r="AC32" s="140" t="s">
-        <v>268</v>
-      </c>
-      <c r="AD32" s="139"/>
-      <c r="AE32" s="141" t="s">
+      <c r="AD32" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AF32" s="139" t="s">
+      <c r="AE32" s="140" t="s">
+        <v>267</v>
+      </c>
+      <c r="AF32" s="139"/>
+      <c r="AG32" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AG32" s="139"/>
-      <c r="AH32" s="141" t="s">
-        <v>265</v>
-      </c>
+      <c r="AH32" s="139"/>
       <c r="AK32" s="168"/>
       <c r="AL32" s="168"/>
       <c r="AM32" s="168"/>
       <c r="AN32" s="168"/>
     </row>
     <row r="33" spans="2:40">
-      <c r="B33" s="141" t="s">
-        <v>265</v>
+      <c r="B33" s="140" t="s">
+        <v>268</v>
       </c>
       <c r="C33" s="139"/>
-      <c r="D33" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="D33" s="139"/>
       <c r="E33" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="F33" s="139" t="s">
+      <c r="F33" s="139"/>
+      <c r="G33" s="139"/>
+      <c r="H33" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="G33" s="139" t="s">
+      <c r="I33" s="139"/>
+      <c r="J33" s="139"/>
+      <c r="K33" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="H33" s="139"/>
-      <c r="I33" s="139" t="s">
+      <c r="L33" s="139"/>
+      <c r="M33" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="N33" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="J33" s="139"/>
-      <c r="K33" s="140" t="s">
-        <v>267</v>
-      </c>
-      <c r="L33" s="139"/>
-      <c r="M33" s="141" t="s">
+      <c r="O33" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="N33" s="139"/>
-      <c r="O33" s="139"/>
-      <c r="P33" s="139"/>
-      <c r="Q33" s="141" t="s">
+      <c r="P33" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q33" s="139"/>
+      <c r="R33" s="139"/>
+      <c r="S33" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="R33" s="139" t="s">
+      <c r="T33" s="139"/>
+      <c r="U33" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="S33" s="139"/>
-      <c r="T33" s="139" t="s">
+      <c r="V33" s="139"/>
+      <c r="W33" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="U33" s="140" t="s">
-        <v>268</v>
-      </c>
-      <c r="V33" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="W33" s="139"/>
       <c r="X33" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="Y33" s="141" t="s">
+      <c r="Y33" s="139" t="s">
         <v>265</v>
       </c>
       <c r="Z33" s="139" t="s">
@@ -30842,22 +30832,20 @@
       <c r="AA33" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AB33" s="139" t="s">
+      <c r="AB33" s="139"/>
+      <c r="AC33" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD33" s="139"/>
+      <c r="AE33" s="141" t="s">
         <v>265</v>
       </c>
-      <c r="AC33" s="139" t="s">
+      <c r="AF33" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AD33" s="139" t="s">
+      <c r="AG33" s="139"/>
+      <c r="AH33" s="141" t="s">
         <v>265</v>
-      </c>
-      <c r="AE33" s="140" t="s">
-        <v>267</v>
-      </c>
-      <c r="AF33" s="139"/>
-      <c r="AG33" s="139"/>
-      <c r="AH33" s="140" t="s">
-        <v>268</v>
       </c>
       <c r="AK33" s="168"/>
       <c r="AL33" s="168"/>
@@ -30865,70 +30853,82 @@
       <c r="AN33" s="168"/>
     </row>
     <row r="34" spans="2:40">
-      <c r="B34" s="140" t="s">
+      <c r="B34" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="C34" s="139"/>
+      <c r="D34" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="E34" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="F34" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="G34" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="H34" s="139"/>
+      <c r="I34" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="J34" s="139"/>
+      <c r="K34" s="140" t="s">
         <v>267</v>
       </c>
-      <c r="C34" s="139" t="s">
+      <c r="L34" s="139"/>
+      <c r="M34" s="141" t="s">
         <v>265</v>
-      </c>
-      <c r="D34" s="139"/>
-      <c r="E34" s="139"/>
-      <c r="F34" s="139"/>
-      <c r="G34" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="H34" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="I34" s="141" t="s">
-        <v>265</v>
-      </c>
-      <c r="J34" s="139"/>
-      <c r="K34" s="139"/>
-      <c r="L34" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="M34" s="140" t="s">
-        <v>267</v>
       </c>
       <c r="N34" s="139"/>
       <c r="O34" s="139"/>
-      <c r="P34" s="139" t="s">
+      <c r="P34" s="139"/>
+      <c r="Q34" s="141" t="s">
         <v>265</v>
-      </c>
-      <c r="Q34" s="140" t="s">
-        <v>267</v>
       </c>
       <c r="R34" s="139" t="s">
         <v>265</v>
       </c>
       <c r="S34" s="139"/>
-      <c r="T34" s="139"/>
-      <c r="U34" s="139" t="s">
+      <c r="T34" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="V34" s="139"/>
+      <c r="U34" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="V34" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="W34" s="139"/>
-      <c r="X34" s="139"/>
-      <c r="Y34" s="140" t="s">
-        <v>267</v>
-      </c>
-      <c r="Z34" s="139"/>
-      <c r="AA34" s="139"/>
-      <c r="AB34" s="139"/>
+      <c r="X34" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="Y34" s="141" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z34" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AA34" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AB34" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="AC34" s="139" t="s">
         <v>265</v>
       </c>
       <c r="AD34" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AE34" s="139"/>
-      <c r="AF34" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="AE34" s="140" t="s">
+        <v>267</v>
+      </c>
+      <c r="AF34" s="139"/>
       <c r="AG34" s="139"/>
-      <c r="AH34" s="139" t="s">
-        <v>265</v>
+      <c r="AH34" s="140" t="s">
+        <v>268</v>
       </c>
       <c r="AK34" s="168"/>
       <c r="AL34" s="168"/>
@@ -30936,69 +30936,134 @@
       <c r="AN34" s="168"/>
     </row>
     <row r="35" spans="2:40">
-      <c r="B35" s="139"/>
-      <c r="C35" s="139"/>
+      <c r="B35" s="140" t="s">
+        <v>267</v>
+      </c>
+      <c r="C35" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="D35" s="139"/>
       <c r="E35" s="139"/>
       <c r="F35" s="139"/>
-      <c r="G35" s="140" t="s">
-        <v>267</v>
+      <c r="G35" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="H35" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="I35" s="140" t="s">
-        <v>266</v>
+      <c r="I35" s="141" t="s">
+        <v>265</v>
       </c>
       <c r="J35" s="139"/>
       <c r="K35" s="139"/>
-      <c r="L35" s="139"/>
-      <c r="M35" s="139"/>
+      <c r="L35" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="M35" s="140" t="s">
+        <v>267</v>
+      </c>
       <c r="N35" s="139"/>
       <c r="O35" s="139"/>
-      <c r="P35" s="139"/>
-      <c r="Q35" s="139" t="s">
+      <c r="P35" s="139" t="s">
         <v>265</v>
+      </c>
+      <c r="Q35" s="140" t="s">
+        <v>267</v>
       </c>
       <c r="R35" s="139" t="s">
         <v>265</v>
       </c>
       <c r="S35" s="139"/>
-      <c r="T35" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="T35" s="139"/>
       <c r="U35" s="139" t="s">
         <v>265</v>
       </c>
       <c r="V35" s="139"/>
       <c r="W35" s="139"/>
-      <c r="X35" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="Y35" s="139" t="s">
-        <v>265</v>
-      </c>
-      <c r="Z35" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="X35" s="139"/>
+      <c r="Y35" s="140" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z35" s="139"/>
       <c r="AA35" s="139"/>
       <c r="AB35" s="139"/>
       <c r="AC35" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="AD35" s="139"/>
+      <c r="AD35" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="AE35" s="139"/>
       <c r="AF35" s="139" t="s">
         <v>265</v>
       </c>
       <c r="AG35" s="139"/>
-      <c r="AH35" s="139"/>
+      <c r="AH35" s="139" t="s">
+        <v>265</v>
+      </c>
       <c r="AK35" s="168"/>
       <c r="AL35" s="168"/>
       <c r="AM35" s="168"/>
       <c r="AN35" s="168"/>
     </row>
     <row r="36" spans="2:40">
+      <c r="B36" s="139"/>
+      <c r="C36" s="139"/>
+      <c r="D36" s="139"/>
+      <c r="E36" s="139"/>
+      <c r="F36" s="139"/>
+      <c r="G36" s="140" t="s">
+        <v>267</v>
+      </c>
+      <c r="H36" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="I36" s="140" t="s">
+        <v>266</v>
+      </c>
+      <c r="J36" s="139"/>
+      <c r="K36" s="139"/>
+      <c r="L36" s="139"/>
+      <c r="M36" s="139"/>
+      <c r="N36" s="139"/>
+      <c r="O36" s="139"/>
+      <c r="P36" s="139"/>
+      <c r="Q36" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="R36" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="S36" s="139"/>
+      <c r="T36" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="U36" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="V36" s="139"/>
+      <c r="W36" s="139"/>
+      <c r="X36" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="Y36" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z36" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AA36" s="139"/>
+      <c r="AB36" s="139"/>
+      <c r="AC36" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AD36" s="139"/>
+      <c r="AE36" s="139"/>
+      <c r="AF36" s="139" t="s">
+        <v>265</v>
+      </c>
+      <c r="AG36" s="139"/>
+      <c r="AH36" s="139"/>
       <c r="AK36" s="168"/>
       <c r="AL36" s="168"/>
       <c r="AM36" s="168"/>
@@ -31027,6 +31092,12 @@
       <c r="AL40" s="168"/>
       <c r="AM40" s="168"/>
       <c r="AN40" s="168"/>
+    </row>
+    <row r="41" spans="2:40">
+      <c r="AK41" s="168"/>
+      <c r="AL41" s="168"/>
+      <c r="AM41" s="168"/>
+      <c r="AN41" s="168"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor fixes to All and started FMWC DAC ENG
</commit_message>
<xml_diff>
--- a/AllsWellThatEndsExcel_Case_and_Answers.xlsx
+++ b/AllsWellThatEndsExcel_Case_and_Answers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8527F6-038C-43F3-9071-B7E52ACDDC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54379AFF-9186-41A9-BB13-031023E01900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{14CF381A-4175-4F53-B406-22934FD6CEB0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{14CF381A-4175-4F53-B406-22934FD6CEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="16" r:id="rId1"/>
@@ -8527,124 +8527,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="55" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="60" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="60" fillId="7" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="66" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="15" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8745,6 +8631,120 @@
     </xf>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="55" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="60" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="60" fillId="7" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="18" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="66" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="15" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -18548,7 +18548,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4489"/>
+                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4491"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -18616,7 +18616,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4490"/>
+                  <a14:cameraTool cellRange="SecretTab!$F$5:$R$24" spid="_x0000_s4492"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -19246,7 +19246,7 @@
   </sheetPr>
   <dimension ref="A1:N285"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -19270,19 +19270,19 @@
       <c r="A1"/>
     </row>
     <row r="2" spans="1:12" ht="59.25" customHeight="1">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="184" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
-      <c r="I2" s="223"/>
-      <c r="J2" s="223"/>
-      <c r="K2" s="223"/>
-      <c r="L2" s="223"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="185"/>
+      <c r="J2" s="185"/>
+      <c r="K2" s="185"/>
+      <c r="L2" s="185"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" outlineLevel="1">
       <c r="A3"/>
@@ -19299,19 +19299,19 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" ht="75" customHeight="1" outlineLevel="1">
-      <c r="B4" s="224" t="s">
+      <c r="B4" s="186" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
-      <c r="L4" s="224"/>
+      <c r="C4" s="186"/>
+      <c r="D4" s="186"/>
+      <c r="E4" s="186"/>
+      <c r="F4" s="186"/>
+      <c r="G4" s="186"/>
+      <c r="H4" s="186"/>
+      <c r="I4" s="186"/>
+      <c r="J4" s="186"/>
+      <c r="K4" s="186"/>
+      <c r="L4" s="186"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="B5" s="2"/>
@@ -19327,112 +19327,112 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="33" customHeight="1">
-      <c r="B6" s="191" t="s">
+      <c r="B6" s="182" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="192"/>
-      <c r="D6" s="192"/>
-      <c r="E6" s="192"/>
-      <c r="F6" s="192"/>
-      <c r="G6" s="192"/>
-      <c r="H6" s="192"/>
-      <c r="I6" s="225"/>
+      <c r="C6" s="183"/>
+      <c r="D6" s="183"/>
+      <c r="E6" s="183"/>
+      <c r="F6" s="183"/>
+      <c r="G6" s="183"/>
+      <c r="H6" s="183"/>
+      <c r="I6" s="187"/>
       <c r="J6"/>
-      <c r="K6" s="226" t="s">
+      <c r="K6" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="227"/>
+      <c r="L6" s="189"/>
     </row>
     <row r="7" spans="1:12" ht="25.95" customHeight="1">
-      <c r="B7" s="228" t="s">
+      <c r="B7" s="190" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="229"/>
-      <c r="D7" s="229"/>
-      <c r="E7" s="229"/>
-      <c r="F7" s="229"/>
-      <c r="G7" s="229"/>
-      <c r="H7" s="229"/>
-      <c r="I7" s="230"/>
+      <c r="C7" s="191"/>
+      <c r="D7" s="191"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="191"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="192"/>
       <c r="K7" s="5"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="231"/>
-      <c r="C8" s="232"/>
-      <c r="D8" s="232"/>
-      <c r="E8" s="232"/>
-      <c r="F8" s="232"/>
-      <c r="G8" s="232"/>
-      <c r="H8" s="232"/>
-      <c r="I8" s="233"/>
+      <c r="B8" s="193"/>
+      <c r="C8" s="194"/>
+      <c r="D8" s="194"/>
+      <c r="E8" s="194"/>
+      <c r="F8" s="194"/>
+      <c r="G8" s="194"/>
+      <c r="H8" s="194"/>
+      <c r="I8" s="195"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="231"/>
-      <c r="C9" s="232"/>
-      <c r="D9" s="232"/>
-      <c r="E9" s="232"/>
-      <c r="F9" s="232"/>
-      <c r="G9" s="232"/>
-      <c r="H9" s="232"/>
-      <c r="I9" s="233"/>
+      <c r="B9" s="193"/>
+      <c r="C9" s="194"/>
+      <c r="D9" s="194"/>
+      <c r="E9" s="194"/>
+      <c r="F9" s="194"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="194"/>
+      <c r="I9" s="195"/>
       <c r="J9"/>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="B10" s="231"/>
-      <c r="C10" s="232"/>
-      <c r="D10" s="232"/>
-      <c r="E10" s="232"/>
-      <c r="F10" s="232"/>
-      <c r="G10" s="232"/>
-      <c r="H10" s="232"/>
-      <c r="I10" s="233"/>
+      <c r="B10" s="193"/>
+      <c r="C10" s="194"/>
+      <c r="D10" s="194"/>
+      <c r="E10" s="194"/>
+      <c r="F10" s="194"/>
+      <c r="G10" s="194"/>
+      <c r="H10" s="194"/>
+      <c r="I10" s="195"/>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="B11" s="231"/>
-      <c r="C11" s="232"/>
-      <c r="D11" s="232"/>
-      <c r="E11" s="232"/>
-      <c r="F11" s="232"/>
-      <c r="G11" s="232"/>
-      <c r="H11" s="232"/>
-      <c r="I11" s="233"/>
+      <c r="B11" s="193"/>
+      <c r="C11" s="194"/>
+      <c r="D11" s="194"/>
+      <c r="E11" s="194"/>
+      <c r="F11" s="194"/>
+      <c r="G11" s="194"/>
+      <c r="H11" s="194"/>
+      <c r="I11" s="195"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="B12" s="231"/>
-      <c r="C12" s="232"/>
-      <c r="D12" s="232"/>
-      <c r="E12" s="232"/>
-      <c r="F12" s="232"/>
-      <c r="G12" s="232"/>
-      <c r="H12" s="232"/>
-      <c r="I12" s="233"/>
+      <c r="B12" s="193"/>
+      <c r="C12" s="194"/>
+      <c r="D12" s="194"/>
+      <c r="E12" s="194"/>
+      <c r="F12" s="194"/>
+      <c r="G12" s="194"/>
+      <c r="H12" s="194"/>
+      <c r="I12" s="195"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:12" ht="23.25" customHeight="1">
-      <c r="B13" s="231"/>
-      <c r="C13" s="232"/>
-      <c r="D13" s="232"/>
-      <c r="E13" s="232"/>
-      <c r="F13" s="232"/>
-      <c r="G13" s="232"/>
-      <c r="H13" s="232"/>
-      <c r="I13" s="233"/>
+      <c r="B13" s="193"/>
+      <c r="C13" s="194"/>
+      <c r="D13" s="194"/>
+      <c r="E13" s="194"/>
+      <c r="F13" s="194"/>
+      <c r="G13" s="194"/>
+      <c r="H13" s="194"/>
+      <c r="I13" s="195"/>
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:12" ht="33" customHeight="1">
-      <c r="B14" s="234"/>
-      <c r="C14" s="235"/>
-      <c r="D14" s="235"/>
-      <c r="E14" s="235"/>
-      <c r="F14" s="235"/>
-      <c r="G14" s="235"/>
-      <c r="H14" s="235"/>
-      <c r="I14" s="236"/>
+      <c r="B14" s="196"/>
+      <c r="C14" s="197"/>
+      <c r="D14" s="197"/>
+      <c r="E14" s="197"/>
+      <c r="F14" s="197"/>
+      <c r="G14" s="197"/>
+      <c r="H14" s="197"/>
+      <c r="I14" s="198"/>
       <c r="K14" s="34" t="s">
         <v>0</v>
       </c>
@@ -19446,60 +19446,60 @@
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B16" s="191" t="s">
+      <c r="B16" s="182" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="192"/>
-      <c r="D16" s="192"/>
-      <c r="E16" s="192"/>
-      <c r="F16" s="192"/>
-      <c r="G16" s="192"/>
-      <c r="H16" s="192"/>
-      <c r="I16" s="192"/>
-      <c r="J16" s="192"/>
-      <c r="K16" s="192"/>
-      <c r="L16" s="192"/>
+      <c r="C16" s="183"/>
+      <c r="D16" s="183"/>
+      <c r="E16" s="183"/>
+      <c r="F16" s="183"/>
+      <c r="G16" s="183"/>
+      <c r="H16" s="183"/>
+      <c r="I16" s="183"/>
+      <c r="J16" s="183"/>
+      <c r="K16" s="183"/>
+      <c r="L16" s="183"/>
     </row>
     <row r="17" spans="1:13" ht="43.2" customHeight="1">
-      <c r="B17" s="237" t="s">
+      <c r="B17" s="199" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="238"/>
-      <c r="D17" s="238"/>
-      <c r="E17" s="238"/>
-      <c r="F17" s="238"/>
-      <c r="G17" s="238"/>
-      <c r="H17" s="238"/>
-      <c r="I17" s="238"/>
-      <c r="J17" s="238"/>
-      <c r="K17" s="238"/>
-      <c r="L17" s="239"/>
+      <c r="C17" s="200"/>
+      <c r="D17" s="200"/>
+      <c r="E17" s="200"/>
+      <c r="F17" s="200"/>
+      <c r="G17" s="200"/>
+      <c r="H17" s="200"/>
+      <c r="I17" s="200"/>
+      <c r="J17" s="200"/>
+      <c r="K17" s="200"/>
+      <c r="L17" s="201"/>
     </row>
     <row r="18" spans="1:13" ht="43.2" customHeight="1">
-      <c r="B18" s="240"/>
-      <c r="C18" s="241"/>
-      <c r="D18" s="241"/>
-      <c r="E18" s="241"/>
-      <c r="F18" s="241"/>
-      <c r="G18" s="241"/>
-      <c r="H18" s="241"/>
-      <c r="I18" s="241"/>
-      <c r="J18" s="241"/>
-      <c r="K18" s="241"/>
-      <c r="L18" s="242"/>
+      <c r="B18" s="202"/>
+      <c r="C18" s="203"/>
+      <c r="D18" s="203"/>
+      <c r="E18" s="203"/>
+      <c r="F18" s="203"/>
+      <c r="G18" s="203"/>
+      <c r="H18" s="203"/>
+      <c r="I18" s="203"/>
+      <c r="J18" s="203"/>
+      <c r="K18" s="203"/>
+      <c r="L18" s="204"/>
     </row>
     <row r="19" spans="1:13" ht="43.2" customHeight="1">
-      <c r="B19" s="243"/>
-      <c r="C19" s="244"/>
-      <c r="D19" s="244"/>
-      <c r="E19" s="244"/>
-      <c r="F19" s="244"/>
-      <c r="G19" s="244"/>
-      <c r="H19" s="244"/>
-      <c r="I19" s="244"/>
-      <c r="J19" s="244"/>
-      <c r="K19" s="244"/>
-      <c r="L19" s="245"/>
+      <c r="B19" s="205"/>
+      <c r="C19" s="206"/>
+      <c r="D19" s="206"/>
+      <c r="E19" s="206"/>
+      <c r="F19" s="206"/>
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206"/>
+      <c r="J19" s="206"/>
+      <c r="K19" s="206"/>
+      <c r="L19" s="207"/>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1">
       <c r="B20" s="8"/>
@@ -19515,19 +19515,19 @@
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:13" ht="21.75" customHeight="1">
-      <c r="B21" s="191" t="s">
+      <c r="B21" s="182" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="192"/>
-      <c r="D21" s="192"/>
-      <c r="E21" s="192"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="192"/>
-      <c r="H21" s="192"/>
-      <c r="I21" s="192"/>
-      <c r="J21" s="192"/>
-      <c r="K21" s="192"/>
-      <c r="L21" s="192"/>
+      <c r="C21" s="183"/>
+      <c r="D21" s="183"/>
+      <c r="E21" s="183"/>
+      <c r="F21" s="183"/>
+      <c r="G21" s="183"/>
+      <c r="H21" s="183"/>
+      <c r="I21" s="183"/>
+      <c r="J21" s="183"/>
+      <c r="K21" s="183"/>
+      <c r="L21" s="183"/>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1">
       <c r="B22" s="9"/>
@@ -19611,14 +19611,14 @@
         <f>IF(ISBLANK(E26),0,IF(E26=Answers!E26,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G26" s="246" t="s">
+      <c r="G26" s="208" t="s">
         <v>187</v>
       </c>
-      <c r="H26" s="247"/>
-      <c r="I26" s="247"/>
-      <c r="J26" s="247"/>
-      <c r="K26" s="247"/>
-      <c r="L26" s="248"/>
+      <c r="H26" s="209"/>
+      <c r="I26" s="209"/>
+      <c r="J26" s="209"/>
+      <c r="K26" s="209"/>
+      <c r="L26" s="210"/>
       <c r="M26" t="s">
         <v>376</v>
       </c>
@@ -19640,14 +19640,14 @@
         <f>IF(ISBLANK(E27),0,IF(E27=Answers!E27,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G27" s="249" t="s">
+      <c r="G27" s="211" t="s">
         <v>186</v>
       </c>
-      <c r="H27" s="250"/>
-      <c r="I27" s="250"/>
-      <c r="J27" s="250"/>
-      <c r="K27" s="250"/>
-      <c r="L27" s="251"/>
+      <c r="H27" s="212"/>
+      <c r="I27" s="212"/>
+      <c r="J27" s="212"/>
+      <c r="K27" s="212"/>
+      <c r="L27" s="213"/>
       <c r="M27" t="s">
         <v>377</v>
       </c>
@@ -19669,14 +19669,14 @@
         <f>IF(ISBLANK(E28),0,IF(E28=Answers!E28,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G28" s="252" t="s">
+      <c r="G28" s="214" t="s">
         <v>345</v>
       </c>
-      <c r="H28" s="253"/>
-      <c r="I28" s="253"/>
-      <c r="J28" s="253"/>
-      <c r="K28" s="253"/>
-      <c r="L28" s="254"/>
+      <c r="H28" s="215"/>
+      <c r="I28" s="215"/>
+      <c r="J28" s="215"/>
+      <c r="K28" s="215"/>
+      <c r="L28" s="216"/>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1">
       <c r="B29" s="2"/>
@@ -19692,19 +19692,19 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:13">
-      <c r="B30" s="191" t="s">
+      <c r="B30" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="192"/>
-      <c r="D30" s="192"/>
-      <c r="E30" s="192"/>
-      <c r="F30" s="192"/>
-      <c r="G30" s="192"/>
-      <c r="H30" s="192"/>
-      <c r="I30" s="192"/>
-      <c r="J30" s="192"/>
-      <c r="K30" s="192"/>
-      <c r="L30" s="192"/>
+      <c r="C30" s="183"/>
+      <c r="D30" s="183"/>
+      <c r="E30" s="183"/>
+      <c r="F30" s="183"/>
+      <c r="G30" s="183"/>
+      <c r="H30" s="183"/>
+      <c r="I30" s="183"/>
+      <c r="J30" s="183"/>
+      <c r="K30" s="183"/>
+      <c r="L30" s="183"/>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1" thickBot="1">
       <c r="B31" s="16"/>
@@ -19734,10 +19734,10 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
-      <c r="K32" s="191" t="s">
+      <c r="K32" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="L32" s="192"/>
+      <c r="L32" s="183"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1">
       <c r="A33" s="13"/>
@@ -19750,11 +19750,11 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
-      <c r="K33" s="193" cm="1">
+      <c r="K33" s="226" cm="1">
         <f t="array" ref="K33">SUMPRODUCT(--($F$26:$F$276=1),$D$26:$D$276)</f>
         <v>750</v>
       </c>
-      <c r="L33" s="194"/>
+      <c r="L33" s="227"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1">
       <c r="A34"/>
@@ -19769,8 +19769,8 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
-      <c r="K34" s="195"/>
-      <c r="L34" s="196"/>
+      <c r="K34" s="228"/>
+      <c r="L34" s="229"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1">
       <c r="A35" s="13"/>
@@ -19785,8 +19785,8 @@
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
-      <c r="K35" s="195"/>
-      <c r="L35" s="196"/>
+      <c r="K35" s="228"/>
+      <c r="L35" s="229"/>
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1">
       <c r="A36" s="13"/>
@@ -19799,8 +19799,8 @@
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
-      <c r="K36" s="197"/>
-      <c r="L36" s="198"/>
+      <c r="K36" s="230"/>
+      <c r="L36" s="231"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1">
       <c r="A37" s="13"/>
@@ -19939,10 +19939,10 @@
         <v>122</v>
       </c>
       <c r="F45" s="18"/>
-      <c r="G45" s="199" t="s">
+      <c r="G45" s="232" t="s">
         <v>324</v>
       </c>
-      <c r="H45" s="200"/>
+      <c r="H45" s="233"/>
       <c r="I45" s="91" t="s">
         <v>52</v>
       </c>
@@ -20401,14 +20401,14 @@
       <c r="F63" s="18"/>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
-      <c r="I63" s="201" t="s">
+      <c r="I63" s="234" t="s">
         <v>138</v>
       </c>
-      <c r="J63" s="202"/>
-      <c r="K63" s="205" t="s">
+      <c r="J63" s="235"/>
+      <c r="K63" s="238" t="s">
         <v>141</v>
       </c>
-      <c r="L63" s="206"/>
+      <c r="L63" s="239"/>
     </row>
     <row r="64" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A64" s="13"/>
@@ -20421,10 +20421,10 @@
       <c r="F64" s="18"/>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
-      <c r="I64" s="203"/>
-      <c r="J64" s="204"/>
-      <c r="K64" s="207"/>
-      <c r="L64" s="208"/>
+      <c r="I64" s="236"/>
+      <c r="J64" s="237"/>
+      <c r="K64" s="240"/>
+      <c r="L64" s="241"/>
     </row>
     <row r="65" spans="1:14" ht="15" customHeight="1">
       <c r="A65" s="13"/>
@@ -20628,12 +20628,12 @@
       </c>
       <c r="F75" s="18"/>
       <c r="G75" s="13"/>
-      <c r="H75" s="209" t="s">
+      <c r="H75" s="242" t="s">
         <v>136</v>
       </c>
-      <c r="I75" s="210"/>
-      <c r="J75" s="210"/>
-      <c r="K75" s="211"/>
+      <c r="I75" s="243"/>
+      <c r="J75" s="243"/>
+      <c r="K75" s="244"/>
       <c r="L75" s="174" t="s">
         <v>135</v>
       </c>
@@ -21355,119 +21355,119 @@
       <c r="L99" s="20"/>
     </row>
     <row r="100" spans="1:13">
-      <c r="B100" s="191" t="s">
+      <c r="B100" s="182" t="s">
         <v>21</v>
       </c>
-      <c r="C100" s="192"/>
-      <c r="D100" s="192"/>
-      <c r="E100" s="192"/>
-      <c r="F100" s="192"/>
-      <c r="G100" s="192"/>
-      <c r="H100" s="192"/>
-      <c r="I100" s="192"/>
-      <c r="J100" s="192"/>
-      <c r="K100" s="192"/>
-      <c r="L100" s="192"/>
+      <c r="C100" s="183"/>
+      <c r="D100" s="183"/>
+      <c r="E100" s="183"/>
+      <c r="F100" s="183"/>
+      <c r="G100" s="183"/>
+      <c r="H100" s="183"/>
+      <c r="I100" s="183"/>
+      <c r="J100" s="183"/>
+      <c r="K100" s="183"/>
+      <c r="L100" s="183"/>
     </row>
     <row r="101" spans="1:13" ht="15" customHeight="1">
       <c r="A101" s="13"/>
-      <c r="B101" s="182" t="s">
+      <c r="B101" s="217" t="s">
         <v>198</v>
       </c>
-      <c r="C101" s="212"/>
-      <c r="D101" s="212"/>
-      <c r="E101" s="212"/>
-      <c r="F101" s="212"/>
-      <c r="G101" s="212"/>
-      <c r="H101" s="212"/>
-      <c r="I101" s="212"/>
-      <c r="J101" s="212"/>
-      <c r="K101" s="212"/>
-      <c r="L101" s="213"/>
+      <c r="C101" s="245"/>
+      <c r="D101" s="245"/>
+      <c r="E101" s="245"/>
+      <c r="F101" s="245"/>
+      <c r="G101" s="245"/>
+      <c r="H101" s="245"/>
+      <c r="I101" s="245"/>
+      <c r="J101" s="245"/>
+      <c r="K101" s="245"/>
+      <c r="L101" s="246"/>
     </row>
     <row r="102" spans="1:13" ht="15" customHeight="1">
       <c r="A102" s="13"/>
-      <c r="B102" s="214"/>
-      <c r="C102" s="215"/>
-      <c r="D102" s="215"/>
-      <c r="E102" s="215"/>
-      <c r="F102" s="215"/>
-      <c r="G102" s="215"/>
-      <c r="H102" s="215"/>
-      <c r="I102" s="215"/>
-      <c r="J102" s="215"/>
-      <c r="K102" s="215"/>
-      <c r="L102" s="216"/>
+      <c r="B102" s="247"/>
+      <c r="C102" s="248"/>
+      <c r="D102" s="248"/>
+      <c r="E102" s="248"/>
+      <c r="F102" s="248"/>
+      <c r="G102" s="248"/>
+      <c r="H102" s="248"/>
+      <c r="I102" s="248"/>
+      <c r="J102" s="248"/>
+      <c r="K102" s="248"/>
+      <c r="L102" s="249"/>
     </row>
     <row r="103" spans="1:13" ht="15" customHeight="1">
       <c r="A103" s="13"/>
-      <c r="B103" s="214"/>
-      <c r="C103" s="215"/>
-      <c r="D103" s="215"/>
-      <c r="E103" s="215"/>
-      <c r="F103" s="215"/>
-      <c r="G103" s="215"/>
-      <c r="H103" s="215"/>
-      <c r="I103" s="215"/>
-      <c r="J103" s="215"/>
-      <c r="K103" s="215"/>
-      <c r="L103" s="216"/>
+      <c r="B103" s="247"/>
+      <c r="C103" s="248"/>
+      <c r="D103" s="248"/>
+      <c r="E103" s="248"/>
+      <c r="F103" s="248"/>
+      <c r="G103" s="248"/>
+      <c r="H103" s="248"/>
+      <c r="I103" s="248"/>
+      <c r="J103" s="248"/>
+      <c r="K103" s="248"/>
+      <c r="L103" s="249"/>
     </row>
     <row r="104" spans="1:13" ht="15" customHeight="1">
       <c r="A104" s="13"/>
-      <c r="B104" s="214"/>
-      <c r="C104" s="215"/>
-      <c r="D104" s="215"/>
-      <c r="E104" s="215"/>
-      <c r="F104" s="215"/>
-      <c r="G104" s="215"/>
-      <c r="H104" s="215"/>
-      <c r="I104" s="215"/>
-      <c r="J104" s="215"/>
-      <c r="K104" s="215"/>
-      <c r="L104" s="216"/>
+      <c r="B104" s="247"/>
+      <c r="C104" s="248"/>
+      <c r="D104" s="248"/>
+      <c r="E104" s="248"/>
+      <c r="F104" s="248"/>
+      <c r="G104" s="248"/>
+      <c r="H104" s="248"/>
+      <c r="I104" s="248"/>
+      <c r="J104" s="248"/>
+      <c r="K104" s="248"/>
+      <c r="L104" s="249"/>
     </row>
     <row r="105" spans="1:13" ht="15" customHeight="1">
       <c r="A105" s="13"/>
-      <c r="B105" s="214"/>
-      <c r="C105" s="215"/>
-      <c r="D105" s="215"/>
-      <c r="E105" s="215"/>
-      <c r="F105" s="215"/>
-      <c r="G105" s="215"/>
-      <c r="H105" s="215"/>
-      <c r="I105" s="215"/>
-      <c r="J105" s="215"/>
-      <c r="K105" s="215"/>
-      <c r="L105" s="216"/>
+      <c r="B105" s="247"/>
+      <c r="C105" s="248"/>
+      <c r="D105" s="248"/>
+      <c r="E105" s="248"/>
+      <c r="F105" s="248"/>
+      <c r="G105" s="248"/>
+      <c r="H105" s="248"/>
+      <c r="I105" s="248"/>
+      <c r="J105" s="248"/>
+      <c r="K105" s="248"/>
+      <c r="L105" s="249"/>
     </row>
     <row r="106" spans="1:13" ht="15" customHeight="1">
       <c r="A106" s="13"/>
-      <c r="B106" s="214"/>
-      <c r="C106" s="215"/>
-      <c r="D106" s="215"/>
-      <c r="E106" s="215"/>
-      <c r="F106" s="215"/>
-      <c r="G106" s="215"/>
-      <c r="H106" s="215"/>
-      <c r="I106" s="215"/>
-      <c r="J106" s="215"/>
-      <c r="K106" s="215"/>
-      <c r="L106" s="216"/>
+      <c r="B106" s="247"/>
+      <c r="C106" s="248"/>
+      <c r="D106" s="248"/>
+      <c r="E106" s="248"/>
+      <c r="F106" s="248"/>
+      <c r="G106" s="248"/>
+      <c r="H106" s="248"/>
+      <c r="I106" s="248"/>
+      <c r="J106" s="248"/>
+      <c r="K106" s="248"/>
+      <c r="L106" s="249"/>
     </row>
     <row r="107" spans="1:13" ht="15" customHeight="1">
       <c r="A107" s="13"/>
-      <c r="B107" s="217"/>
-      <c r="C107" s="218"/>
-      <c r="D107" s="218"/>
-      <c r="E107" s="218"/>
-      <c r="F107" s="218"/>
-      <c r="G107" s="218"/>
-      <c r="H107" s="218"/>
-      <c r="I107" s="218"/>
-      <c r="J107" s="218"/>
-      <c r="K107" s="218"/>
-      <c r="L107" s="219"/>
+      <c r="B107" s="250"/>
+      <c r="C107" s="251"/>
+      <c r="D107" s="251"/>
+      <c r="E107" s="251"/>
+      <c r="F107" s="251"/>
+      <c r="G107" s="251"/>
+      <c r="H107" s="251"/>
+      <c r="I107" s="251"/>
+      <c r="J107" s="251"/>
+      <c r="K107" s="251"/>
+      <c r="L107" s="252"/>
     </row>
     <row r="108" spans="1:13" ht="15" customHeight="1">
       <c r="A108" s="13"/>
@@ -21484,19 +21484,19 @@
       <c r="L108" s="20"/>
     </row>
     <row r="109" spans="1:13">
-      <c r="B109" s="191" t="s">
+      <c r="B109" s="182" t="s">
         <v>118</v>
       </c>
-      <c r="C109" s="192"/>
-      <c r="D109" s="192"/>
-      <c r="E109" s="192"/>
-      <c r="F109" s="192"/>
-      <c r="G109" s="192"/>
-      <c r="H109" s="192"/>
-      <c r="I109" s="192"/>
-      <c r="J109" s="192"/>
-      <c r="K109" s="192"/>
-      <c r="L109" s="192"/>
+      <c r="C109" s="183"/>
+      <c r="D109" s="183"/>
+      <c r="E109" s="183"/>
+      <c r="F109" s="183"/>
+      <c r="G109" s="183"/>
+      <c r="H109" s="183"/>
+      <c r="I109" s="183"/>
+      <c r="J109" s="183"/>
+      <c r="K109" s="183"/>
+      <c r="L109" s="183"/>
     </row>
     <row r="110" spans="1:13" ht="15" customHeight="1">
       <c r="A110" s="13"/>
@@ -21620,8 +21620,8 @@
     </row>
     <row r="118" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A118" s="13"/>
-      <c r="B118" s="220"/>
-      <c r="C118" s="221"/>
+      <c r="B118" s="253"/>
+      <c r="C118" s="254"/>
       <c r="D118" s="63"/>
       <c r="E118" s="63"/>
       <c r="F118" s="62"/>
@@ -21634,8 +21634,8 @@
     </row>
     <row r="119" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A119" s="13"/>
-      <c r="B119" s="220"/>
-      <c r="C119" s="221"/>
+      <c r="B119" s="253"/>
+      <c r="C119" s="254"/>
       <c r="D119" s="63"/>
       <c r="E119" s="63"/>
       <c r="F119" s="62"/>
@@ -25172,128 +25172,140 @@
       <c r="L276" s="27"/>
     </row>
     <row r="277" spans="1:12">
-      <c r="B277" s="191" t="s">
+      <c r="B277" s="182" t="s">
         <v>22</v>
       </c>
-      <c r="C277" s="192"/>
-      <c r="D277" s="192"/>
-      <c r="E277" s="192"/>
-      <c r="F277" s="192"/>
-      <c r="G277" s="192"/>
-      <c r="H277" s="192"/>
-      <c r="I277" s="192"/>
-      <c r="J277" s="192"/>
-      <c r="K277" s="192"/>
-      <c r="L277" s="192"/>
+      <c r="C277" s="183"/>
+      <c r="D277" s="183"/>
+      <c r="E277" s="183"/>
+      <c r="F277" s="183"/>
+      <c r="G277" s="183"/>
+      <c r="H277" s="183"/>
+      <c r="I277" s="183"/>
+      <c r="J277" s="183"/>
+      <c r="K277" s="183"/>
+      <c r="L277" s="183"/>
     </row>
     <row r="278" spans="1:12">
-      <c r="B278" s="182" t="s">
+      <c r="B278" s="217" t="s">
         <v>317</v>
       </c>
-      <c r="C278" s="183"/>
-      <c r="D278" s="183"/>
-      <c r="E278" s="183"/>
-      <c r="F278" s="183"/>
-      <c r="G278" s="183"/>
-      <c r="H278" s="183"/>
-      <c r="I278" s="183"/>
-      <c r="J278" s="183"/>
-      <c r="K278" s="183"/>
-      <c r="L278" s="184"/>
+      <c r="C278" s="218"/>
+      <c r="D278" s="218"/>
+      <c r="E278" s="218"/>
+      <c r="F278" s="218"/>
+      <c r="G278" s="218"/>
+      <c r="H278" s="218"/>
+      <c r="I278" s="218"/>
+      <c r="J278" s="218"/>
+      <c r="K278" s="218"/>
+      <c r="L278" s="219"/>
     </row>
     <row r="279" spans="1:12">
-      <c r="B279" s="185"/>
-      <c r="C279" s="186"/>
-      <c r="D279" s="186"/>
-      <c r="E279" s="186"/>
-      <c r="F279" s="186"/>
-      <c r="G279" s="186"/>
-      <c r="H279" s="186"/>
-      <c r="I279" s="186"/>
-      <c r="J279" s="186"/>
-      <c r="K279" s="186"/>
-      <c r="L279" s="187"/>
+      <c r="B279" s="220"/>
+      <c r="C279" s="221"/>
+      <c r="D279" s="221"/>
+      <c r="E279" s="221"/>
+      <c r="F279" s="221"/>
+      <c r="G279" s="221"/>
+      <c r="H279" s="221"/>
+      <c r="I279" s="221"/>
+      <c r="J279" s="221"/>
+      <c r="K279" s="221"/>
+      <c r="L279" s="222"/>
     </row>
     <row r="280" spans="1:12">
-      <c r="B280" s="185"/>
-      <c r="C280" s="186"/>
-      <c r="D280" s="186"/>
-      <c r="E280" s="186"/>
-      <c r="F280" s="186"/>
-      <c r="G280" s="186"/>
-      <c r="H280" s="186"/>
-      <c r="I280" s="186"/>
-      <c r="J280" s="186"/>
-      <c r="K280" s="186"/>
-      <c r="L280" s="187"/>
+      <c r="B280" s="220"/>
+      <c r="C280" s="221"/>
+      <c r="D280" s="221"/>
+      <c r="E280" s="221"/>
+      <c r="F280" s="221"/>
+      <c r="G280" s="221"/>
+      <c r="H280" s="221"/>
+      <c r="I280" s="221"/>
+      <c r="J280" s="221"/>
+      <c r="K280" s="221"/>
+      <c r="L280" s="222"/>
     </row>
     <row r="281" spans="1:12">
-      <c r="B281" s="185"/>
-      <c r="C281" s="186"/>
-      <c r="D281" s="186"/>
-      <c r="E281" s="186"/>
-      <c r="F281" s="186"/>
-      <c r="G281" s="186"/>
-      <c r="H281" s="186"/>
-      <c r="I281" s="186"/>
-      <c r="J281" s="186"/>
-      <c r="K281" s="186"/>
-      <c r="L281" s="187"/>
+      <c r="B281" s="220"/>
+      <c r="C281" s="221"/>
+      <c r="D281" s="221"/>
+      <c r="E281" s="221"/>
+      <c r="F281" s="221"/>
+      <c r="G281" s="221"/>
+      <c r="H281" s="221"/>
+      <c r="I281" s="221"/>
+      <c r="J281" s="221"/>
+      <c r="K281" s="221"/>
+      <c r="L281" s="222"/>
     </row>
     <row r="282" spans="1:12">
-      <c r="B282" s="185"/>
-      <c r="C282" s="186"/>
-      <c r="D282" s="186"/>
-      <c r="E282" s="186"/>
-      <c r="F282" s="186"/>
-      <c r="G282" s="186"/>
-      <c r="H282" s="186"/>
-      <c r="I282" s="186"/>
-      <c r="J282" s="186"/>
-      <c r="K282" s="186"/>
-      <c r="L282" s="187"/>
+      <c r="B282" s="220"/>
+      <c r="C282" s="221"/>
+      <c r="D282" s="221"/>
+      <c r="E282" s="221"/>
+      <c r="F282" s="221"/>
+      <c r="G282" s="221"/>
+      <c r="H282" s="221"/>
+      <c r="I282" s="221"/>
+      <c r="J282" s="221"/>
+      <c r="K282" s="221"/>
+      <c r="L282" s="222"/>
     </row>
     <row r="283" spans="1:12">
-      <c r="B283" s="185"/>
-      <c r="C283" s="186"/>
-      <c r="D283" s="186"/>
-      <c r="E283" s="186"/>
-      <c r="F283" s="186"/>
-      <c r="G283" s="186"/>
-      <c r="H283" s="186"/>
-      <c r="I283" s="186"/>
-      <c r="J283" s="186"/>
-      <c r="K283" s="186"/>
-      <c r="L283" s="187"/>
+      <c r="B283" s="220"/>
+      <c r="C283" s="221"/>
+      <c r="D283" s="221"/>
+      <c r="E283" s="221"/>
+      <c r="F283" s="221"/>
+      <c r="G283" s="221"/>
+      <c r="H283" s="221"/>
+      <c r="I283" s="221"/>
+      <c r="J283" s="221"/>
+      <c r="K283" s="221"/>
+      <c r="L283" s="222"/>
     </row>
     <row r="284" spans="1:12">
-      <c r="B284" s="185"/>
-      <c r="C284" s="186"/>
-      <c r="D284" s="186"/>
-      <c r="E284" s="186"/>
-      <c r="F284" s="186"/>
-      <c r="G284" s="186"/>
-      <c r="H284" s="186"/>
-      <c r="I284" s="186"/>
-      <c r="J284" s="186"/>
-      <c r="K284" s="186"/>
-      <c r="L284" s="187"/>
+      <c r="B284" s="220"/>
+      <c r="C284" s="221"/>
+      <c r="D284" s="221"/>
+      <c r="E284" s="221"/>
+      <c r="F284" s="221"/>
+      <c r="G284" s="221"/>
+      <c r="H284" s="221"/>
+      <c r="I284" s="221"/>
+      <c r="J284" s="221"/>
+      <c r="K284" s="221"/>
+      <c r="L284" s="222"/>
     </row>
     <row r="285" spans="1:12">
-      <c r="B285" s="188"/>
-      <c r="C285" s="189"/>
-      <c r="D285" s="189"/>
-      <c r="E285" s="189"/>
-      <c r="F285" s="189"/>
-      <c r="G285" s="189"/>
-      <c r="H285" s="189"/>
-      <c r="I285" s="189"/>
-      <c r="J285" s="189"/>
-      <c r="K285" s="189"/>
-      <c r="L285" s="190"/>
+      <c r="B285" s="223"/>
+      <c r="C285" s="224"/>
+      <c r="D285" s="224"/>
+      <c r="E285" s="224"/>
+      <c r="F285" s="224"/>
+      <c r="G285" s="224"/>
+      <c r="H285" s="224"/>
+      <c r="I285" s="224"/>
+      <c r="J285" s="224"/>
+      <c r="K285" s="224"/>
+      <c r="L285" s="225"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B278:L285"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L36"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I63:J64"/>
+    <mergeCell ref="K63:L64"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="B100:L100"/>
+    <mergeCell ref="B101:L107"/>
+    <mergeCell ref="B109:L109"/>
+    <mergeCell ref="B118:C119"/>
+    <mergeCell ref="B277:L277"/>
     <mergeCell ref="B30:L30"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B4:L4"/>
@@ -25306,18 +25318,6 @@
     <mergeCell ref="G26:L26"/>
     <mergeCell ref="G27:L27"/>
     <mergeCell ref="G28:L28"/>
-    <mergeCell ref="B278:L285"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L36"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I63:J64"/>
-    <mergeCell ref="K63:L64"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="B100:L100"/>
-    <mergeCell ref="B101:L107"/>
-    <mergeCell ref="B109:L109"/>
-    <mergeCell ref="B118:C119"/>
-    <mergeCell ref="B277:L277"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -25373,15 +25373,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="22.8">
-      <c r="B2" s="191" t="s">
+      <c r="B2" s="182" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
-      <c r="G2" s="192"/>
-      <c r="H2" s="192"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="177" t="s">
@@ -25671,15 +25671,15 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="22.8">
-      <c r="B18" s="191" t="s">
+      <c r="B18" s="182" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="192"/>
-      <c r="D18" s="192"/>
-      <c r="E18" s="192"/>
-      <c r="F18" s="192"/>
-      <c r="G18" s="192"/>
-      <c r="H18" s="192"/>
+      <c r="C18" s="183"/>
+      <c r="D18" s="183"/>
+      <c r="E18" s="183"/>
+      <c r="F18" s="183"/>
+      <c r="G18" s="183"/>
+      <c r="H18" s="183"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="U5:X14">
@@ -28139,8 +28139,8 @@
   </sheetPr>
   <dimension ref="A1:AN41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="25.2" zeroHeight="1"/>
@@ -28354,14 +28354,8 @@
       <c r="V5" s="140"/>
       <c r="W5" s="140"/>
       <c r="X5" s="140"/>
-      <c r="Y5" s="140" cm="1">
-        <f t="array" ref="Y5">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(AB$15:AB$36))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(AB$15:AB$36,$AK$8:$AK$14,$AM$8:$AM$14,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>13</v>
-      </c>
-      <c r="Z5" s="140" cm="1">
-        <f t="array" ref="Z5">_xlfn.LET(_xlpm.z,TRANSPOSE(ROW(AF$15:AF$36))-_xlfn.TOROW(3*(_xlfn.XLOOKUP(AF$15:AF$36,$AK$8:$AK$14,$AM$8:$AM$14,NA()))),_xlfn._xlws.FILTER(_xlpm.z,ISNUMBER(_xlpm.z)))</f>
-        <v>10</v>
-      </c>
+      <c r="Y5" s="140"/>
+      <c r="Z5" s="140"/>
       <c r="AA5" s="140"/>
       <c r="AB5" s="140"/>
       <c r="AC5" s="140"/>
@@ -31138,19 +31132,19 @@
       <c r="A1"/>
     </row>
     <row r="2" spans="1:12" ht="59.25" customHeight="1">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="184" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
-      <c r="I2" s="223"/>
-      <c r="J2" s="223"/>
-      <c r="K2" s="223"/>
-      <c r="L2" s="223"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="185"/>
+      <c r="J2" s="185"/>
+      <c r="K2" s="185"/>
+      <c r="L2" s="185"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" outlineLevel="1">
       <c r="A3"/>
@@ -31167,19 +31161,19 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" ht="75" customHeight="1" outlineLevel="1">
-      <c r="B4" s="224" t="s">
+      <c r="B4" s="186" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
-      <c r="L4" s="224"/>
+      <c r="C4" s="186"/>
+      <c r="D4" s="186"/>
+      <c r="E4" s="186"/>
+      <c r="F4" s="186"/>
+      <c r="G4" s="186"/>
+      <c r="H4" s="186"/>
+      <c r="I4" s="186"/>
+      <c r="J4" s="186"/>
+      <c r="K4" s="186"/>
+      <c r="L4" s="186"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="B5" s="2"/>
@@ -31195,112 +31189,112 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="33" customHeight="1">
-      <c r="B6" s="191" t="s">
+      <c r="B6" s="182" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="192"/>
-      <c r="D6" s="192"/>
-      <c r="E6" s="192"/>
-      <c r="F6" s="192"/>
-      <c r="G6" s="192"/>
-      <c r="H6" s="192"/>
-      <c r="I6" s="225"/>
+      <c r="C6" s="183"/>
+      <c r="D6" s="183"/>
+      <c r="E6" s="183"/>
+      <c r="F6" s="183"/>
+      <c r="G6" s="183"/>
+      <c r="H6" s="183"/>
+      <c r="I6" s="187"/>
       <c r="J6"/>
-      <c r="K6" s="226" t="s">
+      <c r="K6" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="227"/>
+      <c r="L6" s="189"/>
     </row>
     <row r="7" spans="1:12" ht="25.95" customHeight="1">
-      <c r="B7" s="228" t="s">
+      <c r="B7" s="190" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="229"/>
-      <c r="D7" s="229"/>
-      <c r="E7" s="229"/>
-      <c r="F7" s="229"/>
-      <c r="G7" s="229"/>
-      <c r="H7" s="229"/>
-      <c r="I7" s="230"/>
+      <c r="C7" s="191"/>
+      <c r="D7" s="191"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="191"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="192"/>
       <c r="K7" s="5"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="231"/>
-      <c r="C8" s="232"/>
-      <c r="D8" s="232"/>
-      <c r="E8" s="232"/>
-      <c r="F8" s="232"/>
-      <c r="G8" s="232"/>
-      <c r="H8" s="232"/>
-      <c r="I8" s="233"/>
+      <c r="B8" s="193"/>
+      <c r="C8" s="194"/>
+      <c r="D8" s="194"/>
+      <c r="E8" s="194"/>
+      <c r="F8" s="194"/>
+      <c r="G8" s="194"/>
+      <c r="H8" s="194"/>
+      <c r="I8" s="195"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="231"/>
-      <c r="C9" s="232"/>
-      <c r="D9" s="232"/>
-      <c r="E9" s="232"/>
-      <c r="F9" s="232"/>
-      <c r="G9" s="232"/>
-      <c r="H9" s="232"/>
-      <c r="I9" s="233"/>
+      <c r="B9" s="193"/>
+      <c r="C9" s="194"/>
+      <c r="D9" s="194"/>
+      <c r="E9" s="194"/>
+      <c r="F9" s="194"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="194"/>
+      <c r="I9" s="195"/>
       <c r="J9"/>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="B10" s="231"/>
-      <c r="C10" s="232"/>
-      <c r="D10" s="232"/>
-      <c r="E10" s="232"/>
-      <c r="F10" s="232"/>
-      <c r="G10" s="232"/>
-      <c r="H10" s="232"/>
-      <c r="I10" s="233"/>
+      <c r="B10" s="193"/>
+      <c r="C10" s="194"/>
+      <c r="D10" s="194"/>
+      <c r="E10" s="194"/>
+      <c r="F10" s="194"/>
+      <c r="G10" s="194"/>
+      <c r="H10" s="194"/>
+      <c r="I10" s="195"/>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="B11" s="231"/>
-      <c r="C11" s="232"/>
-      <c r="D11" s="232"/>
-      <c r="E11" s="232"/>
-      <c r="F11" s="232"/>
-      <c r="G11" s="232"/>
-      <c r="H11" s="232"/>
-      <c r="I11" s="233"/>
+      <c r="B11" s="193"/>
+      <c r="C11" s="194"/>
+      <c r="D11" s="194"/>
+      <c r="E11" s="194"/>
+      <c r="F11" s="194"/>
+      <c r="G11" s="194"/>
+      <c r="H11" s="194"/>
+      <c r="I11" s="195"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="B12" s="231"/>
-      <c r="C12" s="232"/>
-      <c r="D12" s="232"/>
-      <c r="E12" s="232"/>
-      <c r="F12" s="232"/>
-      <c r="G12" s="232"/>
-      <c r="H12" s="232"/>
-      <c r="I12" s="233"/>
+      <c r="B12" s="193"/>
+      <c r="C12" s="194"/>
+      <c r="D12" s="194"/>
+      <c r="E12" s="194"/>
+      <c r="F12" s="194"/>
+      <c r="G12" s="194"/>
+      <c r="H12" s="194"/>
+      <c r="I12" s="195"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:12" ht="23.25" customHeight="1">
-      <c r="B13" s="231"/>
-      <c r="C13" s="232"/>
-      <c r="D13" s="232"/>
-      <c r="E13" s="232"/>
-      <c r="F13" s="232"/>
-      <c r="G13" s="232"/>
-      <c r="H13" s="232"/>
-      <c r="I13" s="233"/>
+      <c r="B13" s="193"/>
+      <c r="C13" s="194"/>
+      <c r="D13" s="194"/>
+      <c r="E13" s="194"/>
+      <c r="F13" s="194"/>
+      <c r="G13" s="194"/>
+      <c r="H13" s="194"/>
+      <c r="I13" s="195"/>
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:12" ht="33" customHeight="1">
-      <c r="B14" s="234"/>
-      <c r="C14" s="235"/>
-      <c r="D14" s="235"/>
-      <c r="E14" s="235"/>
-      <c r="F14" s="235"/>
-      <c r="G14" s="235"/>
-      <c r="H14" s="235"/>
-      <c r="I14" s="236"/>
+      <c r="B14" s="196"/>
+      <c r="C14" s="197"/>
+      <c r="D14" s="197"/>
+      <c r="E14" s="197"/>
+      <c r="F14" s="197"/>
+      <c r="G14" s="197"/>
+      <c r="H14" s="197"/>
+      <c r="I14" s="198"/>
       <c r="K14" s="34" t="s">
         <v>0</v>
       </c>
@@ -31314,60 +31308,60 @@
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B16" s="191" t="s">
+      <c r="B16" s="182" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="192"/>
-      <c r="D16" s="192"/>
-      <c r="E16" s="192"/>
-      <c r="F16" s="192"/>
-      <c r="G16" s="192"/>
-      <c r="H16" s="192"/>
-      <c r="I16" s="192"/>
-      <c r="J16" s="192"/>
-      <c r="K16" s="192"/>
-      <c r="L16" s="192"/>
+      <c r="C16" s="183"/>
+      <c r="D16" s="183"/>
+      <c r="E16" s="183"/>
+      <c r="F16" s="183"/>
+      <c r="G16" s="183"/>
+      <c r="H16" s="183"/>
+      <c r="I16" s="183"/>
+      <c r="J16" s="183"/>
+      <c r="K16" s="183"/>
+      <c r="L16" s="183"/>
     </row>
     <row r="17" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B17" s="237" t="s">
+      <c r="B17" s="199" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="238"/>
-      <c r="D17" s="238"/>
-      <c r="E17" s="238"/>
-      <c r="F17" s="238"/>
-      <c r="G17" s="238"/>
-      <c r="H17" s="238"/>
-      <c r="I17" s="238"/>
-      <c r="J17" s="238"/>
-      <c r="K17" s="238"/>
-      <c r="L17" s="239"/>
+      <c r="C17" s="200"/>
+      <c r="D17" s="200"/>
+      <c r="E17" s="200"/>
+      <c r="F17" s="200"/>
+      <c r="G17" s="200"/>
+      <c r="H17" s="200"/>
+      <c r="I17" s="200"/>
+      <c r="J17" s="200"/>
+      <c r="K17" s="200"/>
+      <c r="L17" s="201"/>
     </row>
     <row r="18" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B18" s="240"/>
-      <c r="C18" s="241"/>
-      <c r="D18" s="241"/>
-      <c r="E18" s="241"/>
-      <c r="F18" s="241"/>
-      <c r="G18" s="241"/>
-      <c r="H18" s="241"/>
-      <c r="I18" s="241"/>
-      <c r="J18" s="241"/>
-      <c r="K18" s="241"/>
-      <c r="L18" s="242"/>
+      <c r="B18" s="202"/>
+      <c r="C18" s="203"/>
+      <c r="D18" s="203"/>
+      <c r="E18" s="203"/>
+      <c r="F18" s="203"/>
+      <c r="G18" s="203"/>
+      <c r="H18" s="203"/>
+      <c r="I18" s="203"/>
+      <c r="J18" s="203"/>
+      <c r="K18" s="203"/>
+      <c r="L18" s="204"/>
     </row>
     <row r="19" spans="1:12" ht="43.2" customHeight="1">
-      <c r="B19" s="243"/>
-      <c r="C19" s="244"/>
-      <c r="D19" s="244"/>
-      <c r="E19" s="244"/>
-      <c r="F19" s="244"/>
-      <c r="G19" s="244"/>
-      <c r="H19" s="244"/>
-      <c r="I19" s="244"/>
-      <c r="J19" s="244"/>
-      <c r="K19" s="244"/>
-      <c r="L19" s="245"/>
+      <c r="B19" s="205"/>
+      <c r="C19" s="206"/>
+      <c r="D19" s="206"/>
+      <c r="E19" s="206"/>
+      <c r="F19" s="206"/>
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206"/>
+      <c r="J19" s="206"/>
+      <c r="K19" s="206"/>
+      <c r="L19" s="207"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="B20" s="8"/>
@@ -31383,19 +31377,19 @@
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B21" s="191" t="s">
+      <c r="B21" s="182" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="192"/>
-      <c r="D21" s="192"/>
-      <c r="E21" s="192"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="192"/>
-      <c r="H21" s="192"/>
-      <c r="I21" s="192"/>
-      <c r="J21" s="192"/>
-      <c r="K21" s="192"/>
-      <c r="L21" s="192"/>
+      <c r="C21" s="183"/>
+      <c r="D21" s="183"/>
+      <c r="E21" s="183"/>
+      <c r="F21" s="183"/>
+      <c r="G21" s="183"/>
+      <c r="H21" s="183"/>
+      <c r="I21" s="183"/>
+      <c r="J21" s="183"/>
+      <c r="K21" s="183"/>
+      <c r="L21" s="183"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="B22" s="9"/>
@@ -31476,14 +31470,14 @@
         <v>2</v>
       </c>
       <c r="F26" s="33"/>
-      <c r="G26" s="246" t="s">
+      <c r="G26" s="208" t="s">
         <v>187</v>
       </c>
-      <c r="H26" s="247"/>
-      <c r="I26" s="247"/>
-      <c r="J26" s="247"/>
-      <c r="K26" s="247"/>
-      <c r="L26" s="248"/>
+      <c r="H26" s="209"/>
+      <c r="I26" s="209"/>
+      <c r="J26" s="209"/>
+      <c r="K26" s="209"/>
+      <c r="L26" s="210"/>
     </row>
     <row r="27" spans="1:12" ht="33.75" customHeight="1">
       <c r="B27" s="36" t="s">
@@ -31499,14 +31493,14 @@
         <v>360360</v>
       </c>
       <c r="F27" s="33"/>
-      <c r="G27" s="249" t="s">
+      <c r="G27" s="211" t="s">
         <v>186</v>
       </c>
-      <c r="H27" s="250"/>
-      <c r="I27" s="250"/>
-      <c r="J27" s="250"/>
-      <c r="K27" s="250"/>
-      <c r="L27" s="251"/>
+      <c r="H27" s="212"/>
+      <c r="I27" s="212"/>
+      <c r="J27" s="212"/>
+      <c r="K27" s="212"/>
+      <c r="L27" s="213"/>
     </row>
     <row r="28" spans="1:12" ht="54" customHeight="1">
       <c r="B28" s="36" t="s">
@@ -31522,14 +31516,14 @@
         <v>312</v>
       </c>
       <c r="F28" s="33"/>
-      <c r="G28" s="252" t="s">
+      <c r="G28" s="214" t="s">
         <v>345</v>
       </c>
-      <c r="H28" s="253"/>
-      <c r="I28" s="253"/>
-      <c r="J28" s="253"/>
-      <c r="K28" s="253"/>
-      <c r="L28" s="254"/>
+      <c r="H28" s="215"/>
+      <c r="I28" s="215"/>
+      <c r="J28" s="215"/>
+      <c r="K28" s="215"/>
+      <c r="L28" s="216"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="B29" s="2"/>
@@ -31545,19 +31539,19 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="B30" s="191" t="s">
+      <c r="B30" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="192"/>
-      <c r="D30" s="192"/>
-      <c r="E30" s="192"/>
-      <c r="F30" s="192"/>
-      <c r="G30" s="192"/>
-      <c r="H30" s="192"/>
-      <c r="I30" s="192"/>
-      <c r="J30" s="192"/>
-      <c r="K30" s="192"/>
-      <c r="L30" s="192"/>
+      <c r="C30" s="183"/>
+      <c r="D30" s="183"/>
+      <c r="E30" s="183"/>
+      <c r="F30" s="183"/>
+      <c r="G30" s="183"/>
+      <c r="H30" s="183"/>
+      <c r="I30" s="183"/>
+      <c r="J30" s="183"/>
+      <c r="K30" s="183"/>
+      <c r="L30" s="183"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="B31" s="16"/>
@@ -31787,10 +31781,10 @@
         <v>122</v>
       </c>
       <c r="F45" s="18"/>
-      <c r="G45" s="199" t="s">
+      <c r="G45" s="232" t="s">
         <v>324</v>
       </c>
-      <c r="H45" s="200"/>
+      <c r="H45" s="233"/>
       <c r="I45" s="91" t="s">
         <v>52</v>
       </c>
@@ -32183,14 +32177,14 @@
       <c r="F63" s="18"/>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
-      <c r="I63" s="201" t="s">
+      <c r="I63" s="234" t="s">
         <v>138</v>
       </c>
-      <c r="J63" s="202"/>
-      <c r="K63" s="205" t="s">
+      <c r="J63" s="235"/>
+      <c r="K63" s="238" t="s">
         <v>141</v>
       </c>
-      <c r="L63" s="206"/>
+      <c r="L63" s="239"/>
     </row>
     <row r="64" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A64" s="13"/>
@@ -32203,10 +32197,10 @@
       <c r="F64" s="18"/>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
-      <c r="I64" s="203"/>
-      <c r="J64" s="204"/>
-      <c r="K64" s="207"/>
-      <c r="L64" s="208"/>
+      <c r="I64" s="236"/>
+      <c r="J64" s="237"/>
+      <c r="K64" s="240"/>
+      <c r="L64" s="241"/>
     </row>
     <row r="65" spans="1:12" ht="15" customHeight="1">
       <c r="A65" s="13"/>
@@ -32375,16 +32369,16 @@
         <v>349</v>
       </c>
       <c r="F75" s="85"/>
-      <c r="G75" s="209" t="s">
+      <c r="G75" s="242" t="s">
         <v>136</v>
       </c>
-      <c r="H75" s="210"/>
-      <c r="I75" s="210"/>
-      <c r="J75" s="211"/>
-      <c r="K75" s="209" t="s">
+      <c r="H75" s="243"/>
+      <c r="I75" s="243"/>
+      <c r="J75" s="244"/>
+      <c r="K75" s="242" t="s">
         <v>135</v>
       </c>
-      <c r="L75" s="211"/>
+      <c r="L75" s="244"/>
     </row>
     <row r="76" spans="1:12" ht="15" customHeight="1">
       <c r="A76" s="13"/>
@@ -32975,119 +32969,119 @@
       <c r="L99" s="20"/>
     </row>
     <row r="100" spans="1:12">
-      <c r="B100" s="191" t="s">
+      <c r="B100" s="182" t="s">
         <v>21</v>
       </c>
-      <c r="C100" s="192"/>
-      <c r="D100" s="192"/>
-      <c r="E100" s="192"/>
-      <c r="F100" s="192"/>
-      <c r="G100" s="192"/>
-      <c r="H100" s="192"/>
-      <c r="I100" s="192"/>
-      <c r="J100" s="192"/>
-      <c r="K100" s="192"/>
-      <c r="L100" s="192"/>
+      <c r="C100" s="183"/>
+      <c r="D100" s="183"/>
+      <c r="E100" s="183"/>
+      <c r="F100" s="183"/>
+      <c r="G100" s="183"/>
+      <c r="H100" s="183"/>
+      <c r="I100" s="183"/>
+      <c r="J100" s="183"/>
+      <c r="K100" s="183"/>
+      <c r="L100" s="183"/>
     </row>
     <row r="101" spans="1:12" ht="15" customHeight="1">
       <c r="A101" s="13"/>
-      <c r="B101" s="182" t="s">
+      <c r="B101" s="217" t="s">
         <v>198</v>
       </c>
-      <c r="C101" s="212"/>
-      <c r="D101" s="212"/>
-      <c r="E101" s="212"/>
-      <c r="F101" s="212"/>
-      <c r="G101" s="212"/>
-      <c r="H101" s="212"/>
-      <c r="I101" s="212"/>
-      <c r="J101" s="212"/>
-      <c r="K101" s="212"/>
-      <c r="L101" s="213"/>
+      <c r="C101" s="245"/>
+      <c r="D101" s="245"/>
+      <c r="E101" s="245"/>
+      <c r="F101" s="245"/>
+      <c r="G101" s="245"/>
+      <c r="H101" s="245"/>
+      <c r="I101" s="245"/>
+      <c r="J101" s="245"/>
+      <c r="K101" s="245"/>
+      <c r="L101" s="246"/>
     </row>
     <row r="102" spans="1:12" ht="15" customHeight="1">
       <c r="A102" s="13"/>
-      <c r="B102" s="214"/>
-      <c r="C102" s="215"/>
-      <c r="D102" s="215"/>
-      <c r="E102" s="215"/>
-      <c r="F102" s="215"/>
-      <c r="G102" s="215"/>
-      <c r="H102" s="215"/>
-      <c r="I102" s="215"/>
-      <c r="J102" s="215"/>
-      <c r="K102" s="215"/>
-      <c r="L102" s="216"/>
+      <c r="B102" s="247"/>
+      <c r="C102" s="248"/>
+      <c r="D102" s="248"/>
+      <c r="E102" s="248"/>
+      <c r="F102" s="248"/>
+      <c r="G102" s="248"/>
+      <c r="H102" s="248"/>
+      <c r="I102" s="248"/>
+      <c r="J102" s="248"/>
+      <c r="K102" s="248"/>
+      <c r="L102" s="249"/>
     </row>
     <row r="103" spans="1:12" ht="15" customHeight="1">
       <c r="A103" s="13"/>
-      <c r="B103" s="214"/>
-      <c r="C103" s="215"/>
-      <c r="D103" s="215"/>
-      <c r="E103" s="215"/>
-      <c r="F103" s="215"/>
-      <c r="G103" s="215"/>
-      <c r="H103" s="215"/>
-      <c r="I103" s="215"/>
-      <c r="J103" s="215"/>
-      <c r="K103" s="215"/>
-      <c r="L103" s="216"/>
+      <c r="B103" s="247"/>
+      <c r="C103" s="248"/>
+      <c r="D103" s="248"/>
+      <c r="E103" s="248"/>
+      <c r="F103" s="248"/>
+      <c r="G103" s="248"/>
+      <c r="H103" s="248"/>
+      <c r="I103" s="248"/>
+      <c r="J103" s="248"/>
+      <c r="K103" s="248"/>
+      <c r="L103" s="249"/>
     </row>
     <row r="104" spans="1:12" ht="15" customHeight="1">
       <c r="A104" s="13"/>
-      <c r="B104" s="214"/>
-      <c r="C104" s="215"/>
-      <c r="D104" s="215"/>
-      <c r="E104" s="215"/>
-      <c r="F104" s="215"/>
-      <c r="G104" s="215"/>
-      <c r="H104" s="215"/>
-      <c r="I104" s="215"/>
-      <c r="J104" s="215"/>
-      <c r="K104" s="215"/>
-      <c r="L104" s="216"/>
+      <c r="B104" s="247"/>
+      <c r="C104" s="248"/>
+      <c r="D104" s="248"/>
+      <c r="E104" s="248"/>
+      <c r="F104" s="248"/>
+      <c r="G104" s="248"/>
+      <c r="H104" s="248"/>
+      <c r="I104" s="248"/>
+      <c r="J104" s="248"/>
+      <c r="K104" s="248"/>
+      <c r="L104" s="249"/>
     </row>
     <row r="105" spans="1:12" ht="15" customHeight="1">
       <c r="A105" s="13"/>
-      <c r="B105" s="214"/>
-      <c r="C105" s="215"/>
-      <c r="D105" s="215"/>
-      <c r="E105" s="215"/>
-      <c r="F105" s="215"/>
-      <c r="G105" s="215"/>
-      <c r="H105" s="215"/>
-      <c r="I105" s="215"/>
-      <c r="J105" s="215"/>
-      <c r="K105" s="215"/>
-      <c r="L105" s="216"/>
+      <c r="B105" s="247"/>
+      <c r="C105" s="248"/>
+      <c r="D105" s="248"/>
+      <c r="E105" s="248"/>
+      <c r="F105" s="248"/>
+      <c r="G105" s="248"/>
+      <c r="H105" s="248"/>
+      <c r="I105" s="248"/>
+      <c r="J105" s="248"/>
+      <c r="K105" s="248"/>
+      <c r="L105" s="249"/>
     </row>
     <row r="106" spans="1:12" ht="15" customHeight="1">
       <c r="A106" s="13"/>
-      <c r="B106" s="214"/>
-      <c r="C106" s="215"/>
-      <c r="D106" s="215"/>
-      <c r="E106" s="215"/>
-      <c r="F106" s="215"/>
-      <c r="G106" s="215"/>
-      <c r="H106" s="215"/>
-      <c r="I106" s="215"/>
-      <c r="J106" s="215"/>
-      <c r="K106" s="215"/>
-      <c r="L106" s="216"/>
+      <c r="B106" s="247"/>
+      <c r="C106" s="248"/>
+      <c r="D106" s="248"/>
+      <c r="E106" s="248"/>
+      <c r="F106" s="248"/>
+      <c r="G106" s="248"/>
+      <c r="H106" s="248"/>
+      <c r="I106" s="248"/>
+      <c r="J106" s="248"/>
+      <c r="K106" s="248"/>
+      <c r="L106" s="249"/>
     </row>
     <row r="107" spans="1:12" ht="15" customHeight="1">
       <c r="A107" s="13"/>
-      <c r="B107" s="217"/>
-      <c r="C107" s="218"/>
-      <c r="D107" s="218"/>
-      <c r="E107" s="218"/>
-      <c r="F107" s="218"/>
-      <c r="G107" s="218"/>
-      <c r="H107" s="218"/>
-      <c r="I107" s="218"/>
-      <c r="J107" s="218"/>
-      <c r="K107" s="218"/>
-      <c r="L107" s="219"/>
+      <c r="B107" s="250"/>
+      <c r="C107" s="251"/>
+      <c r="D107" s="251"/>
+      <c r="E107" s="251"/>
+      <c r="F107" s="251"/>
+      <c r="G107" s="251"/>
+      <c r="H107" s="251"/>
+      <c r="I107" s="251"/>
+      <c r="J107" s="251"/>
+      <c r="K107" s="251"/>
+      <c r="L107" s="252"/>
     </row>
     <row r="108" spans="1:12" ht="15" customHeight="1">
       <c r="A108" s="13"/>
@@ -33104,19 +33098,19 @@
       <c r="L108" s="20"/>
     </row>
     <row r="109" spans="1:12">
-      <c r="B109" s="191" t="s">
+      <c r="B109" s="182" t="s">
         <v>118</v>
       </c>
-      <c r="C109" s="192"/>
-      <c r="D109" s="192"/>
-      <c r="E109" s="192"/>
-      <c r="F109" s="192"/>
-      <c r="G109" s="192"/>
-      <c r="H109" s="192"/>
-      <c r="I109" s="192"/>
-      <c r="J109" s="192"/>
-      <c r="K109" s="192"/>
-      <c r="L109" s="192"/>
+      <c r="C109" s="183"/>
+      <c r="D109" s="183"/>
+      <c r="E109" s="183"/>
+      <c r="F109" s="183"/>
+      <c r="G109" s="183"/>
+      <c r="H109" s="183"/>
+      <c r="I109" s="183"/>
+      <c r="J109" s="183"/>
+      <c r="K109" s="183"/>
+      <c r="L109" s="183"/>
     </row>
     <row r="110" spans="1:12" ht="15" customHeight="1">
       <c r="A110" s="13"/>
@@ -33240,8 +33234,8 @@
     </row>
     <row r="118" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A118" s="13"/>
-      <c r="B118" s="220"/>
-      <c r="C118" s="221"/>
+      <c r="B118" s="253"/>
+      <c r="C118" s="254"/>
       <c r="D118" s="63"/>
       <c r="E118" s="63"/>
       <c r="F118" s="62"/>
@@ -33254,8 +33248,8 @@
     </row>
     <row r="119" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A119" s="13"/>
-      <c r="B119" s="220"/>
-      <c r="C119" s="221"/>
+      <c r="B119" s="253"/>
+      <c r="C119" s="254"/>
       <c r="D119" s="63"/>
       <c r="E119" s="63"/>
       <c r="F119" s="62"/>
@@ -36137,128 +36131,136 @@
       <c r="L262" s="27"/>
     </row>
     <row r="263" spans="1:12">
-      <c r="B263" s="191" t="s">
+      <c r="B263" s="182" t="s">
         <v>22</v>
       </c>
-      <c r="C263" s="192"/>
-      <c r="D263" s="192"/>
-      <c r="E263" s="192"/>
-      <c r="F263" s="192"/>
-      <c r="G263" s="192"/>
-      <c r="H263" s="192"/>
-      <c r="I263" s="192"/>
-      <c r="J263" s="192"/>
-      <c r="K263" s="192"/>
-      <c r="L263" s="192"/>
+      <c r="C263" s="183"/>
+      <c r="D263" s="183"/>
+      <c r="E263" s="183"/>
+      <c r="F263" s="183"/>
+      <c r="G263" s="183"/>
+      <c r="H263" s="183"/>
+      <c r="I263" s="183"/>
+      <c r="J263" s="183"/>
+      <c r="K263" s="183"/>
+      <c r="L263" s="183"/>
     </row>
     <row r="264" spans="1:12">
-      <c r="B264" s="182" t="s">
+      <c r="B264" s="217" t="s">
         <v>317</v>
       </c>
-      <c r="C264" s="183"/>
-      <c r="D264" s="183"/>
-      <c r="E264" s="183"/>
-      <c r="F264" s="183"/>
-      <c r="G264" s="183"/>
-      <c r="H264" s="183"/>
-      <c r="I264" s="183"/>
-      <c r="J264" s="183"/>
-      <c r="K264" s="183"/>
-      <c r="L264" s="184"/>
+      <c r="C264" s="218"/>
+      <c r="D264" s="218"/>
+      <c r="E264" s="218"/>
+      <c r="F264" s="218"/>
+      <c r="G264" s="218"/>
+      <c r="H264" s="218"/>
+      <c r="I264" s="218"/>
+      <c r="J264" s="218"/>
+      <c r="K264" s="218"/>
+      <c r="L264" s="219"/>
     </row>
     <row r="265" spans="1:12">
-      <c r="B265" s="185"/>
-      <c r="C265" s="186"/>
-      <c r="D265" s="186"/>
-      <c r="E265" s="186"/>
-      <c r="F265" s="186"/>
-      <c r="G265" s="186"/>
-      <c r="H265" s="186"/>
-      <c r="I265" s="186"/>
-      <c r="J265" s="186"/>
-      <c r="K265" s="186"/>
-      <c r="L265" s="187"/>
+      <c r="B265" s="220"/>
+      <c r="C265" s="221"/>
+      <c r="D265" s="221"/>
+      <c r="E265" s="221"/>
+      <c r="F265" s="221"/>
+      <c r="G265" s="221"/>
+      <c r="H265" s="221"/>
+      <c r="I265" s="221"/>
+      <c r="J265" s="221"/>
+      <c r="K265" s="221"/>
+      <c r="L265" s="222"/>
     </row>
     <row r="266" spans="1:12">
-      <c r="B266" s="185"/>
-      <c r="C266" s="186"/>
-      <c r="D266" s="186"/>
-      <c r="E266" s="186"/>
-      <c r="F266" s="186"/>
-      <c r="G266" s="186"/>
-      <c r="H266" s="186"/>
-      <c r="I266" s="186"/>
-      <c r="J266" s="186"/>
-      <c r="K266" s="186"/>
-      <c r="L266" s="187"/>
+      <c r="B266" s="220"/>
+      <c r="C266" s="221"/>
+      <c r="D266" s="221"/>
+      <c r="E266" s="221"/>
+      <c r="F266" s="221"/>
+      <c r="G266" s="221"/>
+      <c r="H266" s="221"/>
+      <c r="I266" s="221"/>
+      <c r="J266" s="221"/>
+      <c r="K266" s="221"/>
+      <c r="L266" s="222"/>
     </row>
     <row r="267" spans="1:12">
-      <c r="B267" s="185"/>
-      <c r="C267" s="186"/>
-      <c r="D267" s="186"/>
-      <c r="E267" s="186"/>
-      <c r="F267" s="186"/>
-      <c r="G267" s="186"/>
-      <c r="H267" s="186"/>
-      <c r="I267" s="186"/>
-      <c r="J267" s="186"/>
-      <c r="K267" s="186"/>
-      <c r="L267" s="187"/>
+      <c r="B267" s="220"/>
+      <c r="C267" s="221"/>
+      <c r="D267" s="221"/>
+      <c r="E267" s="221"/>
+      <c r="F267" s="221"/>
+      <c r="G267" s="221"/>
+      <c r="H267" s="221"/>
+      <c r="I267" s="221"/>
+      <c r="J267" s="221"/>
+      <c r="K267" s="221"/>
+      <c r="L267" s="222"/>
     </row>
     <row r="268" spans="1:12">
-      <c r="B268" s="185"/>
-      <c r="C268" s="186"/>
-      <c r="D268" s="186"/>
-      <c r="E268" s="186"/>
-      <c r="F268" s="186"/>
-      <c r="G268" s="186"/>
-      <c r="H268" s="186"/>
-      <c r="I268" s="186"/>
-      <c r="J268" s="186"/>
-      <c r="K268" s="186"/>
-      <c r="L268" s="187"/>
+      <c r="B268" s="220"/>
+      <c r="C268" s="221"/>
+      <c r="D268" s="221"/>
+      <c r="E268" s="221"/>
+      <c r="F268" s="221"/>
+      <c r="G268" s="221"/>
+      <c r="H268" s="221"/>
+      <c r="I268" s="221"/>
+      <c r="J268" s="221"/>
+      <c r="K268" s="221"/>
+      <c r="L268" s="222"/>
     </row>
     <row r="269" spans="1:12">
-      <c r="B269" s="185"/>
-      <c r="C269" s="186"/>
-      <c r="D269" s="186"/>
-      <c r="E269" s="186"/>
-      <c r="F269" s="186"/>
-      <c r="G269" s="186"/>
-      <c r="H269" s="186"/>
-      <c r="I269" s="186"/>
-      <c r="J269" s="186"/>
-      <c r="K269" s="186"/>
-      <c r="L269" s="187"/>
+      <c r="B269" s="220"/>
+      <c r="C269" s="221"/>
+      <c r="D269" s="221"/>
+      <c r="E269" s="221"/>
+      <c r="F269" s="221"/>
+      <c r="G269" s="221"/>
+      <c r="H269" s="221"/>
+      <c r="I269" s="221"/>
+      <c r="J269" s="221"/>
+      <c r="K269" s="221"/>
+      <c r="L269" s="222"/>
     </row>
     <row r="270" spans="1:12">
-      <c r="B270" s="185"/>
-      <c r="C270" s="186"/>
-      <c r="D270" s="186"/>
-      <c r="E270" s="186"/>
-      <c r="F270" s="186"/>
-      <c r="G270" s="186"/>
-      <c r="H270" s="186"/>
-      <c r="I270" s="186"/>
-      <c r="J270" s="186"/>
-      <c r="K270" s="186"/>
-      <c r="L270" s="187"/>
+      <c r="B270" s="220"/>
+      <c r="C270" s="221"/>
+      <c r="D270" s="221"/>
+      <c r="E270" s="221"/>
+      <c r="F270" s="221"/>
+      <c r="G270" s="221"/>
+      <c r="H270" s="221"/>
+      <c r="I270" s="221"/>
+      <c r="J270" s="221"/>
+      <c r="K270" s="221"/>
+      <c r="L270" s="222"/>
     </row>
     <row r="271" spans="1:12">
-      <c r="B271" s="188"/>
-      <c r="C271" s="189"/>
-      <c r="D271" s="189"/>
-      <c r="E271" s="189"/>
-      <c r="F271" s="189"/>
-      <c r="G271" s="189"/>
-      <c r="H271" s="189"/>
-      <c r="I271" s="189"/>
-      <c r="J271" s="189"/>
-      <c r="K271" s="189"/>
-      <c r="L271" s="190"/>
+      <c r="B271" s="223"/>
+      <c r="C271" s="224"/>
+      <c r="D271" s="224"/>
+      <c r="E271" s="224"/>
+      <c r="F271" s="224"/>
+      <c r="G271" s="224"/>
+      <c r="H271" s="224"/>
+      <c r="I271" s="224"/>
+      <c r="J271" s="224"/>
+      <c r="K271" s="224"/>
+      <c r="L271" s="225"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B16:L16"/>
+    <mergeCell ref="B17:L19"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="B4:L4"/>
     <mergeCell ref="B264:L271"/>
     <mergeCell ref="B109:L109"/>
     <mergeCell ref="B7:I14"/>
@@ -36274,14 +36276,6 @@
     <mergeCell ref="K75:L75"/>
     <mergeCell ref="B263:L263"/>
     <mergeCell ref="B101:L107"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B17:L19"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="B4:L4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>